<commit_message>
added ARDUINO Project. FINALIZED PLANO DE PROJETO!!!!!
</commit_message>
<xml_diff>
--- a/LaTeX Project/Documentos/Gantt.xlsx
+++ b/LaTeX Project/Documentos/Gantt.xlsx
@@ -1013,12 +1013,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,6 +1021,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="10" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1040,7 +1037,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1807,8 +1807,8 @@
   </sheetPr>
   <dimension ref="A2:CU83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AS20" sqref="AS20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1833,47 +1833,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="24" t="s">
         <v>78</v>
       </c>
       <c r="I2" s="16"/>
-      <c r="BE2" s="56" t="s">
+      <c r="BE2" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" s="56"/>
-      <c r="BG2" s="56"/>
-      <c r="BH2" s="56"/>
-      <c r="BI2" s="56"/>
-      <c r="BJ2" s="56"/>
-      <c r="BK2" s="56"/>
-      <c r="BL2" s="56"/>
-      <c r="BM2" s="56"/>
-      <c r="BN2" s="56"/>
-      <c r="BO2" s="56"/>
-      <c r="BP2" s="56"/>
-      <c r="BQ2" s="56"/>
-      <c r="BR2" s="56"/>
-      <c r="BS2" s="56"/>
-      <c r="BT2" s="56"/>
-      <c r="BU2" s="56"/>
-      <c r="BV2" s="56"/>
-      <c r="BW2" s="56"/>
+      <c r="BF2" s="50"/>
+      <c r="BG2" s="50"/>
+      <c r="BH2" s="50"/>
+      <c r="BI2" s="50"/>
+      <c r="BJ2" s="50"/>
+      <c r="BK2" s="50"/>
+      <c r="BL2" s="50"/>
+      <c r="BM2" s="50"/>
+      <c r="BN2" s="50"/>
+      <c r="BO2" s="50"/>
+      <c r="BP2" s="50"/>
+      <c r="BQ2" s="50"/>
+      <c r="BR2" s="50"/>
+      <c r="BS2" s="50"/>
+      <c r="BT2" s="50"/>
+      <c r="BU2" s="50"/>
+      <c r="BV2" s="50"/>
+      <c r="BW2" s="50"/>
     </row>
     <row r="3" spans="1:99" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="24" t="s">
         <v>79</v>
       </c>
@@ -1922,35 +1922,35 @@
       <c r="AQ3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="BE3" s="56" t="s">
+      <c r="BE3" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="BF3" s="56"/>
-      <c r="BG3" s="56"/>
-      <c r="BH3" s="56"/>
-      <c r="BI3" s="56"/>
-      <c r="BJ3" s="56"/>
-      <c r="BK3" s="56"/>
-      <c r="BL3" s="56"/>
-      <c r="BM3" s="56"/>
-      <c r="BN3" s="56"/>
-      <c r="BO3" s="56"/>
-      <c r="BP3" s="56"/>
-      <c r="BQ3" s="56"/>
-      <c r="BR3" s="56"/>
-      <c r="BS3" s="56"/>
-      <c r="BT3" s="56"/>
-      <c r="BU3" s="56"/>
-      <c r="BV3" s="56"/>
-      <c r="BW3" s="56"/>
+      <c r="BF3" s="50"/>
+      <c r="BG3" s="50"/>
+      <c r="BH3" s="50"/>
+      <c r="BI3" s="50"/>
+      <c r="BJ3" s="50"/>
+      <c r="BK3" s="50"/>
+      <c r="BL3" s="50"/>
+      <c r="BM3" s="50"/>
+      <c r="BN3" s="50"/>
+      <c r="BO3" s="50"/>
+      <c r="BP3" s="50"/>
+      <c r="BQ3" s="50"/>
+      <c r="BR3" s="50"/>
+      <c r="BS3" s="50"/>
+      <c r="BT3" s="50"/>
+      <c r="BU3" s="50"/>
+      <c r="BV3" s="50"/>
+      <c r="BW3" s="50"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="24" t="s">
         <v>80</v>
       </c>
@@ -1981,132 +1981,132 @@
       <c r="AY4" s="19"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="J5" s="52" t="s">
+      <c r="J5" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="49" t="s">
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="52" t="s">
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
-      <c r="W5" s="53"/>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="49" t="s">
+      <c r="U5" s="52"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52"/>
+      <c r="X5" s="53"/>
+      <c r="Y5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="50"/>
-      <c r="AC5" s="51"/>
-      <c r="AD5" s="52" t="s">
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="48"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="53"/>
-      <c r="AF5" s="53"/>
-      <c r="AG5" s="53"/>
-      <c r="AH5" s="54"/>
-      <c r="AI5" s="49" t="s">
+      <c r="AE5" s="52"/>
+      <c r="AF5" s="52"/>
+      <c r="AG5" s="52"/>
+      <c r="AH5" s="53"/>
+      <c r="AI5" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="AJ5" s="50"/>
-      <c r="AK5" s="50"/>
-      <c r="AL5" s="50"/>
-      <c r="AM5" s="51"/>
-      <c r="AN5" s="52" t="s">
+      <c r="AJ5" s="48"/>
+      <c r="AK5" s="48"/>
+      <c r="AL5" s="48"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="53"/>
-      <c r="AP5" s="53"/>
-      <c r="AQ5" s="53"/>
-      <c r="AR5" s="54"/>
-      <c r="AS5" s="49" t="s">
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="52"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="53"/>
+      <c r="AS5" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="AT5" s="50"/>
-      <c r="AU5" s="50"/>
-      <c r="AV5" s="50"/>
-      <c r="AW5" s="51"/>
-      <c r="AX5" s="52" t="s">
+      <c r="AT5" s="48"/>
+      <c r="AU5" s="48"/>
+      <c r="AV5" s="48"/>
+      <c r="AW5" s="49"/>
+      <c r="AX5" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="AY5" s="53"/>
-      <c r="AZ5" s="53"/>
-      <c r="BA5" s="53"/>
-      <c r="BB5" s="54"/>
-      <c r="BC5" s="49" t="s">
+      <c r="AY5" s="52"/>
+      <c r="AZ5" s="52"/>
+      <c r="BA5" s="52"/>
+      <c r="BB5" s="53"/>
+      <c r="BC5" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="BD5" s="50"/>
-      <c r="BE5" s="50"/>
-      <c r="BF5" s="50"/>
-      <c r="BG5" s="51"/>
-      <c r="BH5" s="52" t="s">
+      <c r="BD5" s="48"/>
+      <c r="BE5" s="48"/>
+      <c r="BF5" s="48"/>
+      <c r="BG5" s="49"/>
+      <c r="BH5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="BI5" s="53"/>
-      <c r="BJ5" s="53"/>
-      <c r="BK5" s="53"/>
-      <c r="BL5" s="54"/>
-      <c r="BM5" s="49" t="s">
+      <c r="BI5" s="52"/>
+      <c r="BJ5" s="52"/>
+      <c r="BK5" s="52"/>
+      <c r="BL5" s="53"/>
+      <c r="BM5" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="BN5" s="50"/>
-      <c r="BO5" s="50"/>
-      <c r="BP5" s="50"/>
-      <c r="BQ5" s="51"/>
-      <c r="BR5" s="52" t="s">
+      <c r="BN5" s="48"/>
+      <c r="BO5" s="48"/>
+      <c r="BP5" s="48"/>
+      <c r="BQ5" s="49"/>
+      <c r="BR5" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="BS5" s="53"/>
-      <c r="BT5" s="53"/>
-      <c r="BU5" s="53"/>
-      <c r="BV5" s="54"/>
-      <c r="BW5" s="49" t="s">
+      <c r="BS5" s="52"/>
+      <c r="BT5" s="52"/>
+      <c r="BU5" s="52"/>
+      <c r="BV5" s="53"/>
+      <c r="BW5" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="BX5" s="50"/>
-      <c r="BY5" s="50"/>
-      <c r="BZ5" s="50"/>
-      <c r="CA5" s="51"/>
-      <c r="CB5" s="52" t="s">
+      <c r="BX5" s="48"/>
+      <c r="BY5" s="48"/>
+      <c r="BZ5" s="48"/>
+      <c r="CA5" s="49"/>
+      <c r="CB5" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="CC5" s="53"/>
-      <c r="CD5" s="53"/>
-      <c r="CE5" s="53"/>
-      <c r="CF5" s="54"/>
-      <c r="CG5" s="49" t="s">
+      <c r="CC5" s="52"/>
+      <c r="CD5" s="52"/>
+      <c r="CE5" s="52"/>
+      <c r="CF5" s="53"/>
+      <c r="CG5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="CH5" s="50"/>
-      <c r="CI5" s="50"/>
-      <c r="CJ5" s="50"/>
-      <c r="CK5" s="51"/>
-      <c r="CL5" s="52" t="s">
+      <c r="CH5" s="48"/>
+      <c r="CI5" s="48"/>
+      <c r="CJ5" s="48"/>
+      <c r="CK5" s="49"/>
+      <c r="CL5" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="CM5" s="53"/>
-      <c r="CN5" s="53"/>
-      <c r="CO5" s="53"/>
-      <c r="CP5" s="54"/>
-      <c r="CQ5" s="49" t="s">
+      <c r="CM5" s="52"/>
+      <c r="CN5" s="52"/>
+      <c r="CO5" s="52"/>
+      <c r="CP5" s="53"/>
+      <c r="CQ5" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="CR5" s="50"/>
-      <c r="CS5" s="50"/>
-      <c r="CT5" s="50"/>
-      <c r="CU5" s="51"/>
+      <c r="CR5" s="48"/>
+      <c r="CS5" s="48"/>
+      <c r="CT5" s="48"/>
+      <c r="CU5" s="49"/>
     </row>
     <row r="6" spans="1:99" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -2129,132 +2129,132 @@
         <v>75</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="49" t="s">
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="51"/>
-      <c r="T6" s="52" t="s">
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
-      <c r="W6" s="53"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="49" t="s">
+      <c r="U6" s="52"/>
+      <c r="V6" s="52"/>
+      <c r="W6" s="52"/>
+      <c r="X6" s="53"/>
+      <c r="Y6" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="Z6" s="50"/>
-      <c r="AA6" s="50"/>
-      <c r="AB6" s="50"/>
-      <c r="AC6" s="51"/>
-      <c r="AD6" s="52" t="s">
+      <c r="Z6" s="48"/>
+      <c r="AA6" s="48"/>
+      <c r="AB6" s="48"/>
+      <c r="AC6" s="49"/>
+      <c r="AD6" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="53"/>
-      <c r="AF6" s="53"/>
-      <c r="AG6" s="53"/>
-      <c r="AH6" s="54"/>
-      <c r="AI6" s="49" t="s">
+      <c r="AE6" s="52"/>
+      <c r="AF6" s="52"/>
+      <c r="AG6" s="52"/>
+      <c r="AH6" s="53"/>
+      <c r="AI6" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="50"/>
-      <c r="AK6" s="50"/>
-      <c r="AL6" s="50"/>
-      <c r="AM6" s="51"/>
-      <c r="AN6" s="52" t="s">
+      <c r="AJ6" s="48"/>
+      <c r="AK6" s="48"/>
+      <c r="AL6" s="48"/>
+      <c r="AM6" s="49"/>
+      <c r="AN6" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" s="53"/>
-      <c r="AP6" s="53"/>
-      <c r="AQ6" s="53"/>
-      <c r="AR6" s="54"/>
-      <c r="AS6" s="49" t="s">
+      <c r="AO6" s="52"/>
+      <c r="AP6" s="52"/>
+      <c r="AQ6" s="52"/>
+      <c r="AR6" s="53"/>
+      <c r="AS6" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="AT6" s="50"/>
-      <c r="AU6" s="50"/>
-      <c r="AV6" s="50"/>
-      <c r="AW6" s="51"/>
-      <c r="AX6" s="52" t="s">
+      <c r="AT6" s="48"/>
+      <c r="AU6" s="48"/>
+      <c r="AV6" s="48"/>
+      <c r="AW6" s="49"/>
+      <c r="AX6" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AY6" s="53"/>
-      <c r="AZ6" s="53"/>
-      <c r="BA6" s="53"/>
-      <c r="BB6" s="54"/>
-      <c r="BC6" s="49" t="s">
+      <c r="AY6" s="52"/>
+      <c r="AZ6" s="52"/>
+      <c r="BA6" s="52"/>
+      <c r="BB6" s="53"/>
+      <c r="BC6" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="BD6" s="50"/>
-      <c r="BE6" s="50"/>
-      <c r="BF6" s="50"/>
-      <c r="BG6" s="51"/>
-      <c r="BH6" s="52" t="s">
+      <c r="BD6" s="48"/>
+      <c r="BE6" s="48"/>
+      <c r="BF6" s="48"/>
+      <c r="BG6" s="49"/>
+      <c r="BH6" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="BI6" s="53"/>
-      <c r="BJ6" s="53"/>
-      <c r="BK6" s="53"/>
-      <c r="BL6" s="54"/>
-      <c r="BM6" s="49" t="s">
+      <c r="BI6" s="52"/>
+      <c r="BJ6" s="52"/>
+      <c r="BK6" s="52"/>
+      <c r="BL6" s="53"/>
+      <c r="BM6" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="BN6" s="50"/>
-      <c r="BO6" s="50"/>
-      <c r="BP6" s="50"/>
-      <c r="BQ6" s="51"/>
-      <c r="BR6" s="52" t="s">
+      <c r="BN6" s="48"/>
+      <c r="BO6" s="48"/>
+      <c r="BP6" s="48"/>
+      <c r="BQ6" s="49"/>
+      <c r="BR6" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="BS6" s="53"/>
-      <c r="BT6" s="53"/>
-      <c r="BU6" s="53"/>
-      <c r="BV6" s="54"/>
-      <c r="BW6" s="49" t="s">
+      <c r="BS6" s="52"/>
+      <c r="BT6" s="52"/>
+      <c r="BU6" s="52"/>
+      <c r="BV6" s="53"/>
+      <c r="BW6" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="BX6" s="50"/>
-      <c r="BY6" s="50"/>
-      <c r="BZ6" s="50"/>
-      <c r="CA6" s="51"/>
-      <c r="CB6" s="52" t="s">
+      <c r="BX6" s="48"/>
+      <c r="BY6" s="48"/>
+      <c r="BZ6" s="48"/>
+      <c r="CA6" s="49"/>
+      <c r="CB6" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="CC6" s="53"/>
-      <c r="CD6" s="53"/>
-      <c r="CE6" s="53"/>
-      <c r="CF6" s="54"/>
-      <c r="CG6" s="49" t="s">
+      <c r="CC6" s="52"/>
+      <c r="CD6" s="52"/>
+      <c r="CE6" s="52"/>
+      <c r="CF6" s="53"/>
+      <c r="CG6" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="CH6" s="50"/>
-      <c r="CI6" s="50"/>
-      <c r="CJ6" s="50"/>
-      <c r="CK6" s="51"/>
-      <c r="CL6" s="52" t="s">
+      <c r="CH6" s="48"/>
+      <c r="CI6" s="48"/>
+      <c r="CJ6" s="48"/>
+      <c r="CK6" s="49"/>
+      <c r="CL6" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="CM6" s="53"/>
-      <c r="CN6" s="53"/>
-      <c r="CO6" s="53"/>
-      <c r="CP6" s="54"/>
-      <c r="CQ6" s="49" t="s">
+      <c r="CM6" s="52"/>
+      <c r="CN6" s="52"/>
+      <c r="CO6" s="52"/>
+      <c r="CP6" s="53"/>
+      <c r="CQ6" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="CR6" s="50"/>
-      <c r="CS6" s="50"/>
-      <c r="CT6" s="50"/>
-      <c r="CU6" s="51"/>
+      <c r="CR6" s="48"/>
+      <c r="CS6" s="48"/>
+      <c r="CT6" s="48"/>
+      <c r="CU6" s="49"/>
     </row>
     <row r="7" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -2869,7 +2869,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="30">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="H14" s="24"/>
       <c r="I14" s="31"/>
@@ -3131,7 +3131,7 @@
         <v>4</v>
       </c>
       <c r="G20" s="30">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H20" s="24" t="s">
         <v>77</v>
@@ -3159,104 +3159,104 @@
       <c r="AC20" s="31"/>
     </row>
     <row r="21" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="47"/>
-      <c r="V21" s="47"/>
-      <c r="W21" s="47"/>
-      <c r="X21" s="47"/>
-      <c r="Y21" s="47"/>
-      <c r="Z21" s="47"/>
-      <c r="AA21" s="47"/>
-      <c r="AB21" s="47"/>
-      <c r="AC21" s="47"/>
-      <c r="AD21" s="47"/>
-      <c r="AE21" s="47"/>
-      <c r="AF21" s="47"/>
-      <c r="AG21" s="47"/>
-      <c r="AH21" s="47"/>
-      <c r="AI21" s="47"/>
-      <c r="AJ21" s="47"/>
-      <c r="AK21" s="47"/>
-      <c r="AL21" s="47"/>
-      <c r="AM21" s="47"/>
-      <c r="AN21" s="47"/>
-      <c r="AO21" s="47"/>
-      <c r="AP21" s="47"/>
-      <c r="AQ21" s="47"/>
-      <c r="AR21" s="47"/>
-      <c r="AS21" s="47"/>
-      <c r="AT21" s="47"/>
-      <c r="AU21" s="47"/>
-      <c r="AV21" s="47"/>
-      <c r="AW21" s="47"/>
-      <c r="AX21" s="47"/>
-      <c r="AY21" s="47"/>
-      <c r="AZ21" s="47"/>
-      <c r="BA21" s="47"/>
-      <c r="BB21" s="47"/>
-      <c r="BC21" s="47"/>
-      <c r="BD21" s="47"/>
-      <c r="BE21" s="47"/>
-      <c r="BF21" s="47"/>
-      <c r="BG21" s="47"/>
-      <c r="BH21" s="47"/>
-      <c r="BI21" s="47"/>
-      <c r="BJ21" s="47"/>
-      <c r="BK21" s="47"/>
-      <c r="BL21" s="47"/>
-      <c r="BM21" s="47"/>
-      <c r="BN21" s="47"/>
-      <c r="BO21" s="47"/>
-      <c r="BP21" s="47"/>
-      <c r="BQ21" s="47"/>
-      <c r="BR21" s="47"/>
-      <c r="BS21" s="47"/>
-      <c r="BT21" s="47"/>
-      <c r="BU21" s="47"/>
-      <c r="BV21" s="47"/>
-      <c r="BW21" s="47"/>
-      <c r="BX21" s="47"/>
-      <c r="BY21" s="47"/>
-      <c r="BZ21" s="47"/>
-      <c r="CA21" s="47"/>
-      <c r="CB21" s="47"/>
-      <c r="CC21" s="47"/>
-      <c r="CD21" s="47"/>
-      <c r="CE21" s="47"/>
-      <c r="CF21" s="47"/>
-      <c r="CG21" s="47"/>
-      <c r="CH21" s="47"/>
-      <c r="CI21" s="47"/>
-      <c r="CJ21" s="47"/>
-      <c r="CK21" s="47"/>
-      <c r="CL21" s="47"/>
-      <c r="CM21" s="47"/>
-      <c r="CN21" s="47"/>
-      <c r="CO21" s="47"/>
-      <c r="CP21" s="47"/>
-      <c r="CQ21" s="47"/>
-      <c r="CR21" s="47"/>
-      <c r="CS21" s="47"/>
-      <c r="CT21" s="47"/>
-      <c r="CU21" s="47"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="55"/>
+      <c r="T21" s="55"/>
+      <c r="U21" s="55"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="55"/>
+      <c r="X21" s="55"/>
+      <c r="Y21" s="55"/>
+      <c r="Z21" s="55"/>
+      <c r="AA21" s="55"/>
+      <c r="AB21" s="55"/>
+      <c r="AC21" s="55"/>
+      <c r="AD21" s="55"/>
+      <c r="AE21" s="55"/>
+      <c r="AF21" s="55"/>
+      <c r="AG21" s="55"/>
+      <c r="AH21" s="55"/>
+      <c r="AI21" s="55"/>
+      <c r="AJ21" s="55"/>
+      <c r="AK21" s="55"/>
+      <c r="AL21" s="55"/>
+      <c r="AM21" s="55"/>
+      <c r="AN21" s="55"/>
+      <c r="AO21" s="55"/>
+      <c r="AP21" s="55"/>
+      <c r="AQ21" s="55"/>
+      <c r="AR21" s="55"/>
+      <c r="AS21" s="55"/>
+      <c r="AT21" s="55"/>
+      <c r="AU21" s="55"/>
+      <c r="AV21" s="55"/>
+      <c r="AW21" s="55"/>
+      <c r="AX21" s="55"/>
+      <c r="AY21" s="55"/>
+      <c r="AZ21" s="55"/>
+      <c r="BA21" s="55"/>
+      <c r="BB21" s="55"/>
+      <c r="BC21" s="55"/>
+      <c r="BD21" s="55"/>
+      <c r="BE21" s="55"/>
+      <c r="BF21" s="55"/>
+      <c r="BG21" s="55"/>
+      <c r="BH21" s="55"/>
+      <c r="BI21" s="55"/>
+      <c r="BJ21" s="55"/>
+      <c r="BK21" s="55"/>
+      <c r="BL21" s="55"/>
+      <c r="BM21" s="55"/>
+      <c r="BN21" s="55"/>
+      <c r="BO21" s="55"/>
+      <c r="BP21" s="55"/>
+      <c r="BQ21" s="55"/>
+      <c r="BR21" s="55"/>
+      <c r="BS21" s="55"/>
+      <c r="BT21" s="55"/>
+      <c r="BU21" s="55"/>
+      <c r="BV21" s="55"/>
+      <c r="BW21" s="55"/>
+      <c r="BX21" s="55"/>
+      <c r="BY21" s="55"/>
+      <c r="BZ21" s="55"/>
+      <c r="CA21" s="55"/>
+      <c r="CB21" s="55"/>
+      <c r="CC21" s="55"/>
+      <c r="CD21" s="55"/>
+      <c r="CE21" s="55"/>
+      <c r="CF21" s="55"/>
+      <c r="CG21" s="55"/>
+      <c r="CH21" s="55"/>
+      <c r="CI21" s="55"/>
+      <c r="CJ21" s="55"/>
+      <c r="CK21" s="55"/>
+      <c r="CL21" s="55"/>
+      <c r="CM21" s="55"/>
+      <c r="CN21" s="55"/>
+      <c r="CO21" s="55"/>
+      <c r="CP21" s="55"/>
+      <c r="CQ21" s="55"/>
+      <c r="CR21" s="55"/>
+      <c r="CS21" s="55"/>
+      <c r="CT21" s="55"/>
+      <c r="CU21" s="55"/>
     </row>
     <row r="22" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
@@ -3541,104 +3541,104 @@
       <c r="CU25" s="35"/>
     </row>
     <row r="26" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="47"/>
-      <c r="Q26" s="47"/>
-      <c r="R26" s="47"/>
-      <c r="S26" s="47"/>
-      <c r="T26" s="47"/>
-      <c r="U26" s="47"/>
-      <c r="V26" s="47"/>
-      <c r="W26" s="47"/>
-      <c r="X26" s="47"/>
-      <c r="Y26" s="47"/>
-      <c r="Z26" s="47"/>
-      <c r="AA26" s="47"/>
-      <c r="AB26" s="47"/>
-      <c r="AC26" s="47"/>
-      <c r="AD26" s="47"/>
-      <c r="AE26" s="47"/>
-      <c r="AF26" s="47"/>
-      <c r="AG26" s="47"/>
-      <c r="AH26" s="47"/>
-      <c r="AI26" s="47"/>
-      <c r="AJ26" s="47"/>
-      <c r="AK26" s="47"/>
-      <c r="AL26" s="47"/>
-      <c r="AM26" s="47"/>
-      <c r="AN26" s="47"/>
-      <c r="AO26" s="47"/>
-      <c r="AP26" s="47"/>
-      <c r="AQ26" s="47"/>
-      <c r="AR26" s="47"/>
-      <c r="AS26" s="47"/>
-      <c r="AT26" s="47"/>
-      <c r="AU26" s="47"/>
-      <c r="AV26" s="47"/>
-      <c r="AW26" s="47"/>
-      <c r="AX26" s="47"/>
-      <c r="AY26" s="47"/>
-      <c r="AZ26" s="47"/>
-      <c r="BA26" s="47"/>
-      <c r="BB26" s="47"/>
-      <c r="BC26" s="47"/>
-      <c r="BD26" s="47"/>
-      <c r="BE26" s="47"/>
-      <c r="BF26" s="47"/>
-      <c r="BG26" s="47"/>
-      <c r="BH26" s="47"/>
-      <c r="BI26" s="47"/>
-      <c r="BJ26" s="47"/>
-      <c r="BK26" s="47"/>
-      <c r="BL26" s="47"/>
-      <c r="BM26" s="47"/>
-      <c r="BN26" s="47"/>
-      <c r="BO26" s="47"/>
-      <c r="BP26" s="47"/>
-      <c r="BQ26" s="47"/>
-      <c r="BR26" s="47"/>
-      <c r="BS26" s="47"/>
-      <c r="BT26" s="47"/>
-      <c r="BU26" s="47"/>
-      <c r="BV26" s="47"/>
-      <c r="BW26" s="47"/>
-      <c r="BX26" s="47"/>
-      <c r="BY26" s="47"/>
-      <c r="BZ26" s="47"/>
-      <c r="CA26" s="47"/>
-      <c r="CB26" s="47"/>
-      <c r="CC26" s="47"/>
-      <c r="CD26" s="47"/>
-      <c r="CE26" s="47"/>
-      <c r="CF26" s="47"/>
-      <c r="CG26" s="47"/>
-      <c r="CH26" s="47"/>
-      <c r="CI26" s="47"/>
-      <c r="CJ26" s="47"/>
-      <c r="CK26" s="47"/>
-      <c r="CL26" s="47"/>
-      <c r="CM26" s="47"/>
-      <c r="CN26" s="47"/>
-      <c r="CO26" s="47"/>
-      <c r="CP26" s="47"/>
-      <c r="CQ26" s="47"/>
-      <c r="CR26" s="47"/>
-      <c r="CS26" s="47"/>
-      <c r="CT26" s="47"/>
-      <c r="CU26" s="47"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
+      <c r="V26" s="55"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="55"/>
+      <c r="Y26" s="55"/>
+      <c r="Z26" s="55"/>
+      <c r="AA26" s="55"/>
+      <c r="AB26" s="55"/>
+      <c r="AC26" s="55"/>
+      <c r="AD26" s="55"/>
+      <c r="AE26" s="55"/>
+      <c r="AF26" s="55"/>
+      <c r="AG26" s="55"/>
+      <c r="AH26" s="55"/>
+      <c r="AI26" s="55"/>
+      <c r="AJ26" s="55"/>
+      <c r="AK26" s="55"/>
+      <c r="AL26" s="55"/>
+      <c r="AM26" s="55"/>
+      <c r="AN26" s="55"/>
+      <c r="AO26" s="55"/>
+      <c r="AP26" s="55"/>
+      <c r="AQ26" s="55"/>
+      <c r="AR26" s="55"/>
+      <c r="AS26" s="55"/>
+      <c r="AT26" s="55"/>
+      <c r="AU26" s="55"/>
+      <c r="AV26" s="55"/>
+      <c r="AW26" s="55"/>
+      <c r="AX26" s="55"/>
+      <c r="AY26" s="55"/>
+      <c r="AZ26" s="55"/>
+      <c r="BA26" s="55"/>
+      <c r="BB26" s="55"/>
+      <c r="BC26" s="55"/>
+      <c r="BD26" s="55"/>
+      <c r="BE26" s="55"/>
+      <c r="BF26" s="55"/>
+      <c r="BG26" s="55"/>
+      <c r="BH26" s="55"/>
+      <c r="BI26" s="55"/>
+      <c r="BJ26" s="55"/>
+      <c r="BK26" s="55"/>
+      <c r="BL26" s="55"/>
+      <c r="BM26" s="55"/>
+      <c r="BN26" s="55"/>
+      <c r="BO26" s="55"/>
+      <c r="BP26" s="55"/>
+      <c r="BQ26" s="55"/>
+      <c r="BR26" s="55"/>
+      <c r="BS26" s="55"/>
+      <c r="BT26" s="55"/>
+      <c r="BU26" s="55"/>
+      <c r="BV26" s="55"/>
+      <c r="BW26" s="55"/>
+      <c r="BX26" s="55"/>
+      <c r="BY26" s="55"/>
+      <c r="BZ26" s="55"/>
+      <c r="CA26" s="55"/>
+      <c r="CB26" s="55"/>
+      <c r="CC26" s="55"/>
+      <c r="CD26" s="55"/>
+      <c r="CE26" s="55"/>
+      <c r="CF26" s="55"/>
+      <c r="CG26" s="55"/>
+      <c r="CH26" s="55"/>
+      <c r="CI26" s="55"/>
+      <c r="CJ26" s="55"/>
+      <c r="CK26" s="55"/>
+      <c r="CL26" s="55"/>
+      <c r="CM26" s="55"/>
+      <c r="CN26" s="55"/>
+      <c r="CO26" s="55"/>
+      <c r="CP26" s="55"/>
+      <c r="CQ26" s="55"/>
+      <c r="CR26" s="55"/>
+      <c r="CS26" s="55"/>
+      <c r="CT26" s="55"/>
+      <c r="CU26" s="55"/>
     </row>
     <row r="27" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
@@ -3939,105 +3939,105 @@
       <c r="CU30" s="35"/>
     </row>
     <row r="31" spans="1:99" s="45" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-      <c r="R31" s="48"/>
-      <c r="S31" s="48"/>
-      <c r="T31" s="48"/>
-      <c r="U31" s="48"/>
-      <c r="V31" s="48"/>
-      <c r="W31" s="48"/>
-      <c r="X31" s="48"/>
-      <c r="Y31" s="48"/>
-      <c r="Z31" s="48"/>
-      <c r="AA31" s="48"/>
-      <c r="AB31" s="48"/>
-      <c r="AC31" s="48"/>
-      <c r="AD31" s="48"/>
-      <c r="AE31" s="48"/>
-      <c r="AF31" s="48"/>
-      <c r="AG31" s="48"/>
-      <c r="AH31" s="48"/>
-      <c r="AI31" s="48"/>
-      <c r="AJ31" s="48"/>
-      <c r="AK31" s="48"/>
-      <c r="AL31" s="48"/>
-      <c r="AM31" s="48"/>
-      <c r="AN31" s="48"/>
-      <c r="AO31" s="48"/>
-      <c r="AP31" s="48"/>
-      <c r="AQ31" s="48"/>
-      <c r="AR31" s="48"/>
-      <c r="AS31" s="48"/>
-      <c r="AT31" s="48"/>
-      <c r="AU31" s="48"/>
-      <c r="AV31" s="48"/>
-      <c r="AW31" s="48"/>
-      <c r="AX31" s="48"/>
-      <c r="AY31" s="48"/>
-      <c r="AZ31" s="48"/>
-      <c r="BA31" s="48"/>
-      <c r="BB31" s="48"/>
-      <c r="BC31" s="48"/>
-      <c r="BD31" s="48"/>
-      <c r="BE31" s="48"/>
-      <c r="BF31" s="48"/>
-      <c r="BG31" s="48"/>
-      <c r="BH31" s="48"/>
-      <c r="BI31" s="48"/>
-      <c r="BJ31" s="48"/>
-      <c r="BK31" s="48"/>
-      <c r="BL31" s="48"/>
-      <c r="BM31" s="48"/>
-      <c r="BN31" s="48"/>
-      <c r="BO31" s="48"/>
-      <c r="BP31" s="48"/>
-      <c r="BQ31" s="48"/>
-      <c r="BR31" s="48"/>
-      <c r="BS31" s="48"/>
-      <c r="BT31" s="48"/>
-      <c r="BU31" s="48"/>
-      <c r="BV31" s="48"/>
-      <c r="BW31" s="48"/>
-      <c r="BX31" s="48"/>
-      <c r="BY31" s="48"/>
-      <c r="BZ31" s="48"/>
-      <c r="CA31" s="48"/>
-      <c r="CB31" s="48"/>
-      <c r="CC31" s="48"/>
-      <c r="CD31" s="48"/>
-      <c r="CE31" s="48"/>
-      <c r="CF31" s="48"/>
-      <c r="CG31" s="48"/>
-      <c r="CH31" s="48"/>
-      <c r="CI31" s="48"/>
-      <c r="CJ31" s="48"/>
-      <c r="CK31" s="48"/>
-      <c r="CL31" s="48"/>
-      <c r="CM31" s="48"/>
-      <c r="CN31" s="48"/>
-      <c r="CO31" s="48"/>
-      <c r="CP31" s="48"/>
-      <c r="CQ31" s="48"/>
-      <c r="CR31" s="48"/>
-      <c r="CS31" s="48"/>
-      <c r="CT31" s="48"/>
-      <c r="CU31" s="48"/>
+      <c r="A31" s="56"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
+      <c r="S31" s="56"/>
+      <c r="T31" s="56"/>
+      <c r="U31" s="56"/>
+      <c r="V31" s="56"/>
+      <c r="W31" s="56"/>
+      <c r="X31" s="56"/>
+      <c r="Y31" s="56"/>
+      <c r="Z31" s="56"/>
+      <c r="AA31" s="56"/>
+      <c r="AB31" s="56"/>
+      <c r="AC31" s="56"/>
+      <c r="AD31" s="56"/>
+      <c r="AE31" s="56"/>
+      <c r="AF31" s="56"/>
+      <c r="AG31" s="56"/>
+      <c r="AH31" s="56"/>
+      <c r="AI31" s="56"/>
+      <c r="AJ31" s="56"/>
+      <c r="AK31" s="56"/>
+      <c r="AL31" s="56"/>
+      <c r="AM31" s="56"/>
+      <c r="AN31" s="56"/>
+      <c r="AO31" s="56"/>
+      <c r="AP31" s="56"/>
+      <c r="AQ31" s="56"/>
+      <c r="AR31" s="56"/>
+      <c r="AS31" s="56"/>
+      <c r="AT31" s="56"/>
+      <c r="AU31" s="56"/>
+      <c r="AV31" s="56"/>
+      <c r="AW31" s="56"/>
+      <c r="AX31" s="56"/>
+      <c r="AY31" s="56"/>
+      <c r="AZ31" s="56"/>
+      <c r="BA31" s="56"/>
+      <c r="BB31" s="56"/>
+      <c r="BC31" s="56"/>
+      <c r="BD31" s="56"/>
+      <c r="BE31" s="56"/>
+      <c r="BF31" s="56"/>
+      <c r="BG31" s="56"/>
+      <c r="BH31" s="56"/>
+      <c r="BI31" s="56"/>
+      <c r="BJ31" s="56"/>
+      <c r="BK31" s="56"/>
+      <c r="BL31" s="56"/>
+      <c r="BM31" s="56"/>
+      <c r="BN31" s="56"/>
+      <c r="BO31" s="56"/>
+      <c r="BP31" s="56"/>
+      <c r="BQ31" s="56"/>
+      <c r="BR31" s="56"/>
+      <c r="BS31" s="56"/>
+      <c r="BT31" s="56"/>
+      <c r="BU31" s="56"/>
+      <c r="BV31" s="56"/>
+      <c r="BW31" s="56"/>
+      <c r="BX31" s="56"/>
+      <c r="BY31" s="56"/>
+      <c r="BZ31" s="56"/>
+      <c r="CA31" s="56"/>
+      <c r="CB31" s="56"/>
+      <c r="CC31" s="56"/>
+      <c r="CD31" s="56"/>
+      <c r="CE31" s="56"/>
+      <c r="CF31" s="56"/>
+      <c r="CG31" s="56"/>
+      <c r="CH31" s="56"/>
+      <c r="CI31" s="56"/>
+      <c r="CJ31" s="56"/>
+      <c r="CK31" s="56"/>
+      <c r="CL31" s="56"/>
+      <c r="CM31" s="56"/>
+      <c r="CN31" s="56"/>
+      <c r="CO31" s="56"/>
+      <c r="CP31" s="56"/>
+      <c r="CQ31" s="56"/>
+      <c r="CR31" s="56"/>
+      <c r="CS31" s="56"/>
+      <c r="CT31" s="56"/>
+      <c r="CU31" s="56"/>
     </row>
     <row r="32" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
@@ -6823,19 +6823,19 @@
         <v>121</v>
       </c>
       <c r="C68" s="41">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D68" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E68" s="41">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F68" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G68" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68" s="24"/>
       <c r="I68" s="31"/>
@@ -7611,38 +7611,11 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A57:CU57"/>
-    <mergeCell ref="B49:CU49"/>
-    <mergeCell ref="A52:CU52"/>
-    <mergeCell ref="CQ5:CU5"/>
-    <mergeCell ref="CQ6:CU6"/>
-    <mergeCell ref="BE2:BW2"/>
-    <mergeCell ref="BE3:BW3"/>
-    <mergeCell ref="CB5:CF5"/>
-    <mergeCell ref="CB6:CF6"/>
-    <mergeCell ref="CG5:CK5"/>
-    <mergeCell ref="CG6:CK6"/>
-    <mergeCell ref="CL5:CP5"/>
-    <mergeCell ref="CL6:CP6"/>
-    <mergeCell ref="BM5:BQ5"/>
-    <mergeCell ref="BM6:BQ6"/>
-    <mergeCell ref="BR5:BV5"/>
-    <mergeCell ref="BR6:BV6"/>
-    <mergeCell ref="BW5:CA5"/>
-    <mergeCell ref="BW6:CA6"/>
-    <mergeCell ref="AX5:BB5"/>
-    <mergeCell ref="AX6:BB6"/>
-    <mergeCell ref="BC5:BG5"/>
-    <mergeCell ref="BC6:BG6"/>
-    <mergeCell ref="BH5:BL5"/>
-    <mergeCell ref="BH6:BL6"/>
-    <mergeCell ref="AI5:AM5"/>
-    <mergeCell ref="AI6:AM6"/>
-    <mergeCell ref="AN5:AR5"/>
-    <mergeCell ref="AN6:AR6"/>
-    <mergeCell ref="AS5:AW5"/>
-    <mergeCell ref="AS6:AW6"/>
-    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="A13:CU13"/>
+    <mergeCell ref="B21:CU21"/>
+    <mergeCell ref="B26:CU26"/>
+    <mergeCell ref="A31:CU31"/>
+    <mergeCell ref="A42:CU42"/>
     <mergeCell ref="Y6:AC6"/>
     <mergeCell ref="AD5:AH5"/>
     <mergeCell ref="AD6:AH6"/>
@@ -7653,11 +7626,38 @@
     <mergeCell ref="O6:S6"/>
     <mergeCell ref="T5:X5"/>
     <mergeCell ref="T6:X6"/>
-    <mergeCell ref="A13:CU13"/>
-    <mergeCell ref="B21:CU21"/>
-    <mergeCell ref="B26:CU26"/>
-    <mergeCell ref="A31:CU31"/>
-    <mergeCell ref="A42:CU42"/>
+    <mergeCell ref="BE2:BW2"/>
+    <mergeCell ref="BE3:BW3"/>
+    <mergeCell ref="CB5:CF5"/>
+    <mergeCell ref="CB6:CF6"/>
+    <mergeCell ref="CG5:CK5"/>
+    <mergeCell ref="CG6:CK6"/>
+    <mergeCell ref="BM5:BQ5"/>
+    <mergeCell ref="BM6:BQ6"/>
+    <mergeCell ref="BR5:BV5"/>
+    <mergeCell ref="BR6:BV6"/>
+    <mergeCell ref="BW5:CA5"/>
+    <mergeCell ref="BW6:CA6"/>
+    <mergeCell ref="BC5:BG5"/>
+    <mergeCell ref="BC6:BG6"/>
+    <mergeCell ref="BH5:BL5"/>
+    <mergeCell ref="BH6:BL6"/>
+    <mergeCell ref="A57:CU57"/>
+    <mergeCell ref="B49:CU49"/>
+    <mergeCell ref="A52:CU52"/>
+    <mergeCell ref="CQ5:CU5"/>
+    <mergeCell ref="CQ6:CU6"/>
+    <mergeCell ref="CL5:CP5"/>
+    <mergeCell ref="CL6:CP6"/>
+    <mergeCell ref="AX5:BB5"/>
+    <mergeCell ref="AX6:BB6"/>
+    <mergeCell ref="AI5:AM5"/>
+    <mergeCell ref="AI6:AM6"/>
+    <mergeCell ref="AN5:AR5"/>
+    <mergeCell ref="AN6:AR6"/>
+    <mergeCell ref="AS5:AW5"/>
+    <mergeCell ref="AS6:AW6"/>
+    <mergeCell ref="Y5:AC5"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J53:CU56 J50:CU51 J32:CU41 J43:CU48 J58:CU59 J74:CU74">
     <cfRule type="expression" dxfId="25" priority="84">

</xml_diff>

<commit_message>
ready to share with u guys
</commit_message>
<xml_diff>
--- a/LaTeX Project/Documentos/Gantt.xlsx
+++ b/LaTeX Project/Documentos/Gantt.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="125">
   <si>
     <t>Dalle Pad</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>Luis Felipe Mazzuchetti Ortiz</t>
+  </si>
+  <si>
+    <t>MIDI</t>
   </si>
 </sst>
 </file>
@@ -1022,9 +1025,6 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="10" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1033,6 +1033,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1805,10 +1808,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:CU83"/>
+  <dimension ref="A2:CU84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1845,27 +1848,27 @@
         <v>78</v>
       </c>
       <c r="I2" s="16"/>
-      <c r="BE2" s="50" t="s">
+      <c r="BE2" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" s="50"/>
-      <c r="BG2" s="50"/>
-      <c r="BH2" s="50"/>
-      <c r="BI2" s="50"/>
-      <c r="BJ2" s="50"/>
-      <c r="BK2" s="50"/>
-      <c r="BL2" s="50"/>
-      <c r="BM2" s="50"/>
-      <c r="BN2" s="50"/>
-      <c r="BO2" s="50"/>
-      <c r="BP2" s="50"/>
-      <c r="BQ2" s="50"/>
-      <c r="BR2" s="50"/>
-      <c r="BS2" s="50"/>
-      <c r="BT2" s="50"/>
-      <c r="BU2" s="50"/>
-      <c r="BV2" s="50"/>
-      <c r="BW2" s="50"/>
+      <c r="BF2" s="53"/>
+      <c r="BG2" s="53"/>
+      <c r="BH2" s="53"/>
+      <c r="BI2" s="53"/>
+      <c r="BJ2" s="53"/>
+      <c r="BK2" s="53"/>
+      <c r="BL2" s="53"/>
+      <c r="BM2" s="53"/>
+      <c r="BN2" s="53"/>
+      <c r="BO2" s="53"/>
+      <c r="BP2" s="53"/>
+      <c r="BQ2" s="53"/>
+      <c r="BR2" s="53"/>
+      <c r="BS2" s="53"/>
+      <c r="BT2" s="53"/>
+      <c r="BU2" s="53"/>
+      <c r="BV2" s="53"/>
+      <c r="BW2" s="53"/>
     </row>
     <row r="3" spans="1:99" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="54"/>
@@ -1922,27 +1925,27 @@
       <c r="AQ3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="BE3" s="50" t="s">
+      <c r="BE3" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="BF3" s="50"/>
-      <c r="BG3" s="50"/>
-      <c r="BH3" s="50"/>
-      <c r="BI3" s="50"/>
-      <c r="BJ3" s="50"/>
-      <c r="BK3" s="50"/>
-      <c r="BL3" s="50"/>
-      <c r="BM3" s="50"/>
-      <c r="BN3" s="50"/>
-      <c r="BO3" s="50"/>
-      <c r="BP3" s="50"/>
-      <c r="BQ3" s="50"/>
-      <c r="BR3" s="50"/>
-      <c r="BS3" s="50"/>
-      <c r="BT3" s="50"/>
-      <c r="BU3" s="50"/>
-      <c r="BV3" s="50"/>
-      <c r="BW3" s="50"/>
+      <c r="BF3" s="53"/>
+      <c r="BG3" s="53"/>
+      <c r="BH3" s="53"/>
+      <c r="BI3" s="53"/>
+      <c r="BJ3" s="53"/>
+      <c r="BK3" s="53"/>
+      <c r="BL3" s="53"/>
+      <c r="BM3" s="53"/>
+      <c r="BN3" s="53"/>
+      <c r="BO3" s="53"/>
+      <c r="BP3" s="53"/>
+      <c r="BQ3" s="53"/>
+      <c r="BR3" s="53"/>
+      <c r="BS3" s="53"/>
+      <c r="BT3" s="53"/>
+      <c r="BU3" s="53"/>
+      <c r="BV3" s="53"/>
+      <c r="BW3" s="53"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="54"/>
@@ -1981,13 +1984,13 @@
       <c r="AY4" s="19"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="J5" s="51" t="s">
+      <c r="J5" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="53"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
       <c r="O5" s="47" t="s">
         <v>18</v>
       </c>
@@ -1995,13 +1998,13 @@
       <c r="Q5" s="48"/>
       <c r="R5" s="48"/>
       <c r="S5" s="49"/>
-      <c r="T5" s="51" t="s">
+      <c r="T5" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="53"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="52"/>
       <c r="Y5" s="47" t="s">
         <v>20</v>
       </c>
@@ -2009,13 +2012,13 @@
       <c r="AA5" s="48"/>
       <c r="AB5" s="48"/>
       <c r="AC5" s="49"/>
-      <c r="AD5" s="51" t="s">
+      <c r="AD5" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="52"/>
-      <c r="AF5" s="52"/>
-      <c r="AG5" s="52"/>
-      <c r="AH5" s="53"/>
+      <c r="AE5" s="51"/>
+      <c r="AF5" s="51"/>
+      <c r="AG5" s="51"/>
+      <c r="AH5" s="52"/>
       <c r="AI5" s="47" t="s">
         <v>22</v>
       </c>
@@ -2023,13 +2026,13 @@
       <c r="AK5" s="48"/>
       <c r="AL5" s="48"/>
       <c r="AM5" s="49"/>
-      <c r="AN5" s="51" t="s">
+      <c r="AN5" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="52"/>
-      <c r="AP5" s="52"/>
-      <c r="AQ5" s="52"/>
-      <c r="AR5" s="53"/>
+      <c r="AO5" s="51"/>
+      <c r="AP5" s="51"/>
+      <c r="AQ5" s="51"/>
+      <c r="AR5" s="52"/>
       <c r="AS5" s="47" t="s">
         <v>24</v>
       </c>
@@ -2037,13 +2040,13 @@
       <c r="AU5" s="48"/>
       <c r="AV5" s="48"/>
       <c r="AW5" s="49"/>
-      <c r="AX5" s="51" t="s">
+      <c r="AX5" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="AY5" s="52"/>
-      <c r="AZ5" s="52"/>
-      <c r="BA5" s="52"/>
-      <c r="BB5" s="53"/>
+      <c r="AY5" s="51"/>
+      <c r="AZ5" s="51"/>
+      <c r="BA5" s="51"/>
+      <c r="BB5" s="52"/>
       <c r="BC5" s="47" t="s">
         <v>26</v>
       </c>
@@ -2051,13 +2054,13 @@
       <c r="BE5" s="48"/>
       <c r="BF5" s="48"/>
       <c r="BG5" s="49"/>
-      <c r="BH5" s="51" t="s">
+      <c r="BH5" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="BI5" s="52"/>
-      <c r="BJ5" s="52"/>
-      <c r="BK5" s="52"/>
-      <c r="BL5" s="53"/>
+      <c r="BI5" s="51"/>
+      <c r="BJ5" s="51"/>
+      <c r="BK5" s="51"/>
+      <c r="BL5" s="52"/>
       <c r="BM5" s="47" t="s">
         <v>28</v>
       </c>
@@ -2065,13 +2068,13 @@
       <c r="BO5" s="48"/>
       <c r="BP5" s="48"/>
       <c r="BQ5" s="49"/>
-      <c r="BR5" s="51" t="s">
+      <c r="BR5" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="BS5" s="52"/>
-      <c r="BT5" s="52"/>
-      <c r="BU5" s="52"/>
-      <c r="BV5" s="53"/>
+      <c r="BS5" s="51"/>
+      <c r="BT5" s="51"/>
+      <c r="BU5" s="51"/>
+      <c r="BV5" s="52"/>
       <c r="BW5" s="47" t="s">
         <v>30</v>
       </c>
@@ -2079,13 +2082,13 @@
       <c r="BY5" s="48"/>
       <c r="BZ5" s="48"/>
       <c r="CA5" s="49"/>
-      <c r="CB5" s="51" t="s">
+      <c r="CB5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="CC5" s="52"/>
-      <c r="CD5" s="52"/>
-      <c r="CE5" s="52"/>
-      <c r="CF5" s="53"/>
+      <c r="CC5" s="51"/>
+      <c r="CD5" s="51"/>
+      <c r="CE5" s="51"/>
+      <c r="CF5" s="52"/>
       <c r="CG5" s="47" t="s">
         <v>32</v>
       </c>
@@ -2093,13 +2096,13 @@
       <c r="CI5" s="48"/>
       <c r="CJ5" s="48"/>
       <c r="CK5" s="49"/>
-      <c r="CL5" s="51" t="s">
+      <c r="CL5" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="CM5" s="52"/>
-      <c r="CN5" s="52"/>
-      <c r="CO5" s="52"/>
-      <c r="CP5" s="53"/>
+      <c r="CM5" s="51"/>
+      <c r="CN5" s="51"/>
+      <c r="CO5" s="51"/>
+      <c r="CP5" s="52"/>
       <c r="CQ5" s="47" t="s">
         <v>34</v>
       </c>
@@ -2129,13 +2132,13 @@
         <v>75</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="53"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="52"/>
       <c r="O6" s="47" t="s">
         <v>36</v>
       </c>
@@ -2143,13 +2146,13 @@
       <c r="Q6" s="48"/>
       <c r="R6" s="48"/>
       <c r="S6" s="49"/>
-      <c r="T6" s="51" t="s">
+      <c r="T6" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="52"/>
-      <c r="X6" s="53"/>
+      <c r="U6" s="51"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="51"/>
+      <c r="X6" s="52"/>
       <c r="Y6" s="47" t="s">
         <v>38</v>
       </c>
@@ -2157,13 +2160,13 @@
       <c r="AA6" s="48"/>
       <c r="AB6" s="48"/>
       <c r="AC6" s="49"/>
-      <c r="AD6" s="51" t="s">
+      <c r="AD6" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="52"/>
-      <c r="AF6" s="52"/>
-      <c r="AG6" s="52"/>
-      <c r="AH6" s="53"/>
+      <c r="AE6" s="51"/>
+      <c r="AF6" s="51"/>
+      <c r="AG6" s="51"/>
+      <c r="AH6" s="52"/>
       <c r="AI6" s="47" t="s">
         <v>40</v>
       </c>
@@ -2171,13 +2174,13 @@
       <c r="AK6" s="48"/>
       <c r="AL6" s="48"/>
       <c r="AM6" s="49"/>
-      <c r="AN6" s="51" t="s">
+      <c r="AN6" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" s="52"/>
-      <c r="AP6" s="52"/>
-      <c r="AQ6" s="52"/>
-      <c r="AR6" s="53"/>
+      <c r="AO6" s="51"/>
+      <c r="AP6" s="51"/>
+      <c r="AQ6" s="51"/>
+      <c r="AR6" s="52"/>
       <c r="AS6" s="47" t="s">
         <v>42</v>
       </c>
@@ -2185,13 +2188,13 @@
       <c r="AU6" s="48"/>
       <c r="AV6" s="48"/>
       <c r="AW6" s="49"/>
-      <c r="AX6" s="51" t="s">
+      <c r="AX6" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="AY6" s="52"/>
-      <c r="AZ6" s="52"/>
-      <c r="BA6" s="52"/>
-      <c r="BB6" s="53"/>
+      <c r="AY6" s="51"/>
+      <c r="AZ6" s="51"/>
+      <c r="BA6" s="51"/>
+      <c r="BB6" s="52"/>
       <c r="BC6" s="47" t="s">
         <v>44</v>
       </c>
@@ -2199,13 +2202,13 @@
       <c r="BE6" s="48"/>
       <c r="BF6" s="48"/>
       <c r="BG6" s="49"/>
-      <c r="BH6" s="51" t="s">
+      <c r="BH6" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="BI6" s="52"/>
-      <c r="BJ6" s="52"/>
-      <c r="BK6" s="52"/>
-      <c r="BL6" s="53"/>
+      <c r="BI6" s="51"/>
+      <c r="BJ6" s="51"/>
+      <c r="BK6" s="51"/>
+      <c r="BL6" s="52"/>
       <c r="BM6" s="47" t="s">
         <v>46</v>
       </c>
@@ -2213,13 +2216,13 @@
       <c r="BO6" s="48"/>
       <c r="BP6" s="48"/>
       <c r="BQ6" s="49"/>
-      <c r="BR6" s="51" t="s">
+      <c r="BR6" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="BS6" s="52"/>
-      <c r="BT6" s="52"/>
-      <c r="BU6" s="52"/>
-      <c r="BV6" s="53"/>
+      <c r="BS6" s="51"/>
+      <c r="BT6" s="51"/>
+      <c r="BU6" s="51"/>
+      <c r="BV6" s="52"/>
       <c r="BW6" s="47" t="s">
         <v>48</v>
       </c>
@@ -2227,13 +2230,13 @@
       <c r="BY6" s="48"/>
       <c r="BZ6" s="48"/>
       <c r="CA6" s="49"/>
-      <c r="CB6" s="51" t="s">
+      <c r="CB6" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="CC6" s="52"/>
-      <c r="CD6" s="52"/>
-      <c r="CE6" s="52"/>
-      <c r="CF6" s="53"/>
+      <c r="CC6" s="51"/>
+      <c r="CD6" s="51"/>
+      <c r="CE6" s="51"/>
+      <c r="CF6" s="52"/>
       <c r="CG6" s="47" t="s">
         <v>50</v>
       </c>
@@ -2241,13 +2244,13 @@
       <c r="CI6" s="48"/>
       <c r="CJ6" s="48"/>
       <c r="CK6" s="49"/>
-      <c r="CL6" s="51" t="s">
+      <c r="CL6" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="CM6" s="52"/>
-      <c r="CN6" s="52"/>
-      <c r="CO6" s="52"/>
-      <c r="CP6" s="53"/>
+      <c r="CM6" s="51"/>
+      <c r="CN6" s="51"/>
+      <c r="CO6" s="51"/>
+      <c r="CP6" s="52"/>
       <c r="CQ6" s="47" t="s">
         <v>52</v>
       </c>
@@ -5186,7 +5189,7 @@
       <c r="CT46" s="35"/>
       <c r="CU46" s="35"/>
     </row>
-    <row r="47" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:99" s="28" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="38" t="s">
         <v>88</v>
       </c>
@@ -6312,7 +6315,7 @@
         <v>3</v>
       </c>
       <c r="G61" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="24" t="s">
         <v>77</v>
@@ -7038,20 +7041,20 @@
       <c r="CU70" s="35"/>
     </row>
     <row r="71" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="38" t="s">
-        <v>111</v>
+      <c r="B71" s="40" t="s">
+        <v>124</v>
       </c>
       <c r="C71" s="41">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D71" s="41">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E71" s="41">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F71" s="41">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="G71" s="30">
         <v>0</v>
@@ -7112,19 +7115,19 @@
     </row>
     <row r="72" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C72" s="41">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="D72" s="41">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E72" s="41">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="F72" s="41">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="G72" s="30">
         <v>0</v>
@@ -7185,19 +7188,19 @@
     </row>
     <row r="73" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C73" s="41">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D73" s="41">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E73" s="41">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F73" s="41">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G73" s="30">
         <v>0</v>
@@ -7258,19 +7261,19 @@
     </row>
     <row r="74" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="38" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C74" s="41">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D74" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E74" s="41">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F74" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G74" s="30">
         <v>0</v>
@@ -7330,20 +7333,20 @@
       <c r="CU74" s="35"/>
     </row>
     <row r="75" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="39" t="s">
-        <v>108</v>
+      <c r="B75" s="38" t="s">
+        <v>107</v>
       </c>
       <c r="C75" s="41">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D75" s="41">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E75" s="41">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F75" s="41">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G75" s="30">
         <v>0</v>
@@ -7402,60 +7405,81 @@
       <c r="CT75" s="35"/>
       <c r="CU75" s="35"/>
     </row>
-    <row r="76" spans="2:99" x14ac:dyDescent="0.3">
-      <c r="H76" s="27"/>
-      <c r="J76" s="19"/>
-      <c r="K76" s="19"/>
-      <c r="L76" s="19"/>
-      <c r="M76" s="19"/>
-      <c r="N76" s="19"/>
-      <c r="O76" s="19"/>
-      <c r="P76" s="19"/>
-      <c r="Q76" s="19"/>
-      <c r="R76" s="19"/>
-      <c r="S76" s="19"/>
-      <c r="T76" s="19"/>
-      <c r="U76" s="19"/>
-      <c r="V76" s="19"/>
-      <c r="W76" s="19"/>
-      <c r="X76" s="19"/>
-      <c r="Y76" s="19"/>
-      <c r="Z76" s="19"/>
-      <c r="AA76" s="19"/>
-      <c r="AB76" s="19"/>
-      <c r="AC76" s="19"/>
-      <c r="BR76" s="21"/>
-      <c r="BS76" s="21"/>
-      <c r="BT76" s="21"/>
-      <c r="BU76" s="21"/>
-      <c r="BV76" s="21"/>
-      <c r="BW76" s="21"/>
-      <c r="BX76" s="21"/>
-      <c r="BY76" s="21"/>
-      <c r="BZ76" s="21"/>
-      <c r="CA76" s="21"/>
-      <c r="CB76" s="21"/>
-      <c r="CC76" s="21"/>
-      <c r="CD76" s="21"/>
-      <c r="CE76" s="21"/>
-      <c r="CF76" s="21"/>
-      <c r="CG76" s="21"/>
-      <c r="CH76" s="21"/>
-      <c r="CI76" s="21"/>
-      <c r="CJ76" s="21"/>
-      <c r="CK76" s="21"/>
-      <c r="CL76" s="21"/>
-      <c r="CM76" s="21"/>
-      <c r="CN76" s="21"/>
-      <c r="CO76" s="21"/>
-      <c r="CP76" s="21"/>
-      <c r="CQ76" s="21"/>
-      <c r="CR76" s="21"/>
-      <c r="CS76" s="21"/>
-      <c r="CT76" s="21"/>
-      <c r="CU76" s="21"/>
+    <row r="76" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C76" s="41">
+        <v>86</v>
+      </c>
+      <c r="D76" s="41">
+        <v>7</v>
+      </c>
+      <c r="E76" s="41">
+        <v>86</v>
+      </c>
+      <c r="F76" s="41">
+        <v>7</v>
+      </c>
+      <c r="G76" s="30">
+        <v>0</v>
+      </c>
+      <c r="H76" s="24"/>
+      <c r="I76" s="31"/>
+      <c r="J76" s="31"/>
+      <c r="K76" s="31"/>
+      <c r="L76" s="31"/>
+      <c r="M76" s="31"/>
+      <c r="N76" s="31"/>
+      <c r="O76" s="31"/>
+      <c r="P76" s="31"/>
+      <c r="Q76" s="31"/>
+      <c r="R76" s="31"/>
+      <c r="S76" s="31"/>
+      <c r="T76" s="31"/>
+      <c r="U76" s="31"/>
+      <c r="V76" s="31"/>
+      <c r="W76" s="31"/>
+      <c r="X76" s="31"/>
+      <c r="Y76" s="31"/>
+      <c r="Z76" s="31"/>
+      <c r="AA76" s="31"/>
+      <c r="AB76" s="31"/>
+      <c r="AC76" s="31"/>
+      <c r="BQ76" s="33"/>
+      <c r="BR76" s="34"/>
+      <c r="BS76" s="33"/>
+      <c r="BT76" s="33"/>
+      <c r="BU76" s="33"/>
+      <c r="BV76" s="33"/>
+      <c r="BW76" s="33"/>
+      <c r="BX76" s="33"/>
+      <c r="BY76" s="33"/>
+      <c r="BZ76" s="33"/>
+      <c r="CA76" s="33"/>
+      <c r="CB76" s="33"/>
+      <c r="CC76" s="33"/>
+      <c r="CD76" s="33"/>
+      <c r="CE76" s="33"/>
+      <c r="CF76" s="33"/>
+      <c r="CG76" s="33"/>
+      <c r="CH76" s="35"/>
+      <c r="CI76" s="35"/>
+      <c r="CJ76" s="35"/>
+      <c r="CK76" s="35"/>
+      <c r="CL76" s="35"/>
+      <c r="CM76" s="35"/>
+      <c r="CN76" s="35"/>
+      <c r="CO76" s="35"/>
+      <c r="CP76" s="35"/>
+      <c r="CQ76" s="35"/>
+      <c r="CR76" s="35"/>
+      <c r="CS76" s="35"/>
+      <c r="CT76" s="35"/>
+      <c r="CU76" s="35"/>
     </row>
     <row r="77" spans="2:99" x14ac:dyDescent="0.3">
+      <c r="H77" s="27"/>
       <c r="J77" s="19"/>
       <c r="K77" s="19"/>
       <c r="L77" s="19"/>
@@ -7476,6 +7500,36 @@
       <c r="AA77" s="19"/>
       <c r="AB77" s="19"/>
       <c r="AC77" s="19"/>
+      <c r="BR77" s="21"/>
+      <c r="BS77" s="21"/>
+      <c r="BT77" s="21"/>
+      <c r="BU77" s="21"/>
+      <c r="BV77" s="21"/>
+      <c r="BW77" s="21"/>
+      <c r="BX77" s="21"/>
+      <c r="BY77" s="21"/>
+      <c r="BZ77" s="21"/>
+      <c r="CA77" s="21"/>
+      <c r="CB77" s="21"/>
+      <c r="CC77" s="21"/>
+      <c r="CD77" s="21"/>
+      <c r="CE77" s="21"/>
+      <c r="CF77" s="21"/>
+      <c r="CG77" s="21"/>
+      <c r="CH77" s="21"/>
+      <c r="CI77" s="21"/>
+      <c r="CJ77" s="21"/>
+      <c r="CK77" s="21"/>
+      <c r="CL77" s="21"/>
+      <c r="CM77" s="21"/>
+      <c r="CN77" s="21"/>
+      <c r="CO77" s="21"/>
+      <c r="CP77" s="21"/>
+      <c r="CQ77" s="21"/>
+      <c r="CR77" s="21"/>
+      <c r="CS77" s="21"/>
+      <c r="CT77" s="21"/>
+      <c r="CU77" s="21"/>
     </row>
     <row r="78" spans="2:99" x14ac:dyDescent="0.3">
       <c r="J78" s="19"/>
@@ -7608,6 +7662,28 @@
       <c r="AA83" s="19"/>
       <c r="AB83" s="19"/>
       <c r="AC83" s="19"/>
+    </row>
+    <row r="84" spans="10:29" x14ac:dyDescent="0.3">
+      <c r="J84" s="19"/>
+      <c r="K84" s="19"/>
+      <c r="L84" s="19"/>
+      <c r="M84" s="19"/>
+      <c r="N84" s="19"/>
+      <c r="O84" s="19"/>
+      <c r="P84" s="19"/>
+      <c r="Q84" s="19"/>
+      <c r="R84" s="19"/>
+      <c r="S84" s="19"/>
+      <c r="T84" s="19"/>
+      <c r="U84" s="19"/>
+      <c r="V84" s="19"/>
+      <c r="W84" s="19"/>
+      <c r="X84" s="19"/>
+      <c r="Y84" s="19"/>
+      <c r="Z84" s="19"/>
+      <c r="AA84" s="19"/>
+      <c r="AB84" s="19"/>
+      <c r="AC84" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -7659,7 +7735,7 @@
     <mergeCell ref="AS6:AW6"/>
     <mergeCell ref="Y5:AC5"/>
   </mergeCells>
-  <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J53:CU56 J50:CU51 J32:CU41 J43:CU48 J58:CU59 J74:CU74">
+  <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J53:CU56 J50:CU51 J32:CU41 J43:CU48 J58:CU59 J75:CU75">
     <cfRule type="expression" dxfId="25" priority="84">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -7685,7 +7761,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B76:G76 I76:BQ76">
+  <conditionalFormatting sqref="B77:G77 I77:BQ77">
     <cfRule type="expression" dxfId="17" priority="85">
       <formula>TRUE</formula>
     </cfRule>
@@ -7695,7 +7771,7 @@
       <formula>J$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J75:CU75">
+  <conditionalFormatting sqref="J76:CU76">
     <cfRule type="expression" dxfId="15" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -7721,7 +7797,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J60:CU73">
+  <conditionalFormatting sqref="J60:CU74">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>

<commit_message>
escrito: Objetivos; Delimitação do estudo....      Melhorado: Tema....      Falta escrever: Procedimentos Metodológicos, Justificativa e Problema
</commit_message>
<xml_diff>
--- a/LaTeX Project/Documentos/Gantt.xlsx
+++ b/LaTeX Project/Documentos/Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -376,9 +376,6 @@
     <t>Finalização do aplicativo para Android</t>
   </si>
   <si>
-    <t>Finalização do software para Windows</t>
-  </si>
-  <si>
     <t>Ensaio pré-defesa</t>
   </si>
   <si>
@@ -476,6 +473,9 @@
   </si>
   <si>
     <t>MIDI</t>
+  </si>
+  <si>
+    <t>Finalização do software para Windows e detalhes finais</t>
   </si>
 </sst>
 </file>
@@ -1016,6 +1016,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1034,16 +1040,10 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1810,8 +1810,8 @@
   </sheetPr>
   <dimension ref="A2:CU84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AI61" sqref="AI61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1836,47 +1836,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="24" t="s">
         <v>78</v>
       </c>
       <c r="I2" s="16"/>
-      <c r="BE2" s="53" t="s">
+      <c r="BE2" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" s="53"/>
-      <c r="BG2" s="53"/>
-      <c r="BH2" s="53"/>
-      <c r="BI2" s="53"/>
-      <c r="BJ2" s="53"/>
-      <c r="BK2" s="53"/>
-      <c r="BL2" s="53"/>
-      <c r="BM2" s="53"/>
-      <c r="BN2" s="53"/>
-      <c r="BO2" s="53"/>
-      <c r="BP2" s="53"/>
-      <c r="BQ2" s="53"/>
-      <c r="BR2" s="53"/>
-      <c r="BS2" s="53"/>
-      <c r="BT2" s="53"/>
-      <c r="BU2" s="53"/>
-      <c r="BV2" s="53"/>
-      <c r="BW2" s="53"/>
+      <c r="BF2" s="56"/>
+      <c r="BG2" s="56"/>
+      <c r="BH2" s="56"/>
+      <c r="BI2" s="56"/>
+      <c r="BJ2" s="56"/>
+      <c r="BK2" s="56"/>
+      <c r="BL2" s="56"/>
+      <c r="BM2" s="56"/>
+      <c r="BN2" s="56"/>
+      <c r="BO2" s="56"/>
+      <c r="BP2" s="56"/>
+      <c r="BQ2" s="56"/>
+      <c r="BR2" s="56"/>
+      <c r="BS2" s="56"/>
+      <c r="BT2" s="56"/>
+      <c r="BU2" s="56"/>
+      <c r="BV2" s="56"/>
+      <c r="BW2" s="56"/>
     </row>
     <row r="3" spans="1:99" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="24" t="s">
         <v>79</v>
       </c>
@@ -1925,35 +1925,35 @@
       <c r="AQ3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="BE3" s="53" t="s">
+      <c r="BE3" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="BF3" s="53"/>
-      <c r="BG3" s="53"/>
-      <c r="BH3" s="53"/>
-      <c r="BI3" s="53"/>
-      <c r="BJ3" s="53"/>
-      <c r="BK3" s="53"/>
-      <c r="BL3" s="53"/>
-      <c r="BM3" s="53"/>
-      <c r="BN3" s="53"/>
-      <c r="BO3" s="53"/>
-      <c r="BP3" s="53"/>
-      <c r="BQ3" s="53"/>
-      <c r="BR3" s="53"/>
-      <c r="BS3" s="53"/>
-      <c r="BT3" s="53"/>
-      <c r="BU3" s="53"/>
-      <c r="BV3" s="53"/>
-      <c r="BW3" s="53"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
+      <c r="BI3" s="56"/>
+      <c r="BJ3" s="56"/>
+      <c r="BK3" s="56"/>
+      <c r="BL3" s="56"/>
+      <c r="BM3" s="56"/>
+      <c r="BN3" s="56"/>
+      <c r="BO3" s="56"/>
+      <c r="BP3" s="56"/>
+      <c r="BQ3" s="56"/>
+      <c r="BR3" s="56"/>
+      <c r="BS3" s="56"/>
+      <c r="BT3" s="56"/>
+      <c r="BU3" s="56"/>
+      <c r="BV3" s="56"/>
+      <c r="BW3" s="56"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="24" t="s">
         <v>80</v>
       </c>
@@ -1984,132 +1984,132 @@
       <c r="AY4" s="19"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="47" t="s">
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="50" t="s">
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="47" t="s">
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="48"/>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="50" t="s">
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="50"/>
+      <c r="AB5" s="50"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="51"/>
-      <c r="AF5" s="51"/>
-      <c r="AG5" s="51"/>
-      <c r="AH5" s="52"/>
-      <c r="AI5" s="47" t="s">
+      <c r="AE5" s="53"/>
+      <c r="AF5" s="53"/>
+      <c r="AG5" s="53"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="48"/>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="49"/>
-      <c r="AN5" s="50" t="s">
+      <c r="AJ5" s="50"/>
+      <c r="AK5" s="50"/>
+      <c r="AL5" s="50"/>
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="51"/>
-      <c r="AP5" s="51"/>
-      <c r="AQ5" s="51"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="47" t="s">
+      <c r="AO5" s="53"/>
+      <c r="AP5" s="53"/>
+      <c r="AQ5" s="53"/>
+      <c r="AR5" s="54"/>
+      <c r="AS5" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="AT5" s="48"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="48"/>
-      <c r="AW5" s="49"/>
-      <c r="AX5" s="50" t="s">
+      <c r="AT5" s="50"/>
+      <c r="AU5" s="50"/>
+      <c r="AV5" s="50"/>
+      <c r="AW5" s="51"/>
+      <c r="AX5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="AY5" s="51"/>
-      <c r="AZ5" s="51"/>
-      <c r="BA5" s="51"/>
-      <c r="BB5" s="52"/>
-      <c r="BC5" s="47" t="s">
+      <c r="AY5" s="53"/>
+      <c r="AZ5" s="53"/>
+      <c r="BA5" s="53"/>
+      <c r="BB5" s="54"/>
+      <c r="BC5" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="BD5" s="48"/>
-      <c r="BE5" s="48"/>
-      <c r="BF5" s="48"/>
-      <c r="BG5" s="49"/>
-      <c r="BH5" s="50" t="s">
+      <c r="BD5" s="50"/>
+      <c r="BE5" s="50"/>
+      <c r="BF5" s="50"/>
+      <c r="BG5" s="51"/>
+      <c r="BH5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="BI5" s="51"/>
-      <c r="BJ5" s="51"/>
-      <c r="BK5" s="51"/>
-      <c r="BL5" s="52"/>
-      <c r="BM5" s="47" t="s">
+      <c r="BI5" s="53"/>
+      <c r="BJ5" s="53"/>
+      <c r="BK5" s="53"/>
+      <c r="BL5" s="54"/>
+      <c r="BM5" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="BN5" s="48"/>
-      <c r="BO5" s="48"/>
-      <c r="BP5" s="48"/>
-      <c r="BQ5" s="49"/>
-      <c r="BR5" s="50" t="s">
+      <c r="BN5" s="50"/>
+      <c r="BO5" s="50"/>
+      <c r="BP5" s="50"/>
+      <c r="BQ5" s="51"/>
+      <c r="BR5" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="BS5" s="51"/>
-      <c r="BT5" s="51"/>
-      <c r="BU5" s="51"/>
-      <c r="BV5" s="52"/>
-      <c r="BW5" s="47" t="s">
+      <c r="BS5" s="53"/>
+      <c r="BT5" s="53"/>
+      <c r="BU5" s="53"/>
+      <c r="BV5" s="54"/>
+      <c r="BW5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="BX5" s="48"/>
-      <c r="BY5" s="48"/>
-      <c r="BZ5" s="48"/>
-      <c r="CA5" s="49"/>
-      <c r="CB5" s="50" t="s">
+      <c r="BX5" s="50"/>
+      <c r="BY5" s="50"/>
+      <c r="BZ5" s="50"/>
+      <c r="CA5" s="51"/>
+      <c r="CB5" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="CC5" s="51"/>
-      <c r="CD5" s="51"/>
-      <c r="CE5" s="51"/>
-      <c r="CF5" s="52"/>
-      <c r="CG5" s="47" t="s">
+      <c r="CC5" s="53"/>
+      <c r="CD5" s="53"/>
+      <c r="CE5" s="53"/>
+      <c r="CF5" s="54"/>
+      <c r="CG5" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="CH5" s="48"/>
-      <c r="CI5" s="48"/>
-      <c r="CJ5" s="48"/>
-      <c r="CK5" s="49"/>
-      <c r="CL5" s="50" t="s">
+      <c r="CH5" s="50"/>
+      <c r="CI5" s="50"/>
+      <c r="CJ5" s="50"/>
+      <c r="CK5" s="51"/>
+      <c r="CL5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="CM5" s="51"/>
-      <c r="CN5" s="51"/>
-      <c r="CO5" s="51"/>
-      <c r="CP5" s="52"/>
-      <c r="CQ5" s="47" t="s">
+      <c r="CM5" s="53"/>
+      <c r="CN5" s="53"/>
+      <c r="CO5" s="53"/>
+      <c r="CP5" s="54"/>
+      <c r="CQ5" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="CR5" s="48"/>
-      <c r="CS5" s="48"/>
-      <c r="CT5" s="48"/>
-      <c r="CU5" s="49"/>
+      <c r="CR5" s="50"/>
+      <c r="CS5" s="50"/>
+      <c r="CT5" s="50"/>
+      <c r="CU5" s="51"/>
     </row>
     <row r="6" spans="1:99" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -2132,132 +2132,132 @@
         <v>75</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="47" t="s">
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="50" t="s">
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="51"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="47" t="s">
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="Z6" s="48"/>
-      <c r="AA6" s="48"/>
-      <c r="AB6" s="48"/>
-      <c r="AC6" s="49"/>
-      <c r="AD6" s="50" t="s">
+      <c r="Z6" s="50"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="50"/>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="51"/>
-      <c r="AF6" s="51"/>
-      <c r="AG6" s="51"/>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="47" t="s">
+      <c r="AE6" s="53"/>
+      <c r="AF6" s="53"/>
+      <c r="AG6" s="53"/>
+      <c r="AH6" s="54"/>
+      <c r="AI6" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="48"/>
-      <c r="AL6" s="48"/>
-      <c r="AM6" s="49"/>
-      <c r="AN6" s="50" t="s">
+      <c r="AJ6" s="50"/>
+      <c r="AK6" s="50"/>
+      <c r="AL6" s="50"/>
+      <c r="AM6" s="51"/>
+      <c r="AN6" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" s="51"/>
-      <c r="AP6" s="51"/>
-      <c r="AQ6" s="51"/>
-      <c r="AR6" s="52"/>
-      <c r="AS6" s="47" t="s">
+      <c r="AO6" s="53"/>
+      <c r="AP6" s="53"/>
+      <c r="AQ6" s="53"/>
+      <c r="AR6" s="54"/>
+      <c r="AS6" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="AT6" s="48"/>
-      <c r="AU6" s="48"/>
-      <c r="AV6" s="48"/>
-      <c r="AW6" s="49"/>
-      <c r="AX6" s="50" t="s">
+      <c r="AT6" s="50"/>
+      <c r="AU6" s="50"/>
+      <c r="AV6" s="50"/>
+      <c r="AW6" s="51"/>
+      <c r="AX6" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="AY6" s="51"/>
-      <c r="AZ6" s="51"/>
-      <c r="BA6" s="51"/>
-      <c r="BB6" s="52"/>
-      <c r="BC6" s="47" t="s">
+      <c r="AY6" s="53"/>
+      <c r="AZ6" s="53"/>
+      <c r="BA6" s="53"/>
+      <c r="BB6" s="54"/>
+      <c r="BC6" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="BD6" s="48"/>
-      <c r="BE6" s="48"/>
-      <c r="BF6" s="48"/>
-      <c r="BG6" s="49"/>
-      <c r="BH6" s="50" t="s">
+      <c r="BD6" s="50"/>
+      <c r="BE6" s="50"/>
+      <c r="BF6" s="50"/>
+      <c r="BG6" s="51"/>
+      <c r="BH6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="BI6" s="51"/>
-      <c r="BJ6" s="51"/>
-      <c r="BK6" s="51"/>
-      <c r="BL6" s="52"/>
-      <c r="BM6" s="47" t="s">
+      <c r="BI6" s="53"/>
+      <c r="BJ6" s="53"/>
+      <c r="BK6" s="53"/>
+      <c r="BL6" s="54"/>
+      <c r="BM6" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="BN6" s="48"/>
-      <c r="BO6" s="48"/>
-      <c r="BP6" s="48"/>
-      <c r="BQ6" s="49"/>
-      <c r="BR6" s="50" t="s">
+      <c r="BN6" s="50"/>
+      <c r="BO6" s="50"/>
+      <c r="BP6" s="50"/>
+      <c r="BQ6" s="51"/>
+      <c r="BR6" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="BS6" s="51"/>
-      <c r="BT6" s="51"/>
-      <c r="BU6" s="51"/>
-      <c r="BV6" s="52"/>
-      <c r="BW6" s="47" t="s">
+      <c r="BS6" s="53"/>
+      <c r="BT6" s="53"/>
+      <c r="BU6" s="53"/>
+      <c r="BV6" s="54"/>
+      <c r="BW6" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="BX6" s="48"/>
-      <c r="BY6" s="48"/>
-      <c r="BZ6" s="48"/>
-      <c r="CA6" s="49"/>
-      <c r="CB6" s="50" t="s">
+      <c r="BX6" s="50"/>
+      <c r="BY6" s="50"/>
+      <c r="BZ6" s="50"/>
+      <c r="CA6" s="51"/>
+      <c r="CB6" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="CC6" s="51"/>
-      <c r="CD6" s="51"/>
-      <c r="CE6" s="51"/>
-      <c r="CF6" s="52"/>
-      <c r="CG6" s="47" t="s">
+      <c r="CC6" s="53"/>
+      <c r="CD6" s="53"/>
+      <c r="CE6" s="53"/>
+      <c r="CF6" s="54"/>
+      <c r="CG6" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="CH6" s="48"/>
-      <c r="CI6" s="48"/>
-      <c r="CJ6" s="48"/>
-      <c r="CK6" s="49"/>
-      <c r="CL6" s="50" t="s">
+      <c r="CH6" s="50"/>
+      <c r="CI6" s="50"/>
+      <c r="CJ6" s="50"/>
+      <c r="CK6" s="51"/>
+      <c r="CL6" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="CM6" s="51"/>
-      <c r="CN6" s="51"/>
-      <c r="CO6" s="51"/>
-      <c r="CP6" s="52"/>
-      <c r="CQ6" s="47" t="s">
+      <c r="CM6" s="53"/>
+      <c r="CN6" s="53"/>
+      <c r="CO6" s="53"/>
+      <c r="CP6" s="54"/>
+      <c r="CQ6" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="CR6" s="48"/>
-      <c r="CS6" s="48"/>
-      <c r="CT6" s="48"/>
-      <c r="CU6" s="49"/>
+      <c r="CR6" s="50"/>
+      <c r="CS6" s="50"/>
+      <c r="CT6" s="50"/>
+      <c r="CU6" s="51"/>
     </row>
     <row r="7" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -3162,114 +3162,124 @@
       <c r="AC20" s="31"/>
     </row>
     <row r="21" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="55"/>
-      <c r="T21" s="55"/>
-      <c r="U21" s="55"/>
-      <c r="V21" s="55"/>
-      <c r="W21" s="55"/>
-      <c r="X21" s="55"/>
-      <c r="Y21" s="55"/>
-      <c r="Z21" s="55"/>
-      <c r="AA21" s="55"/>
-      <c r="AB21" s="55"/>
-      <c r="AC21" s="55"/>
-      <c r="AD21" s="55"/>
-      <c r="AE21" s="55"/>
-      <c r="AF21" s="55"/>
-      <c r="AG21" s="55"/>
-      <c r="AH21" s="55"/>
-      <c r="AI21" s="55"/>
-      <c r="AJ21" s="55"/>
-      <c r="AK21" s="55"/>
-      <c r="AL21" s="55"/>
-      <c r="AM21" s="55"/>
-      <c r="AN21" s="55"/>
-      <c r="AO21" s="55"/>
-      <c r="AP21" s="55"/>
-      <c r="AQ21" s="55"/>
-      <c r="AR21" s="55"/>
-      <c r="AS21" s="55"/>
-      <c r="AT21" s="55"/>
-      <c r="AU21" s="55"/>
-      <c r="AV21" s="55"/>
-      <c r="AW21" s="55"/>
-      <c r="AX21" s="55"/>
-      <c r="AY21" s="55"/>
-      <c r="AZ21" s="55"/>
-      <c r="BA21" s="55"/>
-      <c r="BB21" s="55"/>
-      <c r="BC21" s="55"/>
-      <c r="BD21" s="55"/>
-      <c r="BE21" s="55"/>
-      <c r="BF21" s="55"/>
-      <c r="BG21" s="55"/>
-      <c r="BH21" s="55"/>
-      <c r="BI21" s="55"/>
-      <c r="BJ21" s="55"/>
-      <c r="BK21" s="55"/>
-      <c r="BL21" s="55"/>
-      <c r="BM21" s="55"/>
-      <c r="BN21" s="55"/>
-      <c r="BO21" s="55"/>
-      <c r="BP21" s="55"/>
-      <c r="BQ21" s="55"/>
-      <c r="BR21" s="55"/>
-      <c r="BS21" s="55"/>
-      <c r="BT21" s="55"/>
-      <c r="BU21" s="55"/>
-      <c r="BV21" s="55"/>
-      <c r="BW21" s="55"/>
-      <c r="BX21" s="55"/>
-      <c r="BY21" s="55"/>
-      <c r="BZ21" s="55"/>
-      <c r="CA21" s="55"/>
-      <c r="CB21" s="55"/>
-      <c r="CC21" s="55"/>
-      <c r="CD21" s="55"/>
-      <c r="CE21" s="55"/>
-      <c r="CF21" s="55"/>
-      <c r="CG21" s="55"/>
-      <c r="CH21" s="55"/>
-      <c r="CI21" s="55"/>
-      <c r="CJ21" s="55"/>
-      <c r="CK21" s="55"/>
-      <c r="CL21" s="55"/>
-      <c r="CM21" s="55"/>
-      <c r="CN21" s="55"/>
-      <c r="CO21" s="55"/>
-      <c r="CP21" s="55"/>
-      <c r="CQ21" s="55"/>
-      <c r="CR21" s="55"/>
-      <c r="CS21" s="55"/>
-      <c r="CT21" s="55"/>
-      <c r="CU21" s="55"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="47"/>
+      <c r="Z21" s="47"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="47"/>
+      <c r="AF21" s="47"/>
+      <c r="AG21" s="47"/>
+      <c r="AH21" s="47"/>
+      <c r="AI21" s="47"/>
+      <c r="AJ21" s="47"/>
+      <c r="AK21" s="47"/>
+      <c r="AL21" s="47"/>
+      <c r="AM21" s="47"/>
+      <c r="AN21" s="47"/>
+      <c r="AO21" s="47"/>
+      <c r="AP21" s="47"/>
+      <c r="AQ21" s="47"/>
+      <c r="AR21" s="47"/>
+      <c r="AS21" s="47"/>
+      <c r="AT21" s="47"/>
+      <c r="AU21" s="47"/>
+      <c r="AV21" s="47"/>
+      <c r="AW21" s="47"/>
+      <c r="AX21" s="47"/>
+      <c r="AY21" s="47"/>
+      <c r="AZ21" s="47"/>
+      <c r="BA21" s="47"/>
+      <c r="BB21" s="47"/>
+      <c r="BC21" s="47"/>
+      <c r="BD21" s="47"/>
+      <c r="BE21" s="47"/>
+      <c r="BF21" s="47"/>
+      <c r="BG21" s="47"/>
+      <c r="BH21" s="47"/>
+      <c r="BI21" s="47"/>
+      <c r="BJ21" s="47"/>
+      <c r="BK21" s="47"/>
+      <c r="BL21" s="47"/>
+      <c r="BM21" s="47"/>
+      <c r="BN21" s="47"/>
+      <c r="BO21" s="47"/>
+      <c r="BP21" s="47"/>
+      <c r="BQ21" s="47"/>
+      <c r="BR21" s="47"/>
+      <c r="BS21" s="47"/>
+      <c r="BT21" s="47"/>
+      <c r="BU21" s="47"/>
+      <c r="BV21" s="47"/>
+      <c r="BW21" s="47"/>
+      <c r="BX21" s="47"/>
+      <c r="BY21" s="47"/>
+      <c r="BZ21" s="47"/>
+      <c r="CA21" s="47"/>
+      <c r="CB21" s="47"/>
+      <c r="CC21" s="47"/>
+      <c r="CD21" s="47"/>
+      <c r="CE21" s="47"/>
+      <c r="CF21" s="47"/>
+      <c r="CG21" s="47"/>
+      <c r="CH21" s="47"/>
+      <c r="CI21" s="47"/>
+      <c r="CJ21" s="47"/>
+      <c r="CK21" s="47"/>
+      <c r="CL21" s="47"/>
+      <c r="CM21" s="47"/>
+      <c r="CN21" s="47"/>
+      <c r="CO21" s="47"/>
+      <c r="CP21" s="47"/>
+      <c r="CQ21" s="47"/>
+      <c r="CR21" s="47"/>
+      <c r="CS21" s="47"/>
+      <c r="CT21" s="47"/>
+      <c r="CU21" s="47"/>
     </row>
     <row r="22" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
+      <c r="C22" s="29">
+        <v>25</v>
+      </c>
+      <c r="D22" s="29">
+        <v>26</v>
+      </c>
+      <c r="E22" s="29">
+        <v>25</v>
+      </c>
+      <c r="F22" s="29">
+        <v>26</v>
+      </c>
+      <c r="G22" s="30">
+        <v>0</v>
+      </c>
       <c r="H22" s="24"/>
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
@@ -3544,104 +3554,104 @@
       <c r="CU25" s="35"/>
     </row>
     <row r="26" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="55"/>
-      <c r="S26" s="55"/>
-      <c r="T26" s="55"/>
-      <c r="U26" s="55"/>
-      <c r="V26" s="55"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="55"/>
-      <c r="Y26" s="55"/>
-      <c r="Z26" s="55"/>
-      <c r="AA26" s="55"/>
-      <c r="AB26" s="55"/>
-      <c r="AC26" s="55"/>
-      <c r="AD26" s="55"/>
-      <c r="AE26" s="55"/>
-      <c r="AF26" s="55"/>
-      <c r="AG26" s="55"/>
-      <c r="AH26" s="55"/>
-      <c r="AI26" s="55"/>
-      <c r="AJ26" s="55"/>
-      <c r="AK26" s="55"/>
-      <c r="AL26" s="55"/>
-      <c r="AM26" s="55"/>
-      <c r="AN26" s="55"/>
-      <c r="AO26" s="55"/>
-      <c r="AP26" s="55"/>
-      <c r="AQ26" s="55"/>
-      <c r="AR26" s="55"/>
-      <c r="AS26" s="55"/>
-      <c r="AT26" s="55"/>
-      <c r="AU26" s="55"/>
-      <c r="AV26" s="55"/>
-      <c r="AW26" s="55"/>
-      <c r="AX26" s="55"/>
-      <c r="AY26" s="55"/>
-      <c r="AZ26" s="55"/>
-      <c r="BA26" s="55"/>
-      <c r="BB26" s="55"/>
-      <c r="BC26" s="55"/>
-      <c r="BD26" s="55"/>
-      <c r="BE26" s="55"/>
-      <c r="BF26" s="55"/>
-      <c r="BG26" s="55"/>
-      <c r="BH26" s="55"/>
-      <c r="BI26" s="55"/>
-      <c r="BJ26" s="55"/>
-      <c r="BK26" s="55"/>
-      <c r="BL26" s="55"/>
-      <c r="BM26" s="55"/>
-      <c r="BN26" s="55"/>
-      <c r="BO26" s="55"/>
-      <c r="BP26" s="55"/>
-      <c r="BQ26" s="55"/>
-      <c r="BR26" s="55"/>
-      <c r="BS26" s="55"/>
-      <c r="BT26" s="55"/>
-      <c r="BU26" s="55"/>
-      <c r="BV26" s="55"/>
-      <c r="BW26" s="55"/>
-      <c r="BX26" s="55"/>
-      <c r="BY26" s="55"/>
-      <c r="BZ26" s="55"/>
-      <c r="CA26" s="55"/>
-      <c r="CB26" s="55"/>
-      <c r="CC26" s="55"/>
-      <c r="CD26" s="55"/>
-      <c r="CE26" s="55"/>
-      <c r="CF26" s="55"/>
-      <c r="CG26" s="55"/>
-      <c r="CH26" s="55"/>
-      <c r="CI26" s="55"/>
-      <c r="CJ26" s="55"/>
-      <c r="CK26" s="55"/>
-      <c r="CL26" s="55"/>
-      <c r="CM26" s="55"/>
-      <c r="CN26" s="55"/>
-      <c r="CO26" s="55"/>
-      <c r="CP26" s="55"/>
-      <c r="CQ26" s="55"/>
-      <c r="CR26" s="55"/>
-      <c r="CS26" s="55"/>
-      <c r="CT26" s="55"/>
-      <c r="CU26" s="55"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="47"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="47"/>
+      <c r="AE26" s="47"/>
+      <c r="AF26" s="47"/>
+      <c r="AG26" s="47"/>
+      <c r="AH26" s="47"/>
+      <c r="AI26" s="47"/>
+      <c r="AJ26" s="47"/>
+      <c r="AK26" s="47"/>
+      <c r="AL26" s="47"/>
+      <c r="AM26" s="47"/>
+      <c r="AN26" s="47"/>
+      <c r="AO26" s="47"/>
+      <c r="AP26" s="47"/>
+      <c r="AQ26" s="47"/>
+      <c r="AR26" s="47"/>
+      <c r="AS26" s="47"/>
+      <c r="AT26" s="47"/>
+      <c r="AU26" s="47"/>
+      <c r="AV26" s="47"/>
+      <c r="AW26" s="47"/>
+      <c r="AX26" s="47"/>
+      <c r="AY26" s="47"/>
+      <c r="AZ26" s="47"/>
+      <c r="BA26" s="47"/>
+      <c r="BB26" s="47"/>
+      <c r="BC26" s="47"/>
+      <c r="BD26" s="47"/>
+      <c r="BE26" s="47"/>
+      <c r="BF26" s="47"/>
+      <c r="BG26" s="47"/>
+      <c r="BH26" s="47"/>
+      <c r="BI26" s="47"/>
+      <c r="BJ26" s="47"/>
+      <c r="BK26" s="47"/>
+      <c r="BL26" s="47"/>
+      <c r="BM26" s="47"/>
+      <c r="BN26" s="47"/>
+      <c r="BO26" s="47"/>
+      <c r="BP26" s="47"/>
+      <c r="BQ26" s="47"/>
+      <c r="BR26" s="47"/>
+      <c r="BS26" s="47"/>
+      <c r="BT26" s="47"/>
+      <c r="BU26" s="47"/>
+      <c r="BV26" s="47"/>
+      <c r="BW26" s="47"/>
+      <c r="BX26" s="47"/>
+      <c r="BY26" s="47"/>
+      <c r="BZ26" s="47"/>
+      <c r="CA26" s="47"/>
+      <c r="CB26" s="47"/>
+      <c r="CC26" s="47"/>
+      <c r="CD26" s="47"/>
+      <c r="CE26" s="47"/>
+      <c r="CF26" s="47"/>
+      <c r="CG26" s="47"/>
+      <c r="CH26" s="47"/>
+      <c r="CI26" s="47"/>
+      <c r="CJ26" s="47"/>
+      <c r="CK26" s="47"/>
+      <c r="CL26" s="47"/>
+      <c r="CM26" s="47"/>
+      <c r="CN26" s="47"/>
+      <c r="CO26" s="47"/>
+      <c r="CP26" s="47"/>
+      <c r="CQ26" s="47"/>
+      <c r="CR26" s="47"/>
+      <c r="CS26" s="47"/>
+      <c r="CT26" s="47"/>
+      <c r="CU26" s="47"/>
     </row>
     <row r="27" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
@@ -3736,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -3811,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
@@ -3942,105 +3952,105 @@
       <c r="CU30" s="35"/>
     </row>
     <row r="31" spans="1:99" s="45" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="56"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
-      <c r="X31" s="56"/>
-      <c r="Y31" s="56"/>
-      <c r="Z31" s="56"/>
-      <c r="AA31" s="56"/>
-      <c r="AB31" s="56"/>
-      <c r="AC31" s="56"/>
-      <c r="AD31" s="56"/>
-      <c r="AE31" s="56"/>
-      <c r="AF31" s="56"/>
-      <c r="AG31" s="56"/>
-      <c r="AH31" s="56"/>
-      <c r="AI31" s="56"/>
-      <c r="AJ31" s="56"/>
-      <c r="AK31" s="56"/>
-      <c r="AL31" s="56"/>
-      <c r="AM31" s="56"/>
-      <c r="AN31" s="56"/>
-      <c r="AO31" s="56"/>
-      <c r="AP31" s="56"/>
-      <c r="AQ31" s="56"/>
-      <c r="AR31" s="56"/>
-      <c r="AS31" s="56"/>
-      <c r="AT31" s="56"/>
-      <c r="AU31" s="56"/>
-      <c r="AV31" s="56"/>
-      <c r="AW31" s="56"/>
-      <c r="AX31" s="56"/>
-      <c r="AY31" s="56"/>
-      <c r="AZ31" s="56"/>
-      <c r="BA31" s="56"/>
-      <c r="BB31" s="56"/>
-      <c r="BC31" s="56"/>
-      <c r="BD31" s="56"/>
-      <c r="BE31" s="56"/>
-      <c r="BF31" s="56"/>
-      <c r="BG31" s="56"/>
-      <c r="BH31" s="56"/>
-      <c r="BI31" s="56"/>
-      <c r="BJ31" s="56"/>
-      <c r="BK31" s="56"/>
-      <c r="BL31" s="56"/>
-      <c r="BM31" s="56"/>
-      <c r="BN31" s="56"/>
-      <c r="BO31" s="56"/>
-      <c r="BP31" s="56"/>
-      <c r="BQ31" s="56"/>
-      <c r="BR31" s="56"/>
-      <c r="BS31" s="56"/>
-      <c r="BT31" s="56"/>
-      <c r="BU31" s="56"/>
-      <c r="BV31" s="56"/>
-      <c r="BW31" s="56"/>
-      <c r="BX31" s="56"/>
-      <c r="BY31" s="56"/>
-      <c r="BZ31" s="56"/>
-      <c r="CA31" s="56"/>
-      <c r="CB31" s="56"/>
-      <c r="CC31" s="56"/>
-      <c r="CD31" s="56"/>
-      <c r="CE31" s="56"/>
-      <c r="CF31" s="56"/>
-      <c r="CG31" s="56"/>
-      <c r="CH31" s="56"/>
-      <c r="CI31" s="56"/>
-      <c r="CJ31" s="56"/>
-      <c r="CK31" s="56"/>
-      <c r="CL31" s="56"/>
-      <c r="CM31" s="56"/>
-      <c r="CN31" s="56"/>
-      <c r="CO31" s="56"/>
-      <c r="CP31" s="56"/>
-      <c r="CQ31" s="56"/>
-      <c r="CR31" s="56"/>
-      <c r="CS31" s="56"/>
-      <c r="CT31" s="56"/>
-      <c r="CU31" s="56"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="48"/>
+      <c r="V31" s="48"/>
+      <c r="W31" s="48"/>
+      <c r="X31" s="48"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="48"/>
+      <c r="AA31" s="48"/>
+      <c r="AB31" s="48"/>
+      <c r="AC31" s="48"/>
+      <c r="AD31" s="48"/>
+      <c r="AE31" s="48"/>
+      <c r="AF31" s="48"/>
+      <c r="AG31" s="48"/>
+      <c r="AH31" s="48"/>
+      <c r="AI31" s="48"/>
+      <c r="AJ31" s="48"/>
+      <c r="AK31" s="48"/>
+      <c r="AL31" s="48"/>
+      <c r="AM31" s="48"/>
+      <c r="AN31" s="48"/>
+      <c r="AO31" s="48"/>
+      <c r="AP31" s="48"/>
+      <c r="AQ31" s="48"/>
+      <c r="AR31" s="48"/>
+      <c r="AS31" s="48"/>
+      <c r="AT31" s="48"/>
+      <c r="AU31" s="48"/>
+      <c r="AV31" s="48"/>
+      <c r="AW31" s="48"/>
+      <c r="AX31" s="48"/>
+      <c r="AY31" s="48"/>
+      <c r="AZ31" s="48"/>
+      <c r="BA31" s="48"/>
+      <c r="BB31" s="48"/>
+      <c r="BC31" s="48"/>
+      <c r="BD31" s="48"/>
+      <c r="BE31" s="48"/>
+      <c r="BF31" s="48"/>
+      <c r="BG31" s="48"/>
+      <c r="BH31" s="48"/>
+      <c r="BI31" s="48"/>
+      <c r="BJ31" s="48"/>
+      <c r="BK31" s="48"/>
+      <c r="BL31" s="48"/>
+      <c r="BM31" s="48"/>
+      <c r="BN31" s="48"/>
+      <c r="BO31" s="48"/>
+      <c r="BP31" s="48"/>
+      <c r="BQ31" s="48"/>
+      <c r="BR31" s="48"/>
+      <c r="BS31" s="48"/>
+      <c r="BT31" s="48"/>
+      <c r="BU31" s="48"/>
+      <c r="BV31" s="48"/>
+      <c r="BW31" s="48"/>
+      <c r="BX31" s="48"/>
+      <c r="BY31" s="48"/>
+      <c r="BZ31" s="48"/>
+      <c r="CA31" s="48"/>
+      <c r="CB31" s="48"/>
+      <c r="CC31" s="48"/>
+      <c r="CD31" s="48"/>
+      <c r="CE31" s="48"/>
+      <c r="CF31" s="48"/>
+      <c r="CG31" s="48"/>
+      <c r="CH31" s="48"/>
+      <c r="CI31" s="48"/>
+      <c r="CJ31" s="48"/>
+      <c r="CK31" s="48"/>
+      <c r="CL31" s="48"/>
+      <c r="CM31" s="48"/>
+      <c r="CN31" s="48"/>
+      <c r="CO31" s="48"/>
+      <c r="CP31" s="48"/>
+      <c r="CQ31" s="48"/>
+      <c r="CR31" s="48"/>
+      <c r="CS31" s="48"/>
+      <c r="CT31" s="48"/>
+      <c r="CU31" s="48"/>
     </row>
     <row r="32" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
@@ -4117,7 +4127,7 @@
     </row>
     <row r="33" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="29">
         <v>36</v>
@@ -4192,7 +4202,7 @@
     </row>
     <row r="34" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="29">
         <v>36</v>
@@ -4267,7 +4277,7 @@
     </row>
     <row r="35" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" s="29">
         <v>41</v>
@@ -4492,7 +4502,7 @@
     </row>
     <row r="38" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C38" s="29">
         <v>36</v>
@@ -4567,7 +4577,7 @@
     </row>
     <row r="39" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C39" s="29">
         <v>36</v>
@@ -4642,7 +4652,7 @@
     </row>
     <row r="40" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C40" s="29">
         <v>40</v>
@@ -4966,7 +4976,7 @@
     </row>
     <row r="44" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" s="29">
         <v>56</v>
@@ -5041,7 +5051,7 @@
     </row>
     <row r="45" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45" s="29">
         <v>59</v>
@@ -5209,7 +5219,7 @@
         <v>0</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I47" s="31"/>
       <c r="J47" s="31"/>
@@ -5266,7 +5276,7 @@
     </row>
     <row r="48" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" s="29">
         <v>68</v>
@@ -5512,7 +5522,7 @@
     </row>
     <row r="51" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="38" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="C51" s="29">
         <v>71</v>
@@ -5759,7 +5769,7 @@
     </row>
     <row r="54" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C54" s="29">
         <v>81</v>
@@ -5832,7 +5842,7 @@
     </row>
     <row r="55" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C55" s="29">
         <v>84</v>
@@ -5905,7 +5915,7 @@
     </row>
     <row r="56" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C56" s="29">
         <v>81</v>
@@ -6094,7 +6104,7 @@
         <v>80</v>
       </c>
       <c r="G58" s="30">
-        <v>0.03</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H58" s="24"/>
       <c r="I58" s="31"/>
@@ -6152,7 +6162,7 @@
     </row>
     <row r="59" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C59" s="41">
         <v>11</v>
@@ -6227,7 +6237,7 @@
     </row>
     <row r="60" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C60" s="41">
         <v>13</v>
@@ -6242,7 +6252,7 @@
         <v>9</v>
       </c>
       <c r="G60" s="30">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="H60" s="24"/>
       <c r="I60" s="31"/>
@@ -6300,7 +6310,7 @@
     </row>
     <row r="61" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C61" s="41">
         <v>13</v>
@@ -6375,7 +6385,7 @@
     </row>
     <row r="62" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C62" s="41">
         <v>13</v>
@@ -6390,7 +6400,7 @@
         <v>3</v>
       </c>
       <c r="G62" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" s="24" t="s">
         <v>81</v>
@@ -6448,9 +6458,9 @@
       <c r="CT62" s="35"/>
       <c r="CU62" s="35"/>
     </row>
-    <row r="63" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:99" s="28" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C63" s="41">
         <v>13</v>
@@ -6468,7 +6478,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I63" s="31"/>
       <c r="J63" s="31"/>
@@ -6525,7 +6535,7 @@
     </row>
     <row r="64" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C64" s="41">
         <v>16</v>
@@ -6540,7 +6550,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" s="24"/>
       <c r="I64" s="31"/>
@@ -6598,7 +6608,7 @@
     </row>
     <row r="65" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C65" s="41">
         <v>17</v>
@@ -6673,7 +6683,7 @@
     </row>
     <row r="66" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C66" s="41">
         <v>17</v>
@@ -6691,7 +6701,7 @@
         <v>0</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I66" s="31"/>
       <c r="J66" s="31"/>
@@ -6748,7 +6758,7 @@
     </row>
     <row r="67" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C67" s="41">
         <v>17</v>
@@ -6763,7 +6773,7 @@
         <v>3</v>
       </c>
       <c r="G67" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" s="24" t="s">
         <v>77</v>
@@ -6823,7 +6833,7 @@
     </row>
     <row r="68" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C68" s="41">
         <v>19</v>
@@ -6896,7 +6906,7 @@
     </row>
     <row r="69" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C69" s="41">
         <v>20</v>
@@ -6969,7 +6979,7 @@
     </row>
     <row r="70" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C70" s="41">
         <v>22</v>
@@ -7042,7 +7052,7 @@
     </row>
     <row r="71" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C71" s="41">
         <v>22</v>
@@ -7115,7 +7125,7 @@
     </row>
     <row r="72" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C72" s="41">
         <v>36</v>
@@ -7188,7 +7198,7 @@
     </row>
     <row r="73" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C73" s="41">
         <v>71</v>
@@ -7261,7 +7271,7 @@
     </row>
     <row r="74" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C74" s="41">
         <v>78</v>
@@ -7334,7 +7344,7 @@
     </row>
     <row r="75" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C75" s="41">
         <v>82</v>
@@ -7407,7 +7417,7 @@
     </row>
     <row r="76" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C76" s="41">
         <v>86</v>
@@ -7687,21 +7697,22 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A13:CU13"/>
-    <mergeCell ref="B21:CU21"/>
-    <mergeCell ref="B26:CU26"/>
-    <mergeCell ref="A31:CU31"/>
-    <mergeCell ref="A42:CU42"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="AD5:AH5"/>
-    <mergeCell ref="AD6:AH6"/>
-    <mergeCell ref="B2:G4"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="O6:S6"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A57:CU57"/>
+    <mergeCell ref="B49:CU49"/>
+    <mergeCell ref="A52:CU52"/>
+    <mergeCell ref="CQ5:CU5"/>
+    <mergeCell ref="CQ6:CU6"/>
+    <mergeCell ref="CL5:CP5"/>
+    <mergeCell ref="CL6:CP6"/>
+    <mergeCell ref="AX5:BB5"/>
+    <mergeCell ref="AX6:BB6"/>
+    <mergeCell ref="AI5:AM5"/>
+    <mergeCell ref="AI6:AM6"/>
+    <mergeCell ref="AN5:AR5"/>
+    <mergeCell ref="AN6:AR6"/>
+    <mergeCell ref="AS5:AW5"/>
+    <mergeCell ref="AS6:AW6"/>
+    <mergeCell ref="Y5:AC5"/>
     <mergeCell ref="BE2:BW2"/>
     <mergeCell ref="BE3:BW3"/>
     <mergeCell ref="CB5:CF5"/>
@@ -7718,22 +7729,21 @@
     <mergeCell ref="BC6:BG6"/>
     <mergeCell ref="BH5:BL5"/>
     <mergeCell ref="BH6:BL6"/>
-    <mergeCell ref="A57:CU57"/>
-    <mergeCell ref="B49:CU49"/>
-    <mergeCell ref="A52:CU52"/>
-    <mergeCell ref="CQ5:CU5"/>
-    <mergeCell ref="CQ6:CU6"/>
-    <mergeCell ref="CL5:CP5"/>
-    <mergeCell ref="CL6:CP6"/>
-    <mergeCell ref="AX5:BB5"/>
-    <mergeCell ref="AX6:BB6"/>
-    <mergeCell ref="AI5:AM5"/>
-    <mergeCell ref="AI6:AM6"/>
-    <mergeCell ref="AN5:AR5"/>
-    <mergeCell ref="AN6:AR6"/>
-    <mergeCell ref="AS5:AW5"/>
-    <mergeCell ref="AS6:AW6"/>
-    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="AD6:AH6"/>
+    <mergeCell ref="B2:G4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="O6:S6"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A13:CU13"/>
+    <mergeCell ref="B21:CU21"/>
+    <mergeCell ref="B26:CU26"/>
+    <mergeCell ref="A31:CU31"/>
+    <mergeCell ref="A42:CU42"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J53:CU56 J50:CU51 J32:CU41 J43:CU48 J58:CU59 J75:CU75">
     <cfRule type="expression" dxfId="25" priority="84">

</xml_diff>

<commit_message>
Fundamentação teórica está ficando LIIIIINDA....
</commit_message>
<xml_diff>
--- a/LaTeX Project/Documentos/Gantt.xlsx
+++ b/LaTeX Project/Documentos/Gantt.xlsx
@@ -1810,8 +1810,8 @@
   </sheetPr>
   <dimension ref="A2:CU84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AV68" sqref="AV68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AX24" sqref="AX24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -6104,7 +6104,7 @@
         <v>80</v>
       </c>
       <c r="G58" s="30">
-        <v>0.14000000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="H58" s="24"/>
       <c r="I58" s="31"/>
@@ -6252,7 +6252,7 @@
         <v>9</v>
       </c>
       <c r="G60" s="30">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="H60" s="24"/>
       <c r="I60" s="31"/>
@@ -6475,7 +6475,7 @@
         <v>3</v>
       </c>
       <c r="G63" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63" s="24" t="s">
         <v>122</v>
@@ -6623,7 +6623,7 @@
         <v>3</v>
       </c>
       <c r="G65" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="24" t="s">
         <v>81</v>
@@ -6698,7 +6698,7 @@
         <v>3</v>
       </c>
       <c r="G66" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" s="24" t="s">
         <v>122</v>
@@ -6994,7 +6994,7 @@
         <v>14</v>
       </c>
       <c r="G70" s="30">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H70" s="24"/>
       <c r="I70" s="31"/>
@@ -7058,16 +7058,16 @@
         <v>22</v>
       </c>
       <c r="D71" s="41">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E71" s="41">
         <v>22</v>
       </c>
       <c r="F71" s="41">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G71" s="30">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H71" s="24"/>
       <c r="I71" s="31"/>

</xml_diff>

<commit_message>
continuação da belezinha da FUNDAMENTAÇÃO TEÓRICA
</commit_message>
<xml_diff>
--- a/LaTeX Project/Documentos/Gantt.xlsx
+++ b/LaTeX Project/Documentos/Gantt.xlsx
@@ -1016,6 +1016,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1034,16 +1040,10 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1810,8 +1810,8 @@
   </sheetPr>
   <dimension ref="A2:CU84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AX24" sqref="AX24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:CU26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1836,47 +1836,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="24" t="s">
         <v>78</v>
       </c>
       <c r="I2" s="16"/>
-      <c r="BE2" s="53" t="s">
+      <c r="BE2" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" s="53"/>
-      <c r="BG2" s="53"/>
-      <c r="BH2" s="53"/>
-      <c r="BI2" s="53"/>
-      <c r="BJ2" s="53"/>
-      <c r="BK2" s="53"/>
-      <c r="BL2" s="53"/>
-      <c r="BM2" s="53"/>
-      <c r="BN2" s="53"/>
-      <c r="BO2" s="53"/>
-      <c r="BP2" s="53"/>
-      <c r="BQ2" s="53"/>
-      <c r="BR2" s="53"/>
-      <c r="BS2" s="53"/>
-      <c r="BT2" s="53"/>
-      <c r="BU2" s="53"/>
-      <c r="BV2" s="53"/>
-      <c r="BW2" s="53"/>
+      <c r="BF2" s="56"/>
+      <c r="BG2" s="56"/>
+      <c r="BH2" s="56"/>
+      <c r="BI2" s="56"/>
+      <c r="BJ2" s="56"/>
+      <c r="BK2" s="56"/>
+      <c r="BL2" s="56"/>
+      <c r="BM2" s="56"/>
+      <c r="BN2" s="56"/>
+      <c r="BO2" s="56"/>
+      <c r="BP2" s="56"/>
+      <c r="BQ2" s="56"/>
+      <c r="BR2" s="56"/>
+      <c r="BS2" s="56"/>
+      <c r="BT2" s="56"/>
+      <c r="BU2" s="56"/>
+      <c r="BV2" s="56"/>
+      <c r="BW2" s="56"/>
     </row>
     <row r="3" spans="1:99" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="24" t="s">
         <v>79</v>
       </c>
@@ -1925,35 +1925,35 @@
       <c r="AQ3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="BE3" s="53" t="s">
+      <c r="BE3" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="BF3" s="53"/>
-      <c r="BG3" s="53"/>
-      <c r="BH3" s="53"/>
-      <c r="BI3" s="53"/>
-      <c r="BJ3" s="53"/>
-      <c r="BK3" s="53"/>
-      <c r="BL3" s="53"/>
-      <c r="BM3" s="53"/>
-      <c r="BN3" s="53"/>
-      <c r="BO3" s="53"/>
-      <c r="BP3" s="53"/>
-      <c r="BQ3" s="53"/>
-      <c r="BR3" s="53"/>
-      <c r="BS3" s="53"/>
-      <c r="BT3" s="53"/>
-      <c r="BU3" s="53"/>
-      <c r="BV3" s="53"/>
-      <c r="BW3" s="53"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
+      <c r="BI3" s="56"/>
+      <c r="BJ3" s="56"/>
+      <c r="BK3" s="56"/>
+      <c r="BL3" s="56"/>
+      <c r="BM3" s="56"/>
+      <c r="BN3" s="56"/>
+      <c r="BO3" s="56"/>
+      <c r="BP3" s="56"/>
+      <c r="BQ3" s="56"/>
+      <c r="BR3" s="56"/>
+      <c r="BS3" s="56"/>
+      <c r="BT3" s="56"/>
+      <c r="BU3" s="56"/>
+      <c r="BV3" s="56"/>
+      <c r="BW3" s="56"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="24" t="s">
         <v>80</v>
       </c>
@@ -1984,132 +1984,132 @@
       <c r="AY4" s="19"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="47" t="s">
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="50" t="s">
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="47" t="s">
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="48"/>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="50" t="s">
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="50"/>
+      <c r="AB5" s="50"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="51"/>
-      <c r="AF5" s="51"/>
-      <c r="AG5" s="51"/>
-      <c r="AH5" s="52"/>
-      <c r="AI5" s="47" t="s">
+      <c r="AE5" s="53"/>
+      <c r="AF5" s="53"/>
+      <c r="AG5" s="53"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="48"/>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="49"/>
-      <c r="AN5" s="50" t="s">
+      <c r="AJ5" s="50"/>
+      <c r="AK5" s="50"/>
+      <c r="AL5" s="50"/>
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="51"/>
-      <c r="AP5" s="51"/>
-      <c r="AQ5" s="51"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="47" t="s">
+      <c r="AO5" s="53"/>
+      <c r="AP5" s="53"/>
+      <c r="AQ5" s="53"/>
+      <c r="AR5" s="54"/>
+      <c r="AS5" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="AT5" s="48"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="48"/>
-      <c r="AW5" s="49"/>
-      <c r="AX5" s="50" t="s">
+      <c r="AT5" s="50"/>
+      <c r="AU5" s="50"/>
+      <c r="AV5" s="50"/>
+      <c r="AW5" s="51"/>
+      <c r="AX5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="AY5" s="51"/>
-      <c r="AZ5" s="51"/>
-      <c r="BA5" s="51"/>
-      <c r="BB5" s="52"/>
-      <c r="BC5" s="47" t="s">
+      <c r="AY5" s="53"/>
+      <c r="AZ5" s="53"/>
+      <c r="BA5" s="53"/>
+      <c r="BB5" s="54"/>
+      <c r="BC5" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="BD5" s="48"/>
-      <c r="BE5" s="48"/>
-      <c r="BF5" s="48"/>
-      <c r="BG5" s="49"/>
-      <c r="BH5" s="50" t="s">
+      <c r="BD5" s="50"/>
+      <c r="BE5" s="50"/>
+      <c r="BF5" s="50"/>
+      <c r="BG5" s="51"/>
+      <c r="BH5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="BI5" s="51"/>
-      <c r="BJ5" s="51"/>
-      <c r="BK5" s="51"/>
-      <c r="BL5" s="52"/>
-      <c r="BM5" s="47" t="s">
+      <c r="BI5" s="53"/>
+      <c r="BJ5" s="53"/>
+      <c r="BK5" s="53"/>
+      <c r="BL5" s="54"/>
+      <c r="BM5" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="BN5" s="48"/>
-      <c r="BO5" s="48"/>
-      <c r="BP5" s="48"/>
-      <c r="BQ5" s="49"/>
-      <c r="BR5" s="50" t="s">
+      <c r="BN5" s="50"/>
+      <c r="BO5" s="50"/>
+      <c r="BP5" s="50"/>
+      <c r="BQ5" s="51"/>
+      <c r="BR5" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="BS5" s="51"/>
-      <c r="BT5" s="51"/>
-      <c r="BU5" s="51"/>
-      <c r="BV5" s="52"/>
-      <c r="BW5" s="47" t="s">
+      <c r="BS5" s="53"/>
+      <c r="BT5" s="53"/>
+      <c r="BU5" s="53"/>
+      <c r="BV5" s="54"/>
+      <c r="BW5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="BX5" s="48"/>
-      <c r="BY5" s="48"/>
-      <c r="BZ5" s="48"/>
-      <c r="CA5" s="49"/>
-      <c r="CB5" s="50" t="s">
+      <c r="BX5" s="50"/>
+      <c r="BY5" s="50"/>
+      <c r="BZ5" s="50"/>
+      <c r="CA5" s="51"/>
+      <c r="CB5" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="CC5" s="51"/>
-      <c r="CD5" s="51"/>
-      <c r="CE5" s="51"/>
-      <c r="CF5" s="52"/>
-      <c r="CG5" s="47" t="s">
+      <c r="CC5" s="53"/>
+      <c r="CD5" s="53"/>
+      <c r="CE5" s="53"/>
+      <c r="CF5" s="54"/>
+      <c r="CG5" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="CH5" s="48"/>
-      <c r="CI5" s="48"/>
-      <c r="CJ5" s="48"/>
-      <c r="CK5" s="49"/>
-      <c r="CL5" s="50" t="s">
+      <c r="CH5" s="50"/>
+      <c r="CI5" s="50"/>
+      <c r="CJ5" s="50"/>
+      <c r="CK5" s="51"/>
+      <c r="CL5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="CM5" s="51"/>
-      <c r="CN5" s="51"/>
-      <c r="CO5" s="51"/>
-      <c r="CP5" s="52"/>
-      <c r="CQ5" s="47" t="s">
+      <c r="CM5" s="53"/>
+      <c r="CN5" s="53"/>
+      <c r="CO5" s="53"/>
+      <c r="CP5" s="54"/>
+      <c r="CQ5" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="CR5" s="48"/>
-      <c r="CS5" s="48"/>
-      <c r="CT5" s="48"/>
-      <c r="CU5" s="49"/>
+      <c r="CR5" s="50"/>
+      <c r="CS5" s="50"/>
+      <c r="CT5" s="50"/>
+      <c r="CU5" s="51"/>
     </row>
     <row r="6" spans="1:99" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -2132,132 +2132,132 @@
         <v>75</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="47" t="s">
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="50" t="s">
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="51"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="47" t="s">
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="Z6" s="48"/>
-      <c r="AA6" s="48"/>
-      <c r="AB6" s="48"/>
-      <c r="AC6" s="49"/>
-      <c r="AD6" s="50" t="s">
+      <c r="Z6" s="50"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="50"/>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="51"/>
-      <c r="AF6" s="51"/>
-      <c r="AG6" s="51"/>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="47" t="s">
+      <c r="AE6" s="53"/>
+      <c r="AF6" s="53"/>
+      <c r="AG6" s="53"/>
+      <c r="AH6" s="54"/>
+      <c r="AI6" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="48"/>
-      <c r="AL6" s="48"/>
-      <c r="AM6" s="49"/>
-      <c r="AN6" s="50" t="s">
+      <c r="AJ6" s="50"/>
+      <c r="AK6" s="50"/>
+      <c r="AL6" s="50"/>
+      <c r="AM6" s="51"/>
+      <c r="AN6" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" s="51"/>
-      <c r="AP6" s="51"/>
-      <c r="AQ6" s="51"/>
-      <c r="AR6" s="52"/>
-      <c r="AS6" s="47" t="s">
+      <c r="AO6" s="53"/>
+      <c r="AP6" s="53"/>
+      <c r="AQ6" s="53"/>
+      <c r="AR6" s="54"/>
+      <c r="AS6" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="AT6" s="48"/>
-      <c r="AU6" s="48"/>
-      <c r="AV6" s="48"/>
-      <c r="AW6" s="49"/>
-      <c r="AX6" s="50" t="s">
+      <c r="AT6" s="50"/>
+      <c r="AU6" s="50"/>
+      <c r="AV6" s="50"/>
+      <c r="AW6" s="51"/>
+      <c r="AX6" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="AY6" s="51"/>
-      <c r="AZ6" s="51"/>
-      <c r="BA6" s="51"/>
-      <c r="BB6" s="52"/>
-      <c r="BC6" s="47" t="s">
+      <c r="AY6" s="53"/>
+      <c r="AZ6" s="53"/>
+      <c r="BA6" s="53"/>
+      <c r="BB6" s="54"/>
+      <c r="BC6" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="BD6" s="48"/>
-      <c r="BE6" s="48"/>
-      <c r="BF6" s="48"/>
-      <c r="BG6" s="49"/>
-      <c r="BH6" s="50" t="s">
+      <c r="BD6" s="50"/>
+      <c r="BE6" s="50"/>
+      <c r="BF6" s="50"/>
+      <c r="BG6" s="51"/>
+      <c r="BH6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="BI6" s="51"/>
-      <c r="BJ6" s="51"/>
-      <c r="BK6" s="51"/>
-      <c r="BL6" s="52"/>
-      <c r="BM6" s="47" t="s">
+      <c r="BI6" s="53"/>
+      <c r="BJ6" s="53"/>
+      <c r="BK6" s="53"/>
+      <c r="BL6" s="54"/>
+      <c r="BM6" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="BN6" s="48"/>
-      <c r="BO6" s="48"/>
-      <c r="BP6" s="48"/>
-      <c r="BQ6" s="49"/>
-      <c r="BR6" s="50" t="s">
+      <c r="BN6" s="50"/>
+      <c r="BO6" s="50"/>
+      <c r="BP6" s="50"/>
+      <c r="BQ6" s="51"/>
+      <c r="BR6" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="BS6" s="51"/>
-      <c r="BT6" s="51"/>
-      <c r="BU6" s="51"/>
-      <c r="BV6" s="52"/>
-      <c r="BW6" s="47" t="s">
+      <c r="BS6" s="53"/>
+      <c r="BT6" s="53"/>
+      <c r="BU6" s="53"/>
+      <c r="BV6" s="54"/>
+      <c r="BW6" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="BX6" s="48"/>
-      <c r="BY6" s="48"/>
-      <c r="BZ6" s="48"/>
-      <c r="CA6" s="49"/>
-      <c r="CB6" s="50" t="s">
+      <c r="BX6" s="50"/>
+      <c r="BY6" s="50"/>
+      <c r="BZ6" s="50"/>
+      <c r="CA6" s="51"/>
+      <c r="CB6" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="CC6" s="51"/>
-      <c r="CD6" s="51"/>
-      <c r="CE6" s="51"/>
-      <c r="CF6" s="52"/>
-      <c r="CG6" s="47" t="s">
+      <c r="CC6" s="53"/>
+      <c r="CD6" s="53"/>
+      <c r="CE6" s="53"/>
+      <c r="CF6" s="54"/>
+      <c r="CG6" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="CH6" s="48"/>
-      <c r="CI6" s="48"/>
-      <c r="CJ6" s="48"/>
-      <c r="CK6" s="49"/>
-      <c r="CL6" s="50" t="s">
+      <c r="CH6" s="50"/>
+      <c r="CI6" s="50"/>
+      <c r="CJ6" s="50"/>
+      <c r="CK6" s="51"/>
+      <c r="CL6" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="CM6" s="51"/>
-      <c r="CN6" s="51"/>
-      <c r="CO6" s="51"/>
-      <c r="CP6" s="52"/>
-      <c r="CQ6" s="47" t="s">
+      <c r="CM6" s="53"/>
+      <c r="CN6" s="53"/>
+      <c r="CO6" s="53"/>
+      <c r="CP6" s="54"/>
+      <c r="CQ6" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="CR6" s="48"/>
-      <c r="CS6" s="48"/>
-      <c r="CT6" s="48"/>
-      <c r="CU6" s="49"/>
+      <c r="CR6" s="50"/>
+      <c r="CS6" s="50"/>
+      <c r="CT6" s="50"/>
+      <c r="CU6" s="51"/>
     </row>
     <row r="7" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -3162,104 +3162,104 @@
       <c r="AC20" s="31"/>
     </row>
     <row r="21" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="55"/>
-      <c r="T21" s="55"/>
-      <c r="U21" s="55"/>
-      <c r="V21" s="55"/>
-      <c r="W21" s="55"/>
-      <c r="X21" s="55"/>
-      <c r="Y21" s="55"/>
-      <c r="Z21" s="55"/>
-      <c r="AA21" s="55"/>
-      <c r="AB21" s="55"/>
-      <c r="AC21" s="55"/>
-      <c r="AD21" s="55"/>
-      <c r="AE21" s="55"/>
-      <c r="AF21" s="55"/>
-      <c r="AG21" s="55"/>
-      <c r="AH21" s="55"/>
-      <c r="AI21" s="55"/>
-      <c r="AJ21" s="55"/>
-      <c r="AK21" s="55"/>
-      <c r="AL21" s="55"/>
-      <c r="AM21" s="55"/>
-      <c r="AN21" s="55"/>
-      <c r="AO21" s="55"/>
-      <c r="AP21" s="55"/>
-      <c r="AQ21" s="55"/>
-      <c r="AR21" s="55"/>
-      <c r="AS21" s="55"/>
-      <c r="AT21" s="55"/>
-      <c r="AU21" s="55"/>
-      <c r="AV21" s="55"/>
-      <c r="AW21" s="55"/>
-      <c r="AX21" s="55"/>
-      <c r="AY21" s="55"/>
-      <c r="AZ21" s="55"/>
-      <c r="BA21" s="55"/>
-      <c r="BB21" s="55"/>
-      <c r="BC21" s="55"/>
-      <c r="BD21" s="55"/>
-      <c r="BE21" s="55"/>
-      <c r="BF21" s="55"/>
-      <c r="BG21" s="55"/>
-      <c r="BH21" s="55"/>
-      <c r="BI21" s="55"/>
-      <c r="BJ21" s="55"/>
-      <c r="BK21" s="55"/>
-      <c r="BL21" s="55"/>
-      <c r="BM21" s="55"/>
-      <c r="BN21" s="55"/>
-      <c r="BO21" s="55"/>
-      <c r="BP21" s="55"/>
-      <c r="BQ21" s="55"/>
-      <c r="BR21" s="55"/>
-      <c r="BS21" s="55"/>
-      <c r="BT21" s="55"/>
-      <c r="BU21" s="55"/>
-      <c r="BV21" s="55"/>
-      <c r="BW21" s="55"/>
-      <c r="BX21" s="55"/>
-      <c r="BY21" s="55"/>
-      <c r="BZ21" s="55"/>
-      <c r="CA21" s="55"/>
-      <c r="CB21" s="55"/>
-      <c r="CC21" s="55"/>
-      <c r="CD21" s="55"/>
-      <c r="CE21" s="55"/>
-      <c r="CF21" s="55"/>
-      <c r="CG21" s="55"/>
-      <c r="CH21" s="55"/>
-      <c r="CI21" s="55"/>
-      <c r="CJ21" s="55"/>
-      <c r="CK21" s="55"/>
-      <c r="CL21" s="55"/>
-      <c r="CM21" s="55"/>
-      <c r="CN21" s="55"/>
-      <c r="CO21" s="55"/>
-      <c r="CP21" s="55"/>
-      <c r="CQ21" s="55"/>
-      <c r="CR21" s="55"/>
-      <c r="CS21" s="55"/>
-      <c r="CT21" s="55"/>
-      <c r="CU21" s="55"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="47"/>
+      <c r="Z21" s="47"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="47"/>
+      <c r="AF21" s="47"/>
+      <c r="AG21" s="47"/>
+      <c r="AH21" s="47"/>
+      <c r="AI21" s="47"/>
+      <c r="AJ21" s="47"/>
+      <c r="AK21" s="47"/>
+      <c r="AL21" s="47"/>
+      <c r="AM21" s="47"/>
+      <c r="AN21" s="47"/>
+      <c r="AO21" s="47"/>
+      <c r="AP21" s="47"/>
+      <c r="AQ21" s="47"/>
+      <c r="AR21" s="47"/>
+      <c r="AS21" s="47"/>
+      <c r="AT21" s="47"/>
+      <c r="AU21" s="47"/>
+      <c r="AV21" s="47"/>
+      <c r="AW21" s="47"/>
+      <c r="AX21" s="47"/>
+      <c r="AY21" s="47"/>
+      <c r="AZ21" s="47"/>
+      <c r="BA21" s="47"/>
+      <c r="BB21" s="47"/>
+      <c r="BC21" s="47"/>
+      <c r="BD21" s="47"/>
+      <c r="BE21" s="47"/>
+      <c r="BF21" s="47"/>
+      <c r="BG21" s="47"/>
+      <c r="BH21" s="47"/>
+      <c r="BI21" s="47"/>
+      <c r="BJ21" s="47"/>
+      <c r="BK21" s="47"/>
+      <c r="BL21" s="47"/>
+      <c r="BM21" s="47"/>
+      <c r="BN21" s="47"/>
+      <c r="BO21" s="47"/>
+      <c r="BP21" s="47"/>
+      <c r="BQ21" s="47"/>
+      <c r="BR21" s="47"/>
+      <c r="BS21" s="47"/>
+      <c r="BT21" s="47"/>
+      <c r="BU21" s="47"/>
+      <c r="BV21" s="47"/>
+      <c r="BW21" s="47"/>
+      <c r="BX21" s="47"/>
+      <c r="BY21" s="47"/>
+      <c r="BZ21" s="47"/>
+      <c r="CA21" s="47"/>
+      <c r="CB21" s="47"/>
+      <c r="CC21" s="47"/>
+      <c r="CD21" s="47"/>
+      <c r="CE21" s="47"/>
+      <c r="CF21" s="47"/>
+      <c r="CG21" s="47"/>
+      <c r="CH21" s="47"/>
+      <c r="CI21" s="47"/>
+      <c r="CJ21" s="47"/>
+      <c r="CK21" s="47"/>
+      <c r="CL21" s="47"/>
+      <c r="CM21" s="47"/>
+      <c r="CN21" s="47"/>
+      <c r="CO21" s="47"/>
+      <c r="CP21" s="47"/>
+      <c r="CQ21" s="47"/>
+      <c r="CR21" s="47"/>
+      <c r="CS21" s="47"/>
+      <c r="CT21" s="47"/>
+      <c r="CU21" s="47"/>
     </row>
     <row r="22" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
@@ -3278,7 +3278,7 @@
         <v>26</v>
       </c>
       <c r="G22" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="31"/>
@@ -3351,7 +3351,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="24"/>
       <c r="I23" s="31"/>
@@ -3424,7 +3424,7 @@
         <v>11</v>
       </c>
       <c r="G24" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="24"/>
       <c r="I24" s="31"/>
@@ -3497,7 +3497,7 @@
         <v>26</v>
       </c>
       <c r="G25" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="31"/>
@@ -3554,104 +3554,104 @@
       <c r="CU25" s="35"/>
     </row>
     <row r="26" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="55"/>
-      <c r="S26" s="55"/>
-      <c r="T26" s="55"/>
-      <c r="U26" s="55"/>
-      <c r="V26" s="55"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="55"/>
-      <c r="Y26" s="55"/>
-      <c r="Z26" s="55"/>
-      <c r="AA26" s="55"/>
-      <c r="AB26" s="55"/>
-      <c r="AC26" s="55"/>
-      <c r="AD26" s="55"/>
-      <c r="AE26" s="55"/>
-      <c r="AF26" s="55"/>
-      <c r="AG26" s="55"/>
-      <c r="AH26" s="55"/>
-      <c r="AI26" s="55"/>
-      <c r="AJ26" s="55"/>
-      <c r="AK26" s="55"/>
-      <c r="AL26" s="55"/>
-      <c r="AM26" s="55"/>
-      <c r="AN26" s="55"/>
-      <c r="AO26" s="55"/>
-      <c r="AP26" s="55"/>
-      <c r="AQ26" s="55"/>
-      <c r="AR26" s="55"/>
-      <c r="AS26" s="55"/>
-      <c r="AT26" s="55"/>
-      <c r="AU26" s="55"/>
-      <c r="AV26" s="55"/>
-      <c r="AW26" s="55"/>
-      <c r="AX26" s="55"/>
-      <c r="AY26" s="55"/>
-      <c r="AZ26" s="55"/>
-      <c r="BA26" s="55"/>
-      <c r="BB26" s="55"/>
-      <c r="BC26" s="55"/>
-      <c r="BD26" s="55"/>
-      <c r="BE26" s="55"/>
-      <c r="BF26" s="55"/>
-      <c r="BG26" s="55"/>
-      <c r="BH26" s="55"/>
-      <c r="BI26" s="55"/>
-      <c r="BJ26" s="55"/>
-      <c r="BK26" s="55"/>
-      <c r="BL26" s="55"/>
-      <c r="BM26" s="55"/>
-      <c r="BN26" s="55"/>
-      <c r="BO26" s="55"/>
-      <c r="BP26" s="55"/>
-      <c r="BQ26" s="55"/>
-      <c r="BR26" s="55"/>
-      <c r="BS26" s="55"/>
-      <c r="BT26" s="55"/>
-      <c r="BU26" s="55"/>
-      <c r="BV26" s="55"/>
-      <c r="BW26" s="55"/>
-      <c r="BX26" s="55"/>
-      <c r="BY26" s="55"/>
-      <c r="BZ26" s="55"/>
-      <c r="CA26" s="55"/>
-      <c r="CB26" s="55"/>
-      <c r="CC26" s="55"/>
-      <c r="CD26" s="55"/>
-      <c r="CE26" s="55"/>
-      <c r="CF26" s="55"/>
-      <c r="CG26" s="55"/>
-      <c r="CH26" s="55"/>
-      <c r="CI26" s="55"/>
-      <c r="CJ26" s="55"/>
-      <c r="CK26" s="55"/>
-      <c r="CL26" s="55"/>
-      <c r="CM26" s="55"/>
-      <c r="CN26" s="55"/>
-      <c r="CO26" s="55"/>
-      <c r="CP26" s="55"/>
-      <c r="CQ26" s="55"/>
-      <c r="CR26" s="55"/>
-      <c r="CS26" s="55"/>
-      <c r="CT26" s="55"/>
-      <c r="CU26" s="55"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="47"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="47"/>
+      <c r="AE26" s="47"/>
+      <c r="AF26" s="47"/>
+      <c r="AG26" s="47"/>
+      <c r="AH26" s="47"/>
+      <c r="AI26" s="47"/>
+      <c r="AJ26" s="47"/>
+      <c r="AK26" s="47"/>
+      <c r="AL26" s="47"/>
+      <c r="AM26" s="47"/>
+      <c r="AN26" s="47"/>
+      <c r="AO26" s="47"/>
+      <c r="AP26" s="47"/>
+      <c r="AQ26" s="47"/>
+      <c r="AR26" s="47"/>
+      <c r="AS26" s="47"/>
+      <c r="AT26" s="47"/>
+      <c r="AU26" s="47"/>
+      <c r="AV26" s="47"/>
+      <c r="AW26" s="47"/>
+      <c r="AX26" s="47"/>
+      <c r="AY26" s="47"/>
+      <c r="AZ26" s="47"/>
+      <c r="BA26" s="47"/>
+      <c r="BB26" s="47"/>
+      <c r="BC26" s="47"/>
+      <c r="BD26" s="47"/>
+      <c r="BE26" s="47"/>
+      <c r="BF26" s="47"/>
+      <c r="BG26" s="47"/>
+      <c r="BH26" s="47"/>
+      <c r="BI26" s="47"/>
+      <c r="BJ26" s="47"/>
+      <c r="BK26" s="47"/>
+      <c r="BL26" s="47"/>
+      <c r="BM26" s="47"/>
+      <c r="BN26" s="47"/>
+      <c r="BO26" s="47"/>
+      <c r="BP26" s="47"/>
+      <c r="BQ26" s="47"/>
+      <c r="BR26" s="47"/>
+      <c r="BS26" s="47"/>
+      <c r="BT26" s="47"/>
+      <c r="BU26" s="47"/>
+      <c r="BV26" s="47"/>
+      <c r="BW26" s="47"/>
+      <c r="BX26" s="47"/>
+      <c r="BY26" s="47"/>
+      <c r="BZ26" s="47"/>
+      <c r="CA26" s="47"/>
+      <c r="CB26" s="47"/>
+      <c r="CC26" s="47"/>
+      <c r="CD26" s="47"/>
+      <c r="CE26" s="47"/>
+      <c r="CF26" s="47"/>
+      <c r="CG26" s="47"/>
+      <c r="CH26" s="47"/>
+      <c r="CI26" s="47"/>
+      <c r="CJ26" s="47"/>
+      <c r="CK26" s="47"/>
+      <c r="CL26" s="47"/>
+      <c r="CM26" s="47"/>
+      <c r="CN26" s="47"/>
+      <c r="CO26" s="47"/>
+      <c r="CP26" s="47"/>
+      <c r="CQ26" s="47"/>
+      <c r="CR26" s="47"/>
+      <c r="CS26" s="47"/>
+      <c r="CT26" s="47"/>
+      <c r="CU26" s="47"/>
     </row>
     <row r="27" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
@@ -3952,105 +3952,105 @@
       <c r="CU30" s="35"/>
     </row>
     <row r="31" spans="1:99" s="45" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="56"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
-      <c r="X31" s="56"/>
-      <c r="Y31" s="56"/>
-      <c r="Z31" s="56"/>
-      <c r="AA31" s="56"/>
-      <c r="AB31" s="56"/>
-      <c r="AC31" s="56"/>
-      <c r="AD31" s="56"/>
-      <c r="AE31" s="56"/>
-      <c r="AF31" s="56"/>
-      <c r="AG31" s="56"/>
-      <c r="AH31" s="56"/>
-      <c r="AI31" s="56"/>
-      <c r="AJ31" s="56"/>
-      <c r="AK31" s="56"/>
-      <c r="AL31" s="56"/>
-      <c r="AM31" s="56"/>
-      <c r="AN31" s="56"/>
-      <c r="AO31" s="56"/>
-      <c r="AP31" s="56"/>
-      <c r="AQ31" s="56"/>
-      <c r="AR31" s="56"/>
-      <c r="AS31" s="56"/>
-      <c r="AT31" s="56"/>
-      <c r="AU31" s="56"/>
-      <c r="AV31" s="56"/>
-      <c r="AW31" s="56"/>
-      <c r="AX31" s="56"/>
-      <c r="AY31" s="56"/>
-      <c r="AZ31" s="56"/>
-      <c r="BA31" s="56"/>
-      <c r="BB31" s="56"/>
-      <c r="BC31" s="56"/>
-      <c r="BD31" s="56"/>
-      <c r="BE31" s="56"/>
-      <c r="BF31" s="56"/>
-      <c r="BG31" s="56"/>
-      <c r="BH31" s="56"/>
-      <c r="BI31" s="56"/>
-      <c r="BJ31" s="56"/>
-      <c r="BK31" s="56"/>
-      <c r="BL31" s="56"/>
-      <c r="BM31" s="56"/>
-      <c r="BN31" s="56"/>
-      <c r="BO31" s="56"/>
-      <c r="BP31" s="56"/>
-      <c r="BQ31" s="56"/>
-      <c r="BR31" s="56"/>
-      <c r="BS31" s="56"/>
-      <c r="BT31" s="56"/>
-      <c r="BU31" s="56"/>
-      <c r="BV31" s="56"/>
-      <c r="BW31" s="56"/>
-      <c r="BX31" s="56"/>
-      <c r="BY31" s="56"/>
-      <c r="BZ31" s="56"/>
-      <c r="CA31" s="56"/>
-      <c r="CB31" s="56"/>
-      <c r="CC31" s="56"/>
-      <c r="CD31" s="56"/>
-      <c r="CE31" s="56"/>
-      <c r="CF31" s="56"/>
-      <c r="CG31" s="56"/>
-      <c r="CH31" s="56"/>
-      <c r="CI31" s="56"/>
-      <c r="CJ31" s="56"/>
-      <c r="CK31" s="56"/>
-      <c r="CL31" s="56"/>
-      <c r="CM31" s="56"/>
-      <c r="CN31" s="56"/>
-      <c r="CO31" s="56"/>
-      <c r="CP31" s="56"/>
-      <c r="CQ31" s="56"/>
-      <c r="CR31" s="56"/>
-      <c r="CS31" s="56"/>
-      <c r="CT31" s="56"/>
-      <c r="CU31" s="56"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="48"/>
+      <c r="V31" s="48"/>
+      <c r="W31" s="48"/>
+      <c r="X31" s="48"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="48"/>
+      <c r="AA31" s="48"/>
+      <c r="AB31" s="48"/>
+      <c r="AC31" s="48"/>
+      <c r="AD31" s="48"/>
+      <c r="AE31" s="48"/>
+      <c r="AF31" s="48"/>
+      <c r="AG31" s="48"/>
+      <c r="AH31" s="48"/>
+      <c r="AI31" s="48"/>
+      <c r="AJ31" s="48"/>
+      <c r="AK31" s="48"/>
+      <c r="AL31" s="48"/>
+      <c r="AM31" s="48"/>
+      <c r="AN31" s="48"/>
+      <c r="AO31" s="48"/>
+      <c r="AP31" s="48"/>
+      <c r="AQ31" s="48"/>
+      <c r="AR31" s="48"/>
+      <c r="AS31" s="48"/>
+      <c r="AT31" s="48"/>
+      <c r="AU31" s="48"/>
+      <c r="AV31" s="48"/>
+      <c r="AW31" s="48"/>
+      <c r="AX31" s="48"/>
+      <c r="AY31" s="48"/>
+      <c r="AZ31" s="48"/>
+      <c r="BA31" s="48"/>
+      <c r="BB31" s="48"/>
+      <c r="BC31" s="48"/>
+      <c r="BD31" s="48"/>
+      <c r="BE31" s="48"/>
+      <c r="BF31" s="48"/>
+      <c r="BG31" s="48"/>
+      <c r="BH31" s="48"/>
+      <c r="BI31" s="48"/>
+      <c r="BJ31" s="48"/>
+      <c r="BK31" s="48"/>
+      <c r="BL31" s="48"/>
+      <c r="BM31" s="48"/>
+      <c r="BN31" s="48"/>
+      <c r="BO31" s="48"/>
+      <c r="BP31" s="48"/>
+      <c r="BQ31" s="48"/>
+      <c r="BR31" s="48"/>
+      <c r="BS31" s="48"/>
+      <c r="BT31" s="48"/>
+      <c r="BU31" s="48"/>
+      <c r="BV31" s="48"/>
+      <c r="BW31" s="48"/>
+      <c r="BX31" s="48"/>
+      <c r="BY31" s="48"/>
+      <c r="BZ31" s="48"/>
+      <c r="CA31" s="48"/>
+      <c r="CB31" s="48"/>
+      <c r="CC31" s="48"/>
+      <c r="CD31" s="48"/>
+      <c r="CE31" s="48"/>
+      <c r="CF31" s="48"/>
+      <c r="CG31" s="48"/>
+      <c r="CH31" s="48"/>
+      <c r="CI31" s="48"/>
+      <c r="CJ31" s="48"/>
+      <c r="CK31" s="48"/>
+      <c r="CL31" s="48"/>
+      <c r="CM31" s="48"/>
+      <c r="CN31" s="48"/>
+      <c r="CO31" s="48"/>
+      <c r="CP31" s="48"/>
+      <c r="CQ31" s="48"/>
+      <c r="CR31" s="48"/>
+      <c r="CS31" s="48"/>
+      <c r="CT31" s="48"/>
+      <c r="CU31" s="48"/>
     </row>
     <row r="32" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
@@ -7697,21 +7697,22 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A13:CU13"/>
-    <mergeCell ref="B21:CU21"/>
-    <mergeCell ref="B26:CU26"/>
-    <mergeCell ref="A31:CU31"/>
-    <mergeCell ref="A42:CU42"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="AD5:AH5"/>
-    <mergeCell ref="AD6:AH6"/>
-    <mergeCell ref="B2:G4"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="O6:S6"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A57:CU57"/>
+    <mergeCell ref="B49:CU49"/>
+    <mergeCell ref="A52:CU52"/>
+    <mergeCell ref="CQ5:CU5"/>
+    <mergeCell ref="CQ6:CU6"/>
+    <mergeCell ref="CL5:CP5"/>
+    <mergeCell ref="CL6:CP6"/>
+    <mergeCell ref="AX5:BB5"/>
+    <mergeCell ref="AX6:BB6"/>
+    <mergeCell ref="AI5:AM5"/>
+    <mergeCell ref="AI6:AM6"/>
+    <mergeCell ref="AN5:AR5"/>
+    <mergeCell ref="AN6:AR6"/>
+    <mergeCell ref="AS5:AW5"/>
+    <mergeCell ref="AS6:AW6"/>
+    <mergeCell ref="Y5:AC5"/>
     <mergeCell ref="BE2:BW2"/>
     <mergeCell ref="BE3:BW3"/>
     <mergeCell ref="CB5:CF5"/>
@@ -7728,22 +7729,21 @@
     <mergeCell ref="BC6:BG6"/>
     <mergeCell ref="BH5:BL5"/>
     <mergeCell ref="BH6:BL6"/>
-    <mergeCell ref="A57:CU57"/>
-    <mergeCell ref="B49:CU49"/>
-    <mergeCell ref="A52:CU52"/>
-    <mergeCell ref="CQ5:CU5"/>
-    <mergeCell ref="CQ6:CU6"/>
-    <mergeCell ref="CL5:CP5"/>
-    <mergeCell ref="CL6:CP6"/>
-    <mergeCell ref="AX5:BB5"/>
-    <mergeCell ref="AX6:BB6"/>
-    <mergeCell ref="AI5:AM5"/>
-    <mergeCell ref="AI6:AM6"/>
-    <mergeCell ref="AN5:AR5"/>
-    <mergeCell ref="AN6:AR6"/>
-    <mergeCell ref="AS5:AW5"/>
-    <mergeCell ref="AS6:AW6"/>
-    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="AD6:AH6"/>
+    <mergeCell ref="B2:G4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="O6:S6"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A13:CU13"/>
+    <mergeCell ref="B21:CU21"/>
+    <mergeCell ref="B26:CU26"/>
+    <mergeCell ref="A31:CU31"/>
+    <mergeCell ref="A42:CU42"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J53:CU56 J50:CU51 J32:CU41 J43:CU48 J58:CU59 J75:CU75">
     <cfRule type="expression" dxfId="25" priority="84">

</xml_diff>

<commit_message>
imagens do projeto renderizadas
</commit_message>
<xml_diff>
--- a/LaTeX Project/Documentos/Gantt.xlsx
+++ b/LaTeX Project/Documentos/Gantt.xlsx
@@ -1016,6 +1016,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1034,16 +1040,10 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1810,8 +1810,8 @@
   </sheetPr>
   <dimension ref="A2:CU84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AS33" sqref="AS33:AZ35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1836,47 +1836,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="24" t="s">
         <v>78</v>
       </c>
       <c r="I2" s="16"/>
-      <c r="BE2" s="53" t="s">
+      <c r="BE2" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" s="53"/>
-      <c r="BG2" s="53"/>
-      <c r="BH2" s="53"/>
-      <c r="BI2" s="53"/>
-      <c r="BJ2" s="53"/>
-      <c r="BK2" s="53"/>
-      <c r="BL2" s="53"/>
-      <c r="BM2" s="53"/>
-      <c r="BN2" s="53"/>
-      <c r="BO2" s="53"/>
-      <c r="BP2" s="53"/>
-      <c r="BQ2" s="53"/>
-      <c r="BR2" s="53"/>
-      <c r="BS2" s="53"/>
-      <c r="BT2" s="53"/>
-      <c r="BU2" s="53"/>
-      <c r="BV2" s="53"/>
-      <c r="BW2" s="53"/>
+      <c r="BF2" s="56"/>
+      <c r="BG2" s="56"/>
+      <c r="BH2" s="56"/>
+      <c r="BI2" s="56"/>
+      <c r="BJ2" s="56"/>
+      <c r="BK2" s="56"/>
+      <c r="BL2" s="56"/>
+      <c r="BM2" s="56"/>
+      <c r="BN2" s="56"/>
+      <c r="BO2" s="56"/>
+      <c r="BP2" s="56"/>
+      <c r="BQ2" s="56"/>
+      <c r="BR2" s="56"/>
+      <c r="BS2" s="56"/>
+      <c r="BT2" s="56"/>
+      <c r="BU2" s="56"/>
+      <c r="BV2" s="56"/>
+      <c r="BW2" s="56"/>
     </row>
     <row r="3" spans="1:99" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="24" t="s">
         <v>79</v>
       </c>
@@ -1925,35 +1925,35 @@
       <c r="AQ3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="BE3" s="53" t="s">
+      <c r="BE3" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="BF3" s="53"/>
-      <c r="BG3" s="53"/>
-      <c r="BH3" s="53"/>
-      <c r="BI3" s="53"/>
-      <c r="BJ3" s="53"/>
-      <c r="BK3" s="53"/>
-      <c r="BL3" s="53"/>
-      <c r="BM3" s="53"/>
-      <c r="BN3" s="53"/>
-      <c r="BO3" s="53"/>
-      <c r="BP3" s="53"/>
-      <c r="BQ3" s="53"/>
-      <c r="BR3" s="53"/>
-      <c r="BS3" s="53"/>
-      <c r="BT3" s="53"/>
-      <c r="BU3" s="53"/>
-      <c r="BV3" s="53"/>
-      <c r="BW3" s="53"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
+      <c r="BI3" s="56"/>
+      <c r="BJ3" s="56"/>
+      <c r="BK3" s="56"/>
+      <c r="BL3" s="56"/>
+      <c r="BM3" s="56"/>
+      <c r="BN3" s="56"/>
+      <c r="BO3" s="56"/>
+      <c r="BP3" s="56"/>
+      <c r="BQ3" s="56"/>
+      <c r="BR3" s="56"/>
+      <c r="BS3" s="56"/>
+      <c r="BT3" s="56"/>
+      <c r="BU3" s="56"/>
+      <c r="BV3" s="56"/>
+      <c r="BW3" s="56"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="24" t="s">
         <v>80</v>
       </c>
@@ -1984,132 +1984,132 @@
       <c r="AY4" s="19"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="47" t="s">
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="50" t="s">
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="47" t="s">
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="48"/>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="50" t="s">
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="50"/>
+      <c r="AB5" s="50"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="51"/>
-      <c r="AF5" s="51"/>
-      <c r="AG5" s="51"/>
-      <c r="AH5" s="52"/>
-      <c r="AI5" s="47" t="s">
+      <c r="AE5" s="53"/>
+      <c r="AF5" s="53"/>
+      <c r="AG5" s="53"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="48"/>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="49"/>
-      <c r="AN5" s="50" t="s">
+      <c r="AJ5" s="50"/>
+      <c r="AK5" s="50"/>
+      <c r="AL5" s="50"/>
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="51"/>
-      <c r="AP5" s="51"/>
-      <c r="AQ5" s="51"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="47" t="s">
+      <c r="AO5" s="53"/>
+      <c r="AP5" s="53"/>
+      <c r="AQ5" s="53"/>
+      <c r="AR5" s="54"/>
+      <c r="AS5" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="AT5" s="48"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="48"/>
-      <c r="AW5" s="49"/>
-      <c r="AX5" s="50" t="s">
+      <c r="AT5" s="50"/>
+      <c r="AU5" s="50"/>
+      <c r="AV5" s="50"/>
+      <c r="AW5" s="51"/>
+      <c r="AX5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="AY5" s="51"/>
-      <c r="AZ5" s="51"/>
-      <c r="BA5" s="51"/>
-      <c r="BB5" s="52"/>
-      <c r="BC5" s="47" t="s">
+      <c r="AY5" s="53"/>
+      <c r="AZ5" s="53"/>
+      <c r="BA5" s="53"/>
+      <c r="BB5" s="54"/>
+      <c r="BC5" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="BD5" s="48"/>
-      <c r="BE5" s="48"/>
-      <c r="BF5" s="48"/>
-      <c r="BG5" s="49"/>
-      <c r="BH5" s="50" t="s">
+      <c r="BD5" s="50"/>
+      <c r="BE5" s="50"/>
+      <c r="BF5" s="50"/>
+      <c r="BG5" s="51"/>
+      <c r="BH5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="BI5" s="51"/>
-      <c r="BJ5" s="51"/>
-      <c r="BK5" s="51"/>
-      <c r="BL5" s="52"/>
-      <c r="BM5" s="47" t="s">
+      <c r="BI5" s="53"/>
+      <c r="BJ5" s="53"/>
+      <c r="BK5" s="53"/>
+      <c r="BL5" s="54"/>
+      <c r="BM5" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="BN5" s="48"/>
-      <c r="BO5" s="48"/>
-      <c r="BP5" s="48"/>
-      <c r="BQ5" s="49"/>
-      <c r="BR5" s="50" t="s">
+      <c r="BN5" s="50"/>
+      <c r="BO5" s="50"/>
+      <c r="BP5" s="50"/>
+      <c r="BQ5" s="51"/>
+      <c r="BR5" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="BS5" s="51"/>
-      <c r="BT5" s="51"/>
-      <c r="BU5" s="51"/>
-      <c r="BV5" s="52"/>
-      <c r="BW5" s="47" t="s">
+      <c r="BS5" s="53"/>
+      <c r="BT5" s="53"/>
+      <c r="BU5" s="53"/>
+      <c r="BV5" s="54"/>
+      <c r="BW5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="BX5" s="48"/>
-      <c r="BY5" s="48"/>
-      <c r="BZ5" s="48"/>
-      <c r="CA5" s="49"/>
-      <c r="CB5" s="50" t="s">
+      <c r="BX5" s="50"/>
+      <c r="BY5" s="50"/>
+      <c r="BZ5" s="50"/>
+      <c r="CA5" s="51"/>
+      <c r="CB5" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="CC5" s="51"/>
-      <c r="CD5" s="51"/>
-      <c r="CE5" s="51"/>
-      <c r="CF5" s="52"/>
-      <c r="CG5" s="47" t="s">
+      <c r="CC5" s="53"/>
+      <c r="CD5" s="53"/>
+      <c r="CE5" s="53"/>
+      <c r="CF5" s="54"/>
+      <c r="CG5" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="CH5" s="48"/>
-      <c r="CI5" s="48"/>
-      <c r="CJ5" s="48"/>
-      <c r="CK5" s="49"/>
-      <c r="CL5" s="50" t="s">
+      <c r="CH5" s="50"/>
+      <c r="CI5" s="50"/>
+      <c r="CJ5" s="50"/>
+      <c r="CK5" s="51"/>
+      <c r="CL5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="CM5" s="51"/>
-      <c r="CN5" s="51"/>
-      <c r="CO5" s="51"/>
-      <c r="CP5" s="52"/>
-      <c r="CQ5" s="47" t="s">
+      <c r="CM5" s="53"/>
+      <c r="CN5" s="53"/>
+      <c r="CO5" s="53"/>
+      <c r="CP5" s="54"/>
+      <c r="CQ5" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="CR5" s="48"/>
-      <c r="CS5" s="48"/>
-      <c r="CT5" s="48"/>
-      <c r="CU5" s="49"/>
+      <c r="CR5" s="50"/>
+      <c r="CS5" s="50"/>
+      <c r="CT5" s="50"/>
+      <c r="CU5" s="51"/>
     </row>
     <row r="6" spans="1:99" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -2132,132 +2132,132 @@
         <v>75</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="47" t="s">
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="50" t="s">
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="51"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="47" t="s">
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="Z6" s="48"/>
-      <c r="AA6" s="48"/>
-      <c r="AB6" s="48"/>
-      <c r="AC6" s="49"/>
-      <c r="AD6" s="50" t="s">
+      <c r="Z6" s="50"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="50"/>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="51"/>
-      <c r="AF6" s="51"/>
-      <c r="AG6" s="51"/>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="47" t="s">
+      <c r="AE6" s="53"/>
+      <c r="AF6" s="53"/>
+      <c r="AG6" s="53"/>
+      <c r="AH6" s="54"/>
+      <c r="AI6" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="48"/>
-      <c r="AL6" s="48"/>
-      <c r="AM6" s="49"/>
-      <c r="AN6" s="50" t="s">
+      <c r="AJ6" s="50"/>
+      <c r="AK6" s="50"/>
+      <c r="AL6" s="50"/>
+      <c r="AM6" s="51"/>
+      <c r="AN6" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" s="51"/>
-      <c r="AP6" s="51"/>
-      <c r="AQ6" s="51"/>
-      <c r="AR6" s="52"/>
-      <c r="AS6" s="47" t="s">
+      <c r="AO6" s="53"/>
+      <c r="AP6" s="53"/>
+      <c r="AQ6" s="53"/>
+      <c r="AR6" s="54"/>
+      <c r="AS6" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="AT6" s="48"/>
-      <c r="AU6" s="48"/>
-      <c r="AV6" s="48"/>
-      <c r="AW6" s="49"/>
-      <c r="AX6" s="50" t="s">
+      <c r="AT6" s="50"/>
+      <c r="AU6" s="50"/>
+      <c r="AV6" s="50"/>
+      <c r="AW6" s="51"/>
+      <c r="AX6" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="AY6" s="51"/>
-      <c r="AZ6" s="51"/>
-      <c r="BA6" s="51"/>
-      <c r="BB6" s="52"/>
-      <c r="BC6" s="47" t="s">
+      <c r="AY6" s="53"/>
+      <c r="AZ6" s="53"/>
+      <c r="BA6" s="53"/>
+      <c r="BB6" s="54"/>
+      <c r="BC6" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="BD6" s="48"/>
-      <c r="BE6" s="48"/>
-      <c r="BF6" s="48"/>
-      <c r="BG6" s="49"/>
-      <c r="BH6" s="50" t="s">
+      <c r="BD6" s="50"/>
+      <c r="BE6" s="50"/>
+      <c r="BF6" s="50"/>
+      <c r="BG6" s="51"/>
+      <c r="BH6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="BI6" s="51"/>
-      <c r="BJ6" s="51"/>
-      <c r="BK6" s="51"/>
-      <c r="BL6" s="52"/>
-      <c r="BM6" s="47" t="s">
+      <c r="BI6" s="53"/>
+      <c r="BJ6" s="53"/>
+      <c r="BK6" s="53"/>
+      <c r="BL6" s="54"/>
+      <c r="BM6" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="BN6" s="48"/>
-      <c r="BO6" s="48"/>
-      <c r="BP6" s="48"/>
-      <c r="BQ6" s="49"/>
-      <c r="BR6" s="50" t="s">
+      <c r="BN6" s="50"/>
+      <c r="BO6" s="50"/>
+      <c r="BP6" s="50"/>
+      <c r="BQ6" s="51"/>
+      <c r="BR6" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="BS6" s="51"/>
-      <c r="BT6" s="51"/>
-      <c r="BU6" s="51"/>
-      <c r="BV6" s="52"/>
-      <c r="BW6" s="47" t="s">
+      <c r="BS6" s="53"/>
+      <c r="BT6" s="53"/>
+      <c r="BU6" s="53"/>
+      <c r="BV6" s="54"/>
+      <c r="BW6" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="BX6" s="48"/>
-      <c r="BY6" s="48"/>
-      <c r="BZ6" s="48"/>
-      <c r="CA6" s="49"/>
-      <c r="CB6" s="50" t="s">
+      <c r="BX6" s="50"/>
+      <c r="BY6" s="50"/>
+      <c r="BZ6" s="50"/>
+      <c r="CA6" s="51"/>
+      <c r="CB6" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="CC6" s="51"/>
-      <c r="CD6" s="51"/>
-      <c r="CE6" s="51"/>
-      <c r="CF6" s="52"/>
-      <c r="CG6" s="47" t="s">
+      <c r="CC6" s="53"/>
+      <c r="CD6" s="53"/>
+      <c r="CE6" s="53"/>
+      <c r="CF6" s="54"/>
+      <c r="CG6" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="CH6" s="48"/>
-      <c r="CI6" s="48"/>
-      <c r="CJ6" s="48"/>
-      <c r="CK6" s="49"/>
-      <c r="CL6" s="50" t="s">
+      <c r="CH6" s="50"/>
+      <c r="CI6" s="50"/>
+      <c r="CJ6" s="50"/>
+      <c r="CK6" s="51"/>
+      <c r="CL6" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="CM6" s="51"/>
-      <c r="CN6" s="51"/>
-      <c r="CO6" s="51"/>
-      <c r="CP6" s="52"/>
-      <c r="CQ6" s="47" t="s">
+      <c r="CM6" s="53"/>
+      <c r="CN6" s="53"/>
+      <c r="CO6" s="53"/>
+      <c r="CP6" s="54"/>
+      <c r="CQ6" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="CR6" s="48"/>
-      <c r="CS6" s="48"/>
-      <c r="CT6" s="48"/>
-      <c r="CU6" s="49"/>
+      <c r="CR6" s="50"/>
+      <c r="CS6" s="50"/>
+      <c r="CT6" s="50"/>
+      <c r="CU6" s="51"/>
     </row>
     <row r="7" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -3162,104 +3162,104 @@
       <c r="AC20" s="31"/>
     </row>
     <row r="21" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="55"/>
-      <c r="T21" s="55"/>
-      <c r="U21" s="55"/>
-      <c r="V21" s="55"/>
-      <c r="W21" s="55"/>
-      <c r="X21" s="55"/>
-      <c r="Y21" s="55"/>
-      <c r="Z21" s="55"/>
-      <c r="AA21" s="55"/>
-      <c r="AB21" s="55"/>
-      <c r="AC21" s="55"/>
-      <c r="AD21" s="55"/>
-      <c r="AE21" s="55"/>
-      <c r="AF21" s="55"/>
-      <c r="AG21" s="55"/>
-      <c r="AH21" s="55"/>
-      <c r="AI21" s="55"/>
-      <c r="AJ21" s="55"/>
-      <c r="AK21" s="55"/>
-      <c r="AL21" s="55"/>
-      <c r="AM21" s="55"/>
-      <c r="AN21" s="55"/>
-      <c r="AO21" s="55"/>
-      <c r="AP21" s="55"/>
-      <c r="AQ21" s="55"/>
-      <c r="AR21" s="55"/>
-      <c r="AS21" s="55"/>
-      <c r="AT21" s="55"/>
-      <c r="AU21" s="55"/>
-      <c r="AV21" s="55"/>
-      <c r="AW21" s="55"/>
-      <c r="AX21" s="55"/>
-      <c r="AY21" s="55"/>
-      <c r="AZ21" s="55"/>
-      <c r="BA21" s="55"/>
-      <c r="BB21" s="55"/>
-      <c r="BC21" s="55"/>
-      <c r="BD21" s="55"/>
-      <c r="BE21" s="55"/>
-      <c r="BF21" s="55"/>
-      <c r="BG21" s="55"/>
-      <c r="BH21" s="55"/>
-      <c r="BI21" s="55"/>
-      <c r="BJ21" s="55"/>
-      <c r="BK21" s="55"/>
-      <c r="BL21" s="55"/>
-      <c r="BM21" s="55"/>
-      <c r="BN21" s="55"/>
-      <c r="BO21" s="55"/>
-      <c r="BP21" s="55"/>
-      <c r="BQ21" s="55"/>
-      <c r="BR21" s="55"/>
-      <c r="BS21" s="55"/>
-      <c r="BT21" s="55"/>
-      <c r="BU21" s="55"/>
-      <c r="BV21" s="55"/>
-      <c r="BW21" s="55"/>
-      <c r="BX21" s="55"/>
-      <c r="BY21" s="55"/>
-      <c r="BZ21" s="55"/>
-      <c r="CA21" s="55"/>
-      <c r="CB21" s="55"/>
-      <c r="CC21" s="55"/>
-      <c r="CD21" s="55"/>
-      <c r="CE21" s="55"/>
-      <c r="CF21" s="55"/>
-      <c r="CG21" s="55"/>
-      <c r="CH21" s="55"/>
-      <c r="CI21" s="55"/>
-      <c r="CJ21" s="55"/>
-      <c r="CK21" s="55"/>
-      <c r="CL21" s="55"/>
-      <c r="CM21" s="55"/>
-      <c r="CN21" s="55"/>
-      <c r="CO21" s="55"/>
-      <c r="CP21" s="55"/>
-      <c r="CQ21" s="55"/>
-      <c r="CR21" s="55"/>
-      <c r="CS21" s="55"/>
-      <c r="CT21" s="55"/>
-      <c r="CU21" s="55"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="47"/>
+      <c r="Z21" s="47"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="47"/>
+      <c r="AF21" s="47"/>
+      <c r="AG21" s="47"/>
+      <c r="AH21" s="47"/>
+      <c r="AI21" s="47"/>
+      <c r="AJ21" s="47"/>
+      <c r="AK21" s="47"/>
+      <c r="AL21" s="47"/>
+      <c r="AM21" s="47"/>
+      <c r="AN21" s="47"/>
+      <c r="AO21" s="47"/>
+      <c r="AP21" s="47"/>
+      <c r="AQ21" s="47"/>
+      <c r="AR21" s="47"/>
+      <c r="AS21" s="47"/>
+      <c r="AT21" s="47"/>
+      <c r="AU21" s="47"/>
+      <c r="AV21" s="47"/>
+      <c r="AW21" s="47"/>
+      <c r="AX21" s="47"/>
+      <c r="AY21" s="47"/>
+      <c r="AZ21" s="47"/>
+      <c r="BA21" s="47"/>
+      <c r="BB21" s="47"/>
+      <c r="BC21" s="47"/>
+      <c r="BD21" s="47"/>
+      <c r="BE21" s="47"/>
+      <c r="BF21" s="47"/>
+      <c r="BG21" s="47"/>
+      <c r="BH21" s="47"/>
+      <c r="BI21" s="47"/>
+      <c r="BJ21" s="47"/>
+      <c r="BK21" s="47"/>
+      <c r="BL21" s="47"/>
+      <c r="BM21" s="47"/>
+      <c r="BN21" s="47"/>
+      <c r="BO21" s="47"/>
+      <c r="BP21" s="47"/>
+      <c r="BQ21" s="47"/>
+      <c r="BR21" s="47"/>
+      <c r="BS21" s="47"/>
+      <c r="BT21" s="47"/>
+      <c r="BU21" s="47"/>
+      <c r="BV21" s="47"/>
+      <c r="BW21" s="47"/>
+      <c r="BX21" s="47"/>
+      <c r="BY21" s="47"/>
+      <c r="BZ21" s="47"/>
+      <c r="CA21" s="47"/>
+      <c r="CB21" s="47"/>
+      <c r="CC21" s="47"/>
+      <c r="CD21" s="47"/>
+      <c r="CE21" s="47"/>
+      <c r="CF21" s="47"/>
+      <c r="CG21" s="47"/>
+      <c r="CH21" s="47"/>
+      <c r="CI21" s="47"/>
+      <c r="CJ21" s="47"/>
+      <c r="CK21" s="47"/>
+      <c r="CL21" s="47"/>
+      <c r="CM21" s="47"/>
+      <c r="CN21" s="47"/>
+      <c r="CO21" s="47"/>
+      <c r="CP21" s="47"/>
+      <c r="CQ21" s="47"/>
+      <c r="CR21" s="47"/>
+      <c r="CS21" s="47"/>
+      <c r="CT21" s="47"/>
+      <c r="CU21" s="47"/>
     </row>
     <row r="22" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
@@ -3554,104 +3554,104 @@
       <c r="CU25" s="35"/>
     </row>
     <row r="26" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="55"/>
-      <c r="S26" s="55"/>
-      <c r="T26" s="55"/>
-      <c r="U26" s="55"/>
-      <c r="V26" s="55"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="55"/>
-      <c r="Y26" s="55"/>
-      <c r="Z26" s="55"/>
-      <c r="AA26" s="55"/>
-      <c r="AB26" s="55"/>
-      <c r="AC26" s="55"/>
-      <c r="AD26" s="55"/>
-      <c r="AE26" s="55"/>
-      <c r="AF26" s="55"/>
-      <c r="AG26" s="55"/>
-      <c r="AH26" s="55"/>
-      <c r="AI26" s="55"/>
-      <c r="AJ26" s="55"/>
-      <c r="AK26" s="55"/>
-      <c r="AL26" s="55"/>
-      <c r="AM26" s="55"/>
-      <c r="AN26" s="55"/>
-      <c r="AO26" s="55"/>
-      <c r="AP26" s="55"/>
-      <c r="AQ26" s="55"/>
-      <c r="AR26" s="55"/>
-      <c r="AS26" s="55"/>
-      <c r="AT26" s="55"/>
-      <c r="AU26" s="55"/>
-      <c r="AV26" s="55"/>
-      <c r="AW26" s="55"/>
-      <c r="AX26" s="55"/>
-      <c r="AY26" s="55"/>
-      <c r="AZ26" s="55"/>
-      <c r="BA26" s="55"/>
-      <c r="BB26" s="55"/>
-      <c r="BC26" s="55"/>
-      <c r="BD26" s="55"/>
-      <c r="BE26" s="55"/>
-      <c r="BF26" s="55"/>
-      <c r="BG26" s="55"/>
-      <c r="BH26" s="55"/>
-      <c r="BI26" s="55"/>
-      <c r="BJ26" s="55"/>
-      <c r="BK26" s="55"/>
-      <c r="BL26" s="55"/>
-      <c r="BM26" s="55"/>
-      <c r="BN26" s="55"/>
-      <c r="BO26" s="55"/>
-      <c r="BP26" s="55"/>
-      <c r="BQ26" s="55"/>
-      <c r="BR26" s="55"/>
-      <c r="BS26" s="55"/>
-      <c r="BT26" s="55"/>
-      <c r="BU26" s="55"/>
-      <c r="BV26" s="55"/>
-      <c r="BW26" s="55"/>
-      <c r="BX26" s="55"/>
-      <c r="BY26" s="55"/>
-      <c r="BZ26" s="55"/>
-      <c r="CA26" s="55"/>
-      <c r="CB26" s="55"/>
-      <c r="CC26" s="55"/>
-      <c r="CD26" s="55"/>
-      <c r="CE26" s="55"/>
-      <c r="CF26" s="55"/>
-      <c r="CG26" s="55"/>
-      <c r="CH26" s="55"/>
-      <c r="CI26" s="55"/>
-      <c r="CJ26" s="55"/>
-      <c r="CK26" s="55"/>
-      <c r="CL26" s="55"/>
-      <c r="CM26" s="55"/>
-      <c r="CN26" s="55"/>
-      <c r="CO26" s="55"/>
-      <c r="CP26" s="55"/>
-      <c r="CQ26" s="55"/>
-      <c r="CR26" s="55"/>
-      <c r="CS26" s="55"/>
-      <c r="CT26" s="55"/>
-      <c r="CU26" s="55"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="47"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="47"/>
+      <c r="AE26" s="47"/>
+      <c r="AF26" s="47"/>
+      <c r="AG26" s="47"/>
+      <c r="AH26" s="47"/>
+      <c r="AI26" s="47"/>
+      <c r="AJ26" s="47"/>
+      <c r="AK26" s="47"/>
+      <c r="AL26" s="47"/>
+      <c r="AM26" s="47"/>
+      <c r="AN26" s="47"/>
+      <c r="AO26" s="47"/>
+      <c r="AP26" s="47"/>
+      <c r="AQ26" s="47"/>
+      <c r="AR26" s="47"/>
+      <c r="AS26" s="47"/>
+      <c r="AT26" s="47"/>
+      <c r="AU26" s="47"/>
+      <c r="AV26" s="47"/>
+      <c r="AW26" s="47"/>
+      <c r="AX26" s="47"/>
+      <c r="AY26" s="47"/>
+      <c r="AZ26" s="47"/>
+      <c r="BA26" s="47"/>
+      <c r="BB26" s="47"/>
+      <c r="BC26" s="47"/>
+      <c r="BD26" s="47"/>
+      <c r="BE26" s="47"/>
+      <c r="BF26" s="47"/>
+      <c r="BG26" s="47"/>
+      <c r="BH26" s="47"/>
+      <c r="BI26" s="47"/>
+      <c r="BJ26" s="47"/>
+      <c r="BK26" s="47"/>
+      <c r="BL26" s="47"/>
+      <c r="BM26" s="47"/>
+      <c r="BN26" s="47"/>
+      <c r="BO26" s="47"/>
+      <c r="BP26" s="47"/>
+      <c r="BQ26" s="47"/>
+      <c r="BR26" s="47"/>
+      <c r="BS26" s="47"/>
+      <c r="BT26" s="47"/>
+      <c r="BU26" s="47"/>
+      <c r="BV26" s="47"/>
+      <c r="BW26" s="47"/>
+      <c r="BX26" s="47"/>
+      <c r="BY26" s="47"/>
+      <c r="BZ26" s="47"/>
+      <c r="CA26" s="47"/>
+      <c r="CB26" s="47"/>
+      <c r="CC26" s="47"/>
+      <c r="CD26" s="47"/>
+      <c r="CE26" s="47"/>
+      <c r="CF26" s="47"/>
+      <c r="CG26" s="47"/>
+      <c r="CH26" s="47"/>
+      <c r="CI26" s="47"/>
+      <c r="CJ26" s="47"/>
+      <c r="CK26" s="47"/>
+      <c r="CL26" s="47"/>
+      <c r="CM26" s="47"/>
+      <c r="CN26" s="47"/>
+      <c r="CO26" s="47"/>
+      <c r="CP26" s="47"/>
+      <c r="CQ26" s="47"/>
+      <c r="CR26" s="47"/>
+      <c r="CS26" s="47"/>
+      <c r="CT26" s="47"/>
+      <c r="CU26" s="47"/>
     </row>
     <row r="27" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
@@ -3952,105 +3952,105 @@
       <c r="CU30" s="35"/>
     </row>
     <row r="31" spans="1:99" s="45" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="56"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
-      <c r="X31" s="56"/>
-      <c r="Y31" s="56"/>
-      <c r="Z31" s="56"/>
-      <c r="AA31" s="56"/>
-      <c r="AB31" s="56"/>
-      <c r="AC31" s="56"/>
-      <c r="AD31" s="56"/>
-      <c r="AE31" s="56"/>
-      <c r="AF31" s="56"/>
-      <c r="AG31" s="56"/>
-      <c r="AH31" s="56"/>
-      <c r="AI31" s="56"/>
-      <c r="AJ31" s="56"/>
-      <c r="AK31" s="56"/>
-      <c r="AL31" s="56"/>
-      <c r="AM31" s="56"/>
-      <c r="AN31" s="56"/>
-      <c r="AO31" s="56"/>
-      <c r="AP31" s="56"/>
-      <c r="AQ31" s="56"/>
-      <c r="AR31" s="56"/>
-      <c r="AS31" s="56"/>
-      <c r="AT31" s="56"/>
-      <c r="AU31" s="56"/>
-      <c r="AV31" s="56"/>
-      <c r="AW31" s="56"/>
-      <c r="AX31" s="56"/>
-      <c r="AY31" s="56"/>
-      <c r="AZ31" s="56"/>
-      <c r="BA31" s="56"/>
-      <c r="BB31" s="56"/>
-      <c r="BC31" s="56"/>
-      <c r="BD31" s="56"/>
-      <c r="BE31" s="56"/>
-      <c r="BF31" s="56"/>
-      <c r="BG31" s="56"/>
-      <c r="BH31" s="56"/>
-      <c r="BI31" s="56"/>
-      <c r="BJ31" s="56"/>
-      <c r="BK31" s="56"/>
-      <c r="BL31" s="56"/>
-      <c r="BM31" s="56"/>
-      <c r="BN31" s="56"/>
-      <c r="BO31" s="56"/>
-      <c r="BP31" s="56"/>
-      <c r="BQ31" s="56"/>
-      <c r="BR31" s="56"/>
-      <c r="BS31" s="56"/>
-      <c r="BT31" s="56"/>
-      <c r="BU31" s="56"/>
-      <c r="BV31" s="56"/>
-      <c r="BW31" s="56"/>
-      <c r="BX31" s="56"/>
-      <c r="BY31" s="56"/>
-      <c r="BZ31" s="56"/>
-      <c r="CA31" s="56"/>
-      <c r="CB31" s="56"/>
-      <c r="CC31" s="56"/>
-      <c r="CD31" s="56"/>
-      <c r="CE31" s="56"/>
-      <c r="CF31" s="56"/>
-      <c r="CG31" s="56"/>
-      <c r="CH31" s="56"/>
-      <c r="CI31" s="56"/>
-      <c r="CJ31" s="56"/>
-      <c r="CK31" s="56"/>
-      <c r="CL31" s="56"/>
-      <c r="CM31" s="56"/>
-      <c r="CN31" s="56"/>
-      <c r="CO31" s="56"/>
-      <c r="CP31" s="56"/>
-      <c r="CQ31" s="56"/>
-      <c r="CR31" s="56"/>
-      <c r="CS31" s="56"/>
-      <c r="CT31" s="56"/>
-      <c r="CU31" s="56"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="48"/>
+      <c r="V31" s="48"/>
+      <c r="W31" s="48"/>
+      <c r="X31" s="48"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="48"/>
+      <c r="AA31" s="48"/>
+      <c r="AB31" s="48"/>
+      <c r="AC31" s="48"/>
+      <c r="AD31" s="48"/>
+      <c r="AE31" s="48"/>
+      <c r="AF31" s="48"/>
+      <c r="AG31" s="48"/>
+      <c r="AH31" s="48"/>
+      <c r="AI31" s="48"/>
+      <c r="AJ31" s="48"/>
+      <c r="AK31" s="48"/>
+      <c r="AL31" s="48"/>
+      <c r="AM31" s="48"/>
+      <c r="AN31" s="48"/>
+      <c r="AO31" s="48"/>
+      <c r="AP31" s="48"/>
+      <c r="AQ31" s="48"/>
+      <c r="AR31" s="48"/>
+      <c r="AS31" s="48"/>
+      <c r="AT31" s="48"/>
+      <c r="AU31" s="48"/>
+      <c r="AV31" s="48"/>
+      <c r="AW31" s="48"/>
+      <c r="AX31" s="48"/>
+      <c r="AY31" s="48"/>
+      <c r="AZ31" s="48"/>
+      <c r="BA31" s="48"/>
+      <c r="BB31" s="48"/>
+      <c r="BC31" s="48"/>
+      <c r="BD31" s="48"/>
+      <c r="BE31" s="48"/>
+      <c r="BF31" s="48"/>
+      <c r="BG31" s="48"/>
+      <c r="BH31" s="48"/>
+      <c r="BI31" s="48"/>
+      <c r="BJ31" s="48"/>
+      <c r="BK31" s="48"/>
+      <c r="BL31" s="48"/>
+      <c r="BM31" s="48"/>
+      <c r="BN31" s="48"/>
+      <c r="BO31" s="48"/>
+      <c r="BP31" s="48"/>
+      <c r="BQ31" s="48"/>
+      <c r="BR31" s="48"/>
+      <c r="BS31" s="48"/>
+      <c r="BT31" s="48"/>
+      <c r="BU31" s="48"/>
+      <c r="BV31" s="48"/>
+      <c r="BW31" s="48"/>
+      <c r="BX31" s="48"/>
+      <c r="BY31" s="48"/>
+      <c r="BZ31" s="48"/>
+      <c r="CA31" s="48"/>
+      <c r="CB31" s="48"/>
+      <c r="CC31" s="48"/>
+      <c r="CD31" s="48"/>
+      <c r="CE31" s="48"/>
+      <c r="CF31" s="48"/>
+      <c r="CG31" s="48"/>
+      <c r="CH31" s="48"/>
+      <c r="CI31" s="48"/>
+      <c r="CJ31" s="48"/>
+      <c r="CK31" s="48"/>
+      <c r="CL31" s="48"/>
+      <c r="CM31" s="48"/>
+      <c r="CN31" s="48"/>
+      <c r="CO31" s="48"/>
+      <c r="CP31" s="48"/>
+      <c r="CQ31" s="48"/>
+      <c r="CR31" s="48"/>
+      <c r="CS31" s="48"/>
+      <c r="CT31" s="48"/>
+      <c r="CU31" s="48"/>
     </row>
     <row r="32" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
@@ -4142,7 +4142,7 @@
         <v>8</v>
       </c>
       <c r="G33" s="30">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="H33" s="24" t="s">
         <v>77</v>
@@ -4217,7 +4217,7 @@
         <v>5</v>
       </c>
       <c r="G34" s="30">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="H34" s="24" t="s">
         <v>77</v>
@@ -6994,7 +6994,7 @@
         <v>14</v>
       </c>
       <c r="G70" s="30">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H70" s="24"/>
       <c r="I70" s="31"/>
@@ -7067,7 +7067,7 @@
         <v>9</v>
       </c>
       <c r="G71" s="30">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="H71" s="24"/>
       <c r="I71" s="31"/>
@@ -7697,21 +7697,22 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A13:CU13"/>
-    <mergeCell ref="B21:CU21"/>
-    <mergeCell ref="B26:CU26"/>
-    <mergeCell ref="A31:CU31"/>
-    <mergeCell ref="A42:CU42"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="AD5:AH5"/>
-    <mergeCell ref="AD6:AH6"/>
-    <mergeCell ref="B2:G4"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="O6:S6"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A57:CU57"/>
+    <mergeCell ref="B49:CU49"/>
+    <mergeCell ref="A52:CU52"/>
+    <mergeCell ref="CQ5:CU5"/>
+    <mergeCell ref="CQ6:CU6"/>
+    <mergeCell ref="CL5:CP5"/>
+    <mergeCell ref="CL6:CP6"/>
+    <mergeCell ref="AX5:BB5"/>
+    <mergeCell ref="AX6:BB6"/>
+    <mergeCell ref="AI5:AM5"/>
+    <mergeCell ref="AI6:AM6"/>
+    <mergeCell ref="AN5:AR5"/>
+    <mergeCell ref="AN6:AR6"/>
+    <mergeCell ref="AS5:AW5"/>
+    <mergeCell ref="AS6:AW6"/>
+    <mergeCell ref="Y5:AC5"/>
     <mergeCell ref="BE2:BW2"/>
     <mergeCell ref="BE3:BW3"/>
     <mergeCell ref="CB5:CF5"/>
@@ -7728,22 +7729,21 @@
     <mergeCell ref="BC6:BG6"/>
     <mergeCell ref="BH5:BL5"/>
     <mergeCell ref="BH6:BL6"/>
-    <mergeCell ref="A57:CU57"/>
-    <mergeCell ref="B49:CU49"/>
-    <mergeCell ref="A52:CU52"/>
-    <mergeCell ref="CQ5:CU5"/>
-    <mergeCell ref="CQ6:CU6"/>
-    <mergeCell ref="CL5:CP5"/>
-    <mergeCell ref="CL6:CP6"/>
-    <mergeCell ref="AX5:BB5"/>
-    <mergeCell ref="AX6:BB6"/>
-    <mergeCell ref="AI5:AM5"/>
-    <mergeCell ref="AI6:AM6"/>
-    <mergeCell ref="AN5:AR5"/>
-    <mergeCell ref="AN6:AR6"/>
-    <mergeCell ref="AS5:AW5"/>
-    <mergeCell ref="AS6:AW6"/>
-    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="AD6:AH6"/>
+    <mergeCell ref="B2:G4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="O6:S6"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A13:CU13"/>
+    <mergeCell ref="B21:CU21"/>
+    <mergeCell ref="B26:CU26"/>
+    <mergeCell ref="A31:CU31"/>
+    <mergeCell ref="A42:CU42"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J53:CU56 J50:CU51 J32:CU41 J43:CU48 J58:CU59 J75:CU75">
     <cfRule type="expression" dxfId="25" priority="84">

</xml_diff>

<commit_message>
finalizado SOLIDWORKS.. MEDO DE NAO CONSEGUIR IMPRIMIR
</commit_message>
<xml_diff>
--- a/LaTeX Project/Documentos/Gantt.xlsx
+++ b/LaTeX Project/Documentos/Gantt.xlsx
@@ -1016,12 +1016,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1040,10 +1034,16 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1810,8 +1810,8 @@
   </sheetPr>
   <dimension ref="A2:CU84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="CA58" sqref="AZ58:CA58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1836,47 +1836,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="24" t="s">
         <v>78</v>
       </c>
       <c r="I2" s="16"/>
-      <c r="BE2" s="56" t="s">
+      <c r="BE2" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" s="56"/>
-      <c r="BG2" s="56"/>
-      <c r="BH2" s="56"/>
-      <c r="BI2" s="56"/>
-      <c r="BJ2" s="56"/>
-      <c r="BK2" s="56"/>
-      <c r="BL2" s="56"/>
-      <c r="BM2" s="56"/>
-      <c r="BN2" s="56"/>
-      <c r="BO2" s="56"/>
-      <c r="BP2" s="56"/>
-      <c r="BQ2" s="56"/>
-      <c r="BR2" s="56"/>
-      <c r="BS2" s="56"/>
-      <c r="BT2" s="56"/>
-      <c r="BU2" s="56"/>
-      <c r="BV2" s="56"/>
-      <c r="BW2" s="56"/>
+      <c r="BF2" s="53"/>
+      <c r="BG2" s="53"/>
+      <c r="BH2" s="53"/>
+      <c r="BI2" s="53"/>
+      <c r="BJ2" s="53"/>
+      <c r="BK2" s="53"/>
+      <c r="BL2" s="53"/>
+      <c r="BM2" s="53"/>
+      <c r="BN2" s="53"/>
+      <c r="BO2" s="53"/>
+      <c r="BP2" s="53"/>
+      <c r="BQ2" s="53"/>
+      <c r="BR2" s="53"/>
+      <c r="BS2" s="53"/>
+      <c r="BT2" s="53"/>
+      <c r="BU2" s="53"/>
+      <c r="BV2" s="53"/>
+      <c r="BW2" s="53"/>
     </row>
     <row r="3" spans="1:99" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="24" t="s">
         <v>79</v>
       </c>
@@ -1925,35 +1925,35 @@
       <c r="AQ3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="BE3" s="56" t="s">
+      <c r="BE3" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="BF3" s="56"/>
-      <c r="BG3" s="56"/>
-      <c r="BH3" s="56"/>
-      <c r="BI3" s="56"/>
-      <c r="BJ3" s="56"/>
-      <c r="BK3" s="56"/>
-      <c r="BL3" s="56"/>
-      <c r="BM3" s="56"/>
-      <c r="BN3" s="56"/>
-      <c r="BO3" s="56"/>
-      <c r="BP3" s="56"/>
-      <c r="BQ3" s="56"/>
-      <c r="BR3" s="56"/>
-      <c r="BS3" s="56"/>
-      <c r="BT3" s="56"/>
-      <c r="BU3" s="56"/>
-      <c r="BV3" s="56"/>
-      <c r="BW3" s="56"/>
+      <c r="BF3" s="53"/>
+      <c r="BG3" s="53"/>
+      <c r="BH3" s="53"/>
+      <c r="BI3" s="53"/>
+      <c r="BJ3" s="53"/>
+      <c r="BK3" s="53"/>
+      <c r="BL3" s="53"/>
+      <c r="BM3" s="53"/>
+      <c r="BN3" s="53"/>
+      <c r="BO3" s="53"/>
+      <c r="BP3" s="53"/>
+      <c r="BQ3" s="53"/>
+      <c r="BR3" s="53"/>
+      <c r="BS3" s="53"/>
+      <c r="BT3" s="53"/>
+      <c r="BU3" s="53"/>
+      <c r="BV3" s="53"/>
+      <c r="BW3" s="53"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="24" t="s">
         <v>80</v>
       </c>
@@ -1984,132 +1984,132 @@
       <c r="AY4" s="19"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="J5" s="52" t="s">
+      <c r="J5" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="49" t="s">
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="52" t="s">
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
-      <c r="W5" s="53"/>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="49" t="s">
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="52"/>
+      <c r="Y5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="50"/>
-      <c r="AC5" s="51"/>
-      <c r="AD5" s="52" t="s">
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="48"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="53"/>
-      <c r="AF5" s="53"/>
-      <c r="AG5" s="53"/>
-      <c r="AH5" s="54"/>
-      <c r="AI5" s="49" t="s">
+      <c r="AE5" s="51"/>
+      <c r="AF5" s="51"/>
+      <c r="AG5" s="51"/>
+      <c r="AH5" s="52"/>
+      <c r="AI5" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="AJ5" s="50"/>
-      <c r="AK5" s="50"/>
-      <c r="AL5" s="50"/>
-      <c r="AM5" s="51"/>
-      <c r="AN5" s="52" t="s">
+      <c r="AJ5" s="48"/>
+      <c r="AK5" s="48"/>
+      <c r="AL5" s="48"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="53"/>
-      <c r="AP5" s="53"/>
-      <c r="AQ5" s="53"/>
-      <c r="AR5" s="54"/>
-      <c r="AS5" s="49" t="s">
+      <c r="AO5" s="51"/>
+      <c r="AP5" s="51"/>
+      <c r="AQ5" s="51"/>
+      <c r="AR5" s="52"/>
+      <c r="AS5" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="AT5" s="50"/>
-      <c r="AU5" s="50"/>
-      <c r="AV5" s="50"/>
-      <c r="AW5" s="51"/>
-      <c r="AX5" s="52" t="s">
+      <c r="AT5" s="48"/>
+      <c r="AU5" s="48"/>
+      <c r="AV5" s="48"/>
+      <c r="AW5" s="49"/>
+      <c r="AX5" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="AY5" s="53"/>
-      <c r="AZ5" s="53"/>
-      <c r="BA5" s="53"/>
-      <c r="BB5" s="54"/>
-      <c r="BC5" s="49" t="s">
+      <c r="AY5" s="51"/>
+      <c r="AZ5" s="51"/>
+      <c r="BA5" s="51"/>
+      <c r="BB5" s="52"/>
+      <c r="BC5" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="BD5" s="50"/>
-      <c r="BE5" s="50"/>
-      <c r="BF5" s="50"/>
-      <c r="BG5" s="51"/>
-      <c r="BH5" s="52" t="s">
+      <c r="BD5" s="48"/>
+      <c r="BE5" s="48"/>
+      <c r="BF5" s="48"/>
+      <c r="BG5" s="49"/>
+      <c r="BH5" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="BI5" s="53"/>
-      <c r="BJ5" s="53"/>
-      <c r="BK5" s="53"/>
-      <c r="BL5" s="54"/>
-      <c r="BM5" s="49" t="s">
+      <c r="BI5" s="51"/>
+      <c r="BJ5" s="51"/>
+      <c r="BK5" s="51"/>
+      <c r="BL5" s="52"/>
+      <c r="BM5" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="BN5" s="50"/>
-      <c r="BO5" s="50"/>
-      <c r="BP5" s="50"/>
-      <c r="BQ5" s="51"/>
-      <c r="BR5" s="52" t="s">
+      <c r="BN5" s="48"/>
+      <c r="BO5" s="48"/>
+      <c r="BP5" s="48"/>
+      <c r="BQ5" s="49"/>
+      <c r="BR5" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="BS5" s="53"/>
-      <c r="BT5" s="53"/>
-      <c r="BU5" s="53"/>
-      <c r="BV5" s="54"/>
-      <c r="BW5" s="49" t="s">
+      <c r="BS5" s="51"/>
+      <c r="BT5" s="51"/>
+      <c r="BU5" s="51"/>
+      <c r="BV5" s="52"/>
+      <c r="BW5" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="BX5" s="50"/>
-      <c r="BY5" s="50"/>
-      <c r="BZ5" s="50"/>
-      <c r="CA5" s="51"/>
-      <c r="CB5" s="52" t="s">
+      <c r="BX5" s="48"/>
+      <c r="BY5" s="48"/>
+      <c r="BZ5" s="48"/>
+      <c r="CA5" s="49"/>
+      <c r="CB5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="CC5" s="53"/>
-      <c r="CD5" s="53"/>
-      <c r="CE5" s="53"/>
-      <c r="CF5" s="54"/>
-      <c r="CG5" s="49" t="s">
+      <c r="CC5" s="51"/>
+      <c r="CD5" s="51"/>
+      <c r="CE5" s="51"/>
+      <c r="CF5" s="52"/>
+      <c r="CG5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="CH5" s="50"/>
-      <c r="CI5" s="50"/>
-      <c r="CJ5" s="50"/>
-      <c r="CK5" s="51"/>
-      <c r="CL5" s="52" t="s">
+      <c r="CH5" s="48"/>
+      <c r="CI5" s="48"/>
+      <c r="CJ5" s="48"/>
+      <c r="CK5" s="49"/>
+      <c r="CL5" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="CM5" s="53"/>
-      <c r="CN5" s="53"/>
-      <c r="CO5" s="53"/>
-      <c r="CP5" s="54"/>
-      <c r="CQ5" s="49" t="s">
+      <c r="CM5" s="51"/>
+      <c r="CN5" s="51"/>
+      <c r="CO5" s="51"/>
+      <c r="CP5" s="52"/>
+      <c r="CQ5" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="CR5" s="50"/>
-      <c r="CS5" s="50"/>
-      <c r="CT5" s="50"/>
-      <c r="CU5" s="51"/>
+      <c r="CR5" s="48"/>
+      <c r="CS5" s="48"/>
+      <c r="CT5" s="48"/>
+      <c r="CU5" s="49"/>
     </row>
     <row r="6" spans="1:99" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -2132,132 +2132,132 @@
         <v>75</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="49" t="s">
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="51"/>
-      <c r="T6" s="52" t="s">
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
-      <c r="W6" s="53"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="49" t="s">
+      <c r="U6" s="51"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="51"/>
+      <c r="X6" s="52"/>
+      <c r="Y6" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="Z6" s="50"/>
-      <c r="AA6" s="50"/>
-      <c r="AB6" s="50"/>
-      <c r="AC6" s="51"/>
-      <c r="AD6" s="52" t="s">
+      <c r="Z6" s="48"/>
+      <c r="AA6" s="48"/>
+      <c r="AB6" s="48"/>
+      <c r="AC6" s="49"/>
+      <c r="AD6" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="53"/>
-      <c r="AF6" s="53"/>
-      <c r="AG6" s="53"/>
-      <c r="AH6" s="54"/>
-      <c r="AI6" s="49" t="s">
+      <c r="AE6" s="51"/>
+      <c r="AF6" s="51"/>
+      <c r="AG6" s="51"/>
+      <c r="AH6" s="52"/>
+      <c r="AI6" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="50"/>
-      <c r="AK6" s="50"/>
-      <c r="AL6" s="50"/>
-      <c r="AM6" s="51"/>
-      <c r="AN6" s="52" t="s">
+      <c r="AJ6" s="48"/>
+      <c r="AK6" s="48"/>
+      <c r="AL6" s="48"/>
+      <c r="AM6" s="49"/>
+      <c r="AN6" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" s="53"/>
-      <c r="AP6" s="53"/>
-      <c r="AQ6" s="53"/>
-      <c r="AR6" s="54"/>
-      <c r="AS6" s="49" t="s">
+      <c r="AO6" s="51"/>
+      <c r="AP6" s="51"/>
+      <c r="AQ6" s="51"/>
+      <c r="AR6" s="52"/>
+      <c r="AS6" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="AT6" s="50"/>
-      <c r="AU6" s="50"/>
-      <c r="AV6" s="50"/>
-      <c r="AW6" s="51"/>
-      <c r="AX6" s="52" t="s">
+      <c r="AT6" s="48"/>
+      <c r="AU6" s="48"/>
+      <c r="AV6" s="48"/>
+      <c r="AW6" s="49"/>
+      <c r="AX6" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="AY6" s="53"/>
-      <c r="AZ6" s="53"/>
-      <c r="BA6" s="53"/>
-      <c r="BB6" s="54"/>
-      <c r="BC6" s="49" t="s">
+      <c r="AY6" s="51"/>
+      <c r="AZ6" s="51"/>
+      <c r="BA6" s="51"/>
+      <c r="BB6" s="52"/>
+      <c r="BC6" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="BD6" s="50"/>
-      <c r="BE6" s="50"/>
-      <c r="BF6" s="50"/>
-      <c r="BG6" s="51"/>
-      <c r="BH6" s="52" t="s">
+      <c r="BD6" s="48"/>
+      <c r="BE6" s="48"/>
+      <c r="BF6" s="48"/>
+      <c r="BG6" s="49"/>
+      <c r="BH6" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="BI6" s="53"/>
-      <c r="BJ6" s="53"/>
-      <c r="BK6" s="53"/>
-      <c r="BL6" s="54"/>
-      <c r="BM6" s="49" t="s">
+      <c r="BI6" s="51"/>
+      <c r="BJ6" s="51"/>
+      <c r="BK6" s="51"/>
+      <c r="BL6" s="52"/>
+      <c r="BM6" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="BN6" s="50"/>
-      <c r="BO6" s="50"/>
-      <c r="BP6" s="50"/>
-      <c r="BQ6" s="51"/>
-      <c r="BR6" s="52" t="s">
+      <c r="BN6" s="48"/>
+      <c r="BO6" s="48"/>
+      <c r="BP6" s="48"/>
+      <c r="BQ6" s="49"/>
+      <c r="BR6" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="BS6" s="53"/>
-      <c r="BT6" s="53"/>
-      <c r="BU6" s="53"/>
-      <c r="BV6" s="54"/>
-      <c r="BW6" s="49" t="s">
+      <c r="BS6" s="51"/>
+      <c r="BT6" s="51"/>
+      <c r="BU6" s="51"/>
+      <c r="BV6" s="52"/>
+      <c r="BW6" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="BX6" s="50"/>
-      <c r="BY6" s="50"/>
-      <c r="BZ6" s="50"/>
-      <c r="CA6" s="51"/>
-      <c r="CB6" s="52" t="s">
+      <c r="BX6" s="48"/>
+      <c r="BY6" s="48"/>
+      <c r="BZ6" s="48"/>
+      <c r="CA6" s="49"/>
+      <c r="CB6" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="CC6" s="53"/>
-      <c r="CD6" s="53"/>
-      <c r="CE6" s="53"/>
-      <c r="CF6" s="54"/>
-      <c r="CG6" s="49" t="s">
+      <c r="CC6" s="51"/>
+      <c r="CD6" s="51"/>
+      <c r="CE6" s="51"/>
+      <c r="CF6" s="52"/>
+      <c r="CG6" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="CH6" s="50"/>
-      <c r="CI6" s="50"/>
-      <c r="CJ6" s="50"/>
-      <c r="CK6" s="51"/>
-      <c r="CL6" s="52" t="s">
+      <c r="CH6" s="48"/>
+      <c r="CI6" s="48"/>
+      <c r="CJ6" s="48"/>
+      <c r="CK6" s="49"/>
+      <c r="CL6" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="CM6" s="53"/>
-      <c r="CN6" s="53"/>
-      <c r="CO6" s="53"/>
-      <c r="CP6" s="54"/>
-      <c r="CQ6" s="49" t="s">
+      <c r="CM6" s="51"/>
+      <c r="CN6" s="51"/>
+      <c r="CO6" s="51"/>
+      <c r="CP6" s="52"/>
+      <c r="CQ6" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="CR6" s="50"/>
-      <c r="CS6" s="50"/>
-      <c r="CT6" s="50"/>
-      <c r="CU6" s="51"/>
+      <c r="CR6" s="48"/>
+      <c r="CS6" s="48"/>
+      <c r="CT6" s="48"/>
+      <c r="CU6" s="49"/>
     </row>
     <row r="7" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -3162,104 +3162,104 @@
       <c r="AC20" s="31"/>
     </row>
     <row r="21" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="47"/>
-      <c r="V21" s="47"/>
-      <c r="W21" s="47"/>
-      <c r="X21" s="47"/>
-      <c r="Y21" s="47"/>
-      <c r="Z21" s="47"/>
-      <c r="AA21" s="47"/>
-      <c r="AB21" s="47"/>
-      <c r="AC21" s="47"/>
-      <c r="AD21" s="47"/>
-      <c r="AE21" s="47"/>
-      <c r="AF21" s="47"/>
-      <c r="AG21" s="47"/>
-      <c r="AH21" s="47"/>
-      <c r="AI21" s="47"/>
-      <c r="AJ21" s="47"/>
-      <c r="AK21" s="47"/>
-      <c r="AL21" s="47"/>
-      <c r="AM21" s="47"/>
-      <c r="AN21" s="47"/>
-      <c r="AO21" s="47"/>
-      <c r="AP21" s="47"/>
-      <c r="AQ21" s="47"/>
-      <c r="AR21" s="47"/>
-      <c r="AS21" s="47"/>
-      <c r="AT21" s="47"/>
-      <c r="AU21" s="47"/>
-      <c r="AV21" s="47"/>
-      <c r="AW21" s="47"/>
-      <c r="AX21" s="47"/>
-      <c r="AY21" s="47"/>
-      <c r="AZ21" s="47"/>
-      <c r="BA21" s="47"/>
-      <c r="BB21" s="47"/>
-      <c r="BC21" s="47"/>
-      <c r="BD21" s="47"/>
-      <c r="BE21" s="47"/>
-      <c r="BF21" s="47"/>
-      <c r="BG21" s="47"/>
-      <c r="BH21" s="47"/>
-      <c r="BI21" s="47"/>
-      <c r="BJ21" s="47"/>
-      <c r="BK21" s="47"/>
-      <c r="BL21" s="47"/>
-      <c r="BM21" s="47"/>
-      <c r="BN21" s="47"/>
-      <c r="BO21" s="47"/>
-      <c r="BP21" s="47"/>
-      <c r="BQ21" s="47"/>
-      <c r="BR21" s="47"/>
-      <c r="BS21" s="47"/>
-      <c r="BT21" s="47"/>
-      <c r="BU21" s="47"/>
-      <c r="BV21" s="47"/>
-      <c r="BW21" s="47"/>
-      <c r="BX21" s="47"/>
-      <c r="BY21" s="47"/>
-      <c r="BZ21" s="47"/>
-      <c r="CA21" s="47"/>
-      <c r="CB21" s="47"/>
-      <c r="CC21" s="47"/>
-      <c r="CD21" s="47"/>
-      <c r="CE21" s="47"/>
-      <c r="CF21" s="47"/>
-      <c r="CG21" s="47"/>
-      <c r="CH21" s="47"/>
-      <c r="CI21" s="47"/>
-      <c r="CJ21" s="47"/>
-      <c r="CK21" s="47"/>
-      <c r="CL21" s="47"/>
-      <c r="CM21" s="47"/>
-      <c r="CN21" s="47"/>
-      <c r="CO21" s="47"/>
-      <c r="CP21" s="47"/>
-      <c r="CQ21" s="47"/>
-      <c r="CR21" s="47"/>
-      <c r="CS21" s="47"/>
-      <c r="CT21" s="47"/>
-      <c r="CU21" s="47"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="55"/>
+      <c r="T21" s="55"/>
+      <c r="U21" s="55"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="55"/>
+      <c r="X21" s="55"/>
+      <c r="Y21" s="55"/>
+      <c r="Z21" s="55"/>
+      <c r="AA21" s="55"/>
+      <c r="AB21" s="55"/>
+      <c r="AC21" s="55"/>
+      <c r="AD21" s="55"/>
+      <c r="AE21" s="55"/>
+      <c r="AF21" s="55"/>
+      <c r="AG21" s="55"/>
+      <c r="AH21" s="55"/>
+      <c r="AI21" s="55"/>
+      <c r="AJ21" s="55"/>
+      <c r="AK21" s="55"/>
+      <c r="AL21" s="55"/>
+      <c r="AM21" s="55"/>
+      <c r="AN21" s="55"/>
+      <c r="AO21" s="55"/>
+      <c r="AP21" s="55"/>
+      <c r="AQ21" s="55"/>
+      <c r="AR21" s="55"/>
+      <c r="AS21" s="55"/>
+      <c r="AT21" s="55"/>
+      <c r="AU21" s="55"/>
+      <c r="AV21" s="55"/>
+      <c r="AW21" s="55"/>
+      <c r="AX21" s="55"/>
+      <c r="AY21" s="55"/>
+      <c r="AZ21" s="55"/>
+      <c r="BA21" s="55"/>
+      <c r="BB21" s="55"/>
+      <c r="BC21" s="55"/>
+      <c r="BD21" s="55"/>
+      <c r="BE21" s="55"/>
+      <c r="BF21" s="55"/>
+      <c r="BG21" s="55"/>
+      <c r="BH21" s="55"/>
+      <c r="BI21" s="55"/>
+      <c r="BJ21" s="55"/>
+      <c r="BK21" s="55"/>
+      <c r="BL21" s="55"/>
+      <c r="BM21" s="55"/>
+      <c r="BN21" s="55"/>
+      <c r="BO21" s="55"/>
+      <c r="BP21" s="55"/>
+      <c r="BQ21" s="55"/>
+      <c r="BR21" s="55"/>
+      <c r="BS21" s="55"/>
+      <c r="BT21" s="55"/>
+      <c r="BU21" s="55"/>
+      <c r="BV21" s="55"/>
+      <c r="BW21" s="55"/>
+      <c r="BX21" s="55"/>
+      <c r="BY21" s="55"/>
+      <c r="BZ21" s="55"/>
+      <c r="CA21" s="55"/>
+      <c r="CB21" s="55"/>
+      <c r="CC21" s="55"/>
+      <c r="CD21" s="55"/>
+      <c r="CE21" s="55"/>
+      <c r="CF21" s="55"/>
+      <c r="CG21" s="55"/>
+      <c r="CH21" s="55"/>
+      <c r="CI21" s="55"/>
+      <c r="CJ21" s="55"/>
+      <c r="CK21" s="55"/>
+      <c r="CL21" s="55"/>
+      <c r="CM21" s="55"/>
+      <c r="CN21" s="55"/>
+      <c r="CO21" s="55"/>
+      <c r="CP21" s="55"/>
+      <c r="CQ21" s="55"/>
+      <c r="CR21" s="55"/>
+      <c r="CS21" s="55"/>
+      <c r="CT21" s="55"/>
+      <c r="CU21" s="55"/>
     </row>
     <row r="22" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
@@ -3554,104 +3554,104 @@
       <c r="CU25" s="35"/>
     </row>
     <row r="26" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="47"/>
-      <c r="Q26" s="47"/>
-      <c r="R26" s="47"/>
-      <c r="S26" s="47"/>
-      <c r="T26" s="47"/>
-      <c r="U26" s="47"/>
-      <c r="V26" s="47"/>
-      <c r="W26" s="47"/>
-      <c r="X26" s="47"/>
-      <c r="Y26" s="47"/>
-      <c r="Z26" s="47"/>
-      <c r="AA26" s="47"/>
-      <c r="AB26" s="47"/>
-      <c r="AC26" s="47"/>
-      <c r="AD26" s="47"/>
-      <c r="AE26" s="47"/>
-      <c r="AF26" s="47"/>
-      <c r="AG26" s="47"/>
-      <c r="AH26" s="47"/>
-      <c r="AI26" s="47"/>
-      <c r="AJ26" s="47"/>
-      <c r="AK26" s="47"/>
-      <c r="AL26" s="47"/>
-      <c r="AM26" s="47"/>
-      <c r="AN26" s="47"/>
-      <c r="AO26" s="47"/>
-      <c r="AP26" s="47"/>
-      <c r="AQ26" s="47"/>
-      <c r="AR26" s="47"/>
-      <c r="AS26" s="47"/>
-      <c r="AT26" s="47"/>
-      <c r="AU26" s="47"/>
-      <c r="AV26" s="47"/>
-      <c r="AW26" s="47"/>
-      <c r="AX26" s="47"/>
-      <c r="AY26" s="47"/>
-      <c r="AZ26" s="47"/>
-      <c r="BA26" s="47"/>
-      <c r="BB26" s="47"/>
-      <c r="BC26" s="47"/>
-      <c r="BD26" s="47"/>
-      <c r="BE26" s="47"/>
-      <c r="BF26" s="47"/>
-      <c r="BG26" s="47"/>
-      <c r="BH26" s="47"/>
-      <c r="BI26" s="47"/>
-      <c r="BJ26" s="47"/>
-      <c r="BK26" s="47"/>
-      <c r="BL26" s="47"/>
-      <c r="BM26" s="47"/>
-      <c r="BN26" s="47"/>
-      <c r="BO26" s="47"/>
-      <c r="BP26" s="47"/>
-      <c r="BQ26" s="47"/>
-      <c r="BR26" s="47"/>
-      <c r="BS26" s="47"/>
-      <c r="BT26" s="47"/>
-      <c r="BU26" s="47"/>
-      <c r="BV26" s="47"/>
-      <c r="BW26" s="47"/>
-      <c r="BX26" s="47"/>
-      <c r="BY26" s="47"/>
-      <c r="BZ26" s="47"/>
-      <c r="CA26" s="47"/>
-      <c r="CB26" s="47"/>
-      <c r="CC26" s="47"/>
-      <c r="CD26" s="47"/>
-      <c r="CE26" s="47"/>
-      <c r="CF26" s="47"/>
-      <c r="CG26" s="47"/>
-      <c r="CH26" s="47"/>
-      <c r="CI26" s="47"/>
-      <c r="CJ26" s="47"/>
-      <c r="CK26" s="47"/>
-      <c r="CL26" s="47"/>
-      <c r="CM26" s="47"/>
-      <c r="CN26" s="47"/>
-      <c r="CO26" s="47"/>
-      <c r="CP26" s="47"/>
-      <c r="CQ26" s="47"/>
-      <c r="CR26" s="47"/>
-      <c r="CS26" s="47"/>
-      <c r="CT26" s="47"/>
-      <c r="CU26" s="47"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
+      <c r="V26" s="55"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="55"/>
+      <c r="Y26" s="55"/>
+      <c r="Z26" s="55"/>
+      <c r="AA26" s="55"/>
+      <c r="AB26" s="55"/>
+      <c r="AC26" s="55"/>
+      <c r="AD26" s="55"/>
+      <c r="AE26" s="55"/>
+      <c r="AF26" s="55"/>
+      <c r="AG26" s="55"/>
+      <c r="AH26" s="55"/>
+      <c r="AI26" s="55"/>
+      <c r="AJ26" s="55"/>
+      <c r="AK26" s="55"/>
+      <c r="AL26" s="55"/>
+      <c r="AM26" s="55"/>
+      <c r="AN26" s="55"/>
+      <c r="AO26" s="55"/>
+      <c r="AP26" s="55"/>
+      <c r="AQ26" s="55"/>
+      <c r="AR26" s="55"/>
+      <c r="AS26" s="55"/>
+      <c r="AT26" s="55"/>
+      <c r="AU26" s="55"/>
+      <c r="AV26" s="55"/>
+      <c r="AW26" s="55"/>
+      <c r="AX26" s="55"/>
+      <c r="AY26" s="55"/>
+      <c r="AZ26" s="55"/>
+      <c r="BA26" s="55"/>
+      <c r="BB26" s="55"/>
+      <c r="BC26" s="55"/>
+      <c r="BD26" s="55"/>
+      <c r="BE26" s="55"/>
+      <c r="BF26" s="55"/>
+      <c r="BG26" s="55"/>
+      <c r="BH26" s="55"/>
+      <c r="BI26" s="55"/>
+      <c r="BJ26" s="55"/>
+      <c r="BK26" s="55"/>
+      <c r="BL26" s="55"/>
+      <c r="BM26" s="55"/>
+      <c r="BN26" s="55"/>
+      <c r="BO26" s="55"/>
+      <c r="BP26" s="55"/>
+      <c r="BQ26" s="55"/>
+      <c r="BR26" s="55"/>
+      <c r="BS26" s="55"/>
+      <c r="BT26" s="55"/>
+      <c r="BU26" s="55"/>
+      <c r="BV26" s="55"/>
+      <c r="BW26" s="55"/>
+      <c r="BX26" s="55"/>
+      <c r="BY26" s="55"/>
+      <c r="BZ26" s="55"/>
+      <c r="CA26" s="55"/>
+      <c r="CB26" s="55"/>
+      <c r="CC26" s="55"/>
+      <c r="CD26" s="55"/>
+      <c r="CE26" s="55"/>
+      <c r="CF26" s="55"/>
+      <c r="CG26" s="55"/>
+      <c r="CH26" s="55"/>
+      <c r="CI26" s="55"/>
+      <c r="CJ26" s="55"/>
+      <c r="CK26" s="55"/>
+      <c r="CL26" s="55"/>
+      <c r="CM26" s="55"/>
+      <c r="CN26" s="55"/>
+      <c r="CO26" s="55"/>
+      <c r="CP26" s="55"/>
+      <c r="CQ26" s="55"/>
+      <c r="CR26" s="55"/>
+      <c r="CS26" s="55"/>
+      <c r="CT26" s="55"/>
+      <c r="CU26" s="55"/>
     </row>
     <row r="27" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
@@ -3952,105 +3952,105 @@
       <c r="CU30" s="35"/>
     </row>
     <row r="31" spans="1:99" s="45" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-      <c r="R31" s="48"/>
-      <c r="S31" s="48"/>
-      <c r="T31" s="48"/>
-      <c r="U31" s="48"/>
-      <c r="V31" s="48"/>
-      <c r="W31" s="48"/>
-      <c r="X31" s="48"/>
-      <c r="Y31" s="48"/>
-      <c r="Z31" s="48"/>
-      <c r="AA31" s="48"/>
-      <c r="AB31" s="48"/>
-      <c r="AC31" s="48"/>
-      <c r="AD31" s="48"/>
-      <c r="AE31" s="48"/>
-      <c r="AF31" s="48"/>
-      <c r="AG31" s="48"/>
-      <c r="AH31" s="48"/>
-      <c r="AI31" s="48"/>
-      <c r="AJ31" s="48"/>
-      <c r="AK31" s="48"/>
-      <c r="AL31" s="48"/>
-      <c r="AM31" s="48"/>
-      <c r="AN31" s="48"/>
-      <c r="AO31" s="48"/>
-      <c r="AP31" s="48"/>
-      <c r="AQ31" s="48"/>
-      <c r="AR31" s="48"/>
-      <c r="AS31" s="48"/>
-      <c r="AT31" s="48"/>
-      <c r="AU31" s="48"/>
-      <c r="AV31" s="48"/>
-      <c r="AW31" s="48"/>
-      <c r="AX31" s="48"/>
-      <c r="AY31" s="48"/>
-      <c r="AZ31" s="48"/>
-      <c r="BA31" s="48"/>
-      <c r="BB31" s="48"/>
-      <c r="BC31" s="48"/>
-      <c r="BD31" s="48"/>
-      <c r="BE31" s="48"/>
-      <c r="BF31" s="48"/>
-      <c r="BG31" s="48"/>
-      <c r="BH31" s="48"/>
-      <c r="BI31" s="48"/>
-      <c r="BJ31" s="48"/>
-      <c r="BK31" s="48"/>
-      <c r="BL31" s="48"/>
-      <c r="BM31" s="48"/>
-      <c r="BN31" s="48"/>
-      <c r="BO31" s="48"/>
-      <c r="BP31" s="48"/>
-      <c r="BQ31" s="48"/>
-      <c r="BR31" s="48"/>
-      <c r="BS31" s="48"/>
-      <c r="BT31" s="48"/>
-      <c r="BU31" s="48"/>
-      <c r="BV31" s="48"/>
-      <c r="BW31" s="48"/>
-      <c r="BX31" s="48"/>
-      <c r="BY31" s="48"/>
-      <c r="BZ31" s="48"/>
-      <c r="CA31" s="48"/>
-      <c r="CB31" s="48"/>
-      <c r="CC31" s="48"/>
-      <c r="CD31" s="48"/>
-      <c r="CE31" s="48"/>
-      <c r="CF31" s="48"/>
-      <c r="CG31" s="48"/>
-      <c r="CH31" s="48"/>
-      <c r="CI31" s="48"/>
-      <c r="CJ31" s="48"/>
-      <c r="CK31" s="48"/>
-      <c r="CL31" s="48"/>
-      <c r="CM31" s="48"/>
-      <c r="CN31" s="48"/>
-      <c r="CO31" s="48"/>
-      <c r="CP31" s="48"/>
-      <c r="CQ31" s="48"/>
-      <c r="CR31" s="48"/>
-      <c r="CS31" s="48"/>
-      <c r="CT31" s="48"/>
-      <c r="CU31" s="48"/>
+      <c r="A31" s="56"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
+      <c r="S31" s="56"/>
+      <c r="T31" s="56"/>
+      <c r="U31" s="56"/>
+      <c r="V31" s="56"/>
+      <c r="W31" s="56"/>
+      <c r="X31" s="56"/>
+      <c r="Y31" s="56"/>
+      <c r="Z31" s="56"/>
+      <c r="AA31" s="56"/>
+      <c r="AB31" s="56"/>
+      <c r="AC31" s="56"/>
+      <c r="AD31" s="56"/>
+      <c r="AE31" s="56"/>
+      <c r="AF31" s="56"/>
+      <c r="AG31" s="56"/>
+      <c r="AH31" s="56"/>
+      <c r="AI31" s="56"/>
+      <c r="AJ31" s="56"/>
+      <c r="AK31" s="56"/>
+      <c r="AL31" s="56"/>
+      <c r="AM31" s="56"/>
+      <c r="AN31" s="56"/>
+      <c r="AO31" s="56"/>
+      <c r="AP31" s="56"/>
+      <c r="AQ31" s="56"/>
+      <c r="AR31" s="56"/>
+      <c r="AS31" s="56"/>
+      <c r="AT31" s="56"/>
+      <c r="AU31" s="56"/>
+      <c r="AV31" s="56"/>
+      <c r="AW31" s="56"/>
+      <c r="AX31" s="56"/>
+      <c r="AY31" s="56"/>
+      <c r="AZ31" s="56"/>
+      <c r="BA31" s="56"/>
+      <c r="BB31" s="56"/>
+      <c r="BC31" s="56"/>
+      <c r="BD31" s="56"/>
+      <c r="BE31" s="56"/>
+      <c r="BF31" s="56"/>
+      <c r="BG31" s="56"/>
+      <c r="BH31" s="56"/>
+      <c r="BI31" s="56"/>
+      <c r="BJ31" s="56"/>
+      <c r="BK31" s="56"/>
+      <c r="BL31" s="56"/>
+      <c r="BM31" s="56"/>
+      <c r="BN31" s="56"/>
+      <c r="BO31" s="56"/>
+      <c r="BP31" s="56"/>
+      <c r="BQ31" s="56"/>
+      <c r="BR31" s="56"/>
+      <c r="BS31" s="56"/>
+      <c r="BT31" s="56"/>
+      <c r="BU31" s="56"/>
+      <c r="BV31" s="56"/>
+      <c r="BW31" s="56"/>
+      <c r="BX31" s="56"/>
+      <c r="BY31" s="56"/>
+      <c r="BZ31" s="56"/>
+      <c r="CA31" s="56"/>
+      <c r="CB31" s="56"/>
+      <c r="CC31" s="56"/>
+      <c r="CD31" s="56"/>
+      <c r="CE31" s="56"/>
+      <c r="CF31" s="56"/>
+      <c r="CG31" s="56"/>
+      <c r="CH31" s="56"/>
+      <c r="CI31" s="56"/>
+      <c r="CJ31" s="56"/>
+      <c r="CK31" s="56"/>
+      <c r="CL31" s="56"/>
+      <c r="CM31" s="56"/>
+      <c r="CN31" s="56"/>
+      <c r="CO31" s="56"/>
+      <c r="CP31" s="56"/>
+      <c r="CQ31" s="56"/>
+      <c r="CR31" s="56"/>
+      <c r="CS31" s="56"/>
+      <c r="CT31" s="56"/>
+      <c r="CU31" s="56"/>
     </row>
     <row r="32" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
@@ -4217,7 +4217,7 @@
         <v>5</v>
       </c>
       <c r="G34" s="30">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="H34" s="24" t="s">
         <v>77</v>
@@ -6104,7 +6104,7 @@
         <v>80</v>
       </c>
       <c r="G58" s="30">
-        <v>0.19</v>
+        <v>0.4</v>
       </c>
       <c r="H58" s="24"/>
       <c r="I58" s="31"/>
@@ -7140,7 +7140,7 @@
         <v>35</v>
       </c>
       <c r="G72" s="30">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H72" s="24"/>
       <c r="I72" s="31"/>
@@ -7697,6 +7697,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A13:CU13"/>
+    <mergeCell ref="B21:CU21"/>
+    <mergeCell ref="B26:CU26"/>
+    <mergeCell ref="A31:CU31"/>
+    <mergeCell ref="A42:CU42"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="AD6:AH6"/>
+    <mergeCell ref="B2:G4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="O6:S6"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="BE2:BW2"/>
+    <mergeCell ref="BE3:BW3"/>
+    <mergeCell ref="CB5:CF5"/>
+    <mergeCell ref="CB6:CF6"/>
+    <mergeCell ref="CG5:CK5"/>
+    <mergeCell ref="CG6:CK6"/>
+    <mergeCell ref="BM5:BQ5"/>
+    <mergeCell ref="BM6:BQ6"/>
+    <mergeCell ref="BR5:BV5"/>
+    <mergeCell ref="BR6:BV6"/>
+    <mergeCell ref="BW5:CA5"/>
+    <mergeCell ref="BW6:CA6"/>
+    <mergeCell ref="BC5:BG5"/>
+    <mergeCell ref="BC6:BG6"/>
+    <mergeCell ref="BH5:BL5"/>
+    <mergeCell ref="BH6:BL6"/>
     <mergeCell ref="A57:CU57"/>
     <mergeCell ref="B49:CU49"/>
     <mergeCell ref="A52:CU52"/>
@@ -7713,37 +7744,6 @@
     <mergeCell ref="AS5:AW5"/>
     <mergeCell ref="AS6:AW6"/>
     <mergeCell ref="Y5:AC5"/>
-    <mergeCell ref="BE2:BW2"/>
-    <mergeCell ref="BE3:BW3"/>
-    <mergeCell ref="CB5:CF5"/>
-    <mergeCell ref="CB6:CF6"/>
-    <mergeCell ref="CG5:CK5"/>
-    <mergeCell ref="CG6:CK6"/>
-    <mergeCell ref="BM5:BQ5"/>
-    <mergeCell ref="BM6:BQ6"/>
-    <mergeCell ref="BR5:BV5"/>
-    <mergeCell ref="BR6:BV6"/>
-    <mergeCell ref="BW5:CA5"/>
-    <mergeCell ref="BW6:CA6"/>
-    <mergeCell ref="BC5:BG5"/>
-    <mergeCell ref="BC6:BG6"/>
-    <mergeCell ref="BH5:BL5"/>
-    <mergeCell ref="BH6:BL6"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="AD5:AH5"/>
-    <mergeCell ref="AD6:AH6"/>
-    <mergeCell ref="B2:G4"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="O6:S6"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="T6:X6"/>
-    <mergeCell ref="A13:CU13"/>
-    <mergeCell ref="B21:CU21"/>
-    <mergeCell ref="B26:CU26"/>
-    <mergeCell ref="A31:CU31"/>
-    <mergeCell ref="A42:CU42"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J53:CU56 J50:CU51 J32:CU41 J43:CU48 J58:CU59 J75:CU75">
     <cfRule type="expression" dxfId="25" priority="84">

</xml_diff>

<commit_message>
quick changes - Gantt
</commit_message>
<xml_diff>
--- a/LaTeX Project/Documentos/Gantt.xlsx
+++ b/LaTeX Project/Documentos/Gantt.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="122">
   <si>
     <t>Dalle Pad</t>
   </si>
@@ -367,12 +367,6 @@
     <t>Soldar todos os componentes necessários na PCB</t>
   </si>
   <si>
-    <t>Amadurecimento do software para Windows</t>
-  </si>
-  <si>
-    <t>Iniciar desenvolvimento do software para Windows</t>
-  </si>
-  <si>
     <t>Finalização do aplicativo para Android</t>
   </si>
   <si>
@@ -406,9 +400,6 @@
     <t>Projetá-lo (via software), com base nos datasheets</t>
   </si>
   <si>
-    <t>L. W. Pereira, L. Z. Cordeiro</t>
-  </si>
-  <si>
     <t>Testes de funcionamento da PCB</t>
   </si>
   <si>
@@ -475,13 +466,13 @@
     <t>MIDI</t>
   </si>
   <si>
-    <t>Finalização do software para Windows e detalhes finais</t>
+    <t>Detalhes finais</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1016,6 +1007,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1034,16 +1031,10 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1808,10 +1799,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:CU84"/>
+  <dimension ref="A2:CU82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="CA58" sqref="AZ58:CA58"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1836,47 +1827,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="24" t="s">
         <v>78</v>
       </c>
       <c r="I2" s="16"/>
-      <c r="BE2" s="53" t="s">
+      <c r="BE2" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" s="53"/>
-      <c r="BG2" s="53"/>
-      <c r="BH2" s="53"/>
-      <c r="BI2" s="53"/>
-      <c r="BJ2" s="53"/>
-      <c r="BK2" s="53"/>
-      <c r="BL2" s="53"/>
-      <c r="BM2" s="53"/>
-      <c r="BN2" s="53"/>
-      <c r="BO2" s="53"/>
-      <c r="BP2" s="53"/>
-      <c r="BQ2" s="53"/>
-      <c r="BR2" s="53"/>
-      <c r="BS2" s="53"/>
-      <c r="BT2" s="53"/>
-      <c r="BU2" s="53"/>
-      <c r="BV2" s="53"/>
-      <c r="BW2" s="53"/>
+      <c r="BF2" s="56"/>
+      <c r="BG2" s="56"/>
+      <c r="BH2" s="56"/>
+      <c r="BI2" s="56"/>
+      <c r="BJ2" s="56"/>
+      <c r="BK2" s="56"/>
+      <c r="BL2" s="56"/>
+      <c r="BM2" s="56"/>
+      <c r="BN2" s="56"/>
+      <c r="BO2" s="56"/>
+      <c r="BP2" s="56"/>
+      <c r="BQ2" s="56"/>
+      <c r="BR2" s="56"/>
+      <c r="BS2" s="56"/>
+      <c r="BT2" s="56"/>
+      <c r="BU2" s="56"/>
+      <c r="BV2" s="56"/>
+      <c r="BW2" s="56"/>
     </row>
     <row r="3" spans="1:99" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="24" t="s">
         <v>79</v>
       </c>
@@ -1925,35 +1916,35 @@
       <c r="AQ3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="BE3" s="53" t="s">
+      <c r="BE3" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="BF3" s="53"/>
-      <c r="BG3" s="53"/>
-      <c r="BH3" s="53"/>
-      <c r="BI3" s="53"/>
-      <c r="BJ3" s="53"/>
-      <c r="BK3" s="53"/>
-      <c r="BL3" s="53"/>
-      <c r="BM3" s="53"/>
-      <c r="BN3" s="53"/>
-      <c r="BO3" s="53"/>
-      <c r="BP3" s="53"/>
-      <c r="BQ3" s="53"/>
-      <c r="BR3" s="53"/>
-      <c r="BS3" s="53"/>
-      <c r="BT3" s="53"/>
-      <c r="BU3" s="53"/>
-      <c r="BV3" s="53"/>
-      <c r="BW3" s="53"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
+      <c r="BI3" s="56"/>
+      <c r="BJ3" s="56"/>
+      <c r="BK3" s="56"/>
+      <c r="BL3" s="56"/>
+      <c r="BM3" s="56"/>
+      <c r="BN3" s="56"/>
+      <c r="BO3" s="56"/>
+      <c r="BP3" s="56"/>
+      <c r="BQ3" s="56"/>
+      <c r="BR3" s="56"/>
+      <c r="BS3" s="56"/>
+      <c r="BT3" s="56"/>
+      <c r="BU3" s="56"/>
+      <c r="BV3" s="56"/>
+      <c r="BW3" s="56"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="24" t="s">
         <v>80</v>
       </c>
@@ -1984,132 +1975,132 @@
       <c r="AY4" s="19"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="47" t="s">
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="50" t="s">
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="47" t="s">
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="48"/>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="50" t="s">
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="50"/>
+      <c r="AB5" s="50"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="51"/>
-      <c r="AF5" s="51"/>
-      <c r="AG5" s="51"/>
-      <c r="AH5" s="52"/>
-      <c r="AI5" s="47" t="s">
+      <c r="AE5" s="53"/>
+      <c r="AF5" s="53"/>
+      <c r="AG5" s="53"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="48"/>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="49"/>
-      <c r="AN5" s="50" t="s">
+      <c r="AJ5" s="50"/>
+      <c r="AK5" s="50"/>
+      <c r="AL5" s="50"/>
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="51"/>
-      <c r="AP5" s="51"/>
-      <c r="AQ5" s="51"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="47" t="s">
+      <c r="AO5" s="53"/>
+      <c r="AP5" s="53"/>
+      <c r="AQ5" s="53"/>
+      <c r="AR5" s="54"/>
+      <c r="AS5" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="AT5" s="48"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="48"/>
-      <c r="AW5" s="49"/>
-      <c r="AX5" s="50" t="s">
+      <c r="AT5" s="50"/>
+      <c r="AU5" s="50"/>
+      <c r="AV5" s="50"/>
+      <c r="AW5" s="51"/>
+      <c r="AX5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="AY5" s="51"/>
-      <c r="AZ5" s="51"/>
-      <c r="BA5" s="51"/>
-      <c r="BB5" s="52"/>
-      <c r="BC5" s="47" t="s">
+      <c r="AY5" s="53"/>
+      <c r="AZ5" s="53"/>
+      <c r="BA5" s="53"/>
+      <c r="BB5" s="54"/>
+      <c r="BC5" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="BD5" s="48"/>
-      <c r="BE5" s="48"/>
-      <c r="BF5" s="48"/>
-      <c r="BG5" s="49"/>
-      <c r="BH5" s="50" t="s">
+      <c r="BD5" s="50"/>
+      <c r="BE5" s="50"/>
+      <c r="BF5" s="50"/>
+      <c r="BG5" s="51"/>
+      <c r="BH5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="BI5" s="51"/>
-      <c r="BJ5" s="51"/>
-      <c r="BK5" s="51"/>
-      <c r="BL5" s="52"/>
-      <c r="BM5" s="47" t="s">
+      <c r="BI5" s="53"/>
+      <c r="BJ5" s="53"/>
+      <c r="BK5" s="53"/>
+      <c r="BL5" s="54"/>
+      <c r="BM5" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="BN5" s="48"/>
-      <c r="BO5" s="48"/>
-      <c r="BP5" s="48"/>
-      <c r="BQ5" s="49"/>
-      <c r="BR5" s="50" t="s">
+      <c r="BN5" s="50"/>
+      <c r="BO5" s="50"/>
+      <c r="BP5" s="50"/>
+      <c r="BQ5" s="51"/>
+      <c r="BR5" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="BS5" s="51"/>
-      <c r="BT5" s="51"/>
-      <c r="BU5" s="51"/>
-      <c r="BV5" s="52"/>
-      <c r="BW5" s="47" t="s">
+      <c r="BS5" s="53"/>
+      <c r="BT5" s="53"/>
+      <c r="BU5" s="53"/>
+      <c r="BV5" s="54"/>
+      <c r="BW5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="BX5" s="48"/>
-      <c r="BY5" s="48"/>
-      <c r="BZ5" s="48"/>
-      <c r="CA5" s="49"/>
-      <c r="CB5" s="50" t="s">
+      <c r="BX5" s="50"/>
+      <c r="BY5" s="50"/>
+      <c r="BZ5" s="50"/>
+      <c r="CA5" s="51"/>
+      <c r="CB5" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="CC5" s="51"/>
-      <c r="CD5" s="51"/>
-      <c r="CE5" s="51"/>
-      <c r="CF5" s="52"/>
-      <c r="CG5" s="47" t="s">
+      <c r="CC5" s="53"/>
+      <c r="CD5" s="53"/>
+      <c r="CE5" s="53"/>
+      <c r="CF5" s="54"/>
+      <c r="CG5" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="CH5" s="48"/>
-      <c r="CI5" s="48"/>
-      <c r="CJ5" s="48"/>
-      <c r="CK5" s="49"/>
-      <c r="CL5" s="50" t="s">
+      <c r="CH5" s="50"/>
+      <c r="CI5" s="50"/>
+      <c r="CJ5" s="50"/>
+      <c r="CK5" s="51"/>
+      <c r="CL5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="CM5" s="51"/>
-      <c r="CN5" s="51"/>
-      <c r="CO5" s="51"/>
-      <c r="CP5" s="52"/>
-      <c r="CQ5" s="47" t="s">
+      <c r="CM5" s="53"/>
+      <c r="CN5" s="53"/>
+      <c r="CO5" s="53"/>
+      <c r="CP5" s="54"/>
+      <c r="CQ5" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="CR5" s="48"/>
-      <c r="CS5" s="48"/>
-      <c r="CT5" s="48"/>
-      <c r="CU5" s="49"/>
+      <c r="CR5" s="50"/>
+      <c r="CS5" s="50"/>
+      <c r="CT5" s="50"/>
+      <c r="CU5" s="51"/>
     </row>
     <row r="6" spans="1:99" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -2132,132 +2123,132 @@
         <v>75</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="47" t="s">
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="50" t="s">
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="51"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="47" t="s">
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="Z6" s="48"/>
-      <c r="AA6" s="48"/>
-      <c r="AB6" s="48"/>
-      <c r="AC6" s="49"/>
-      <c r="AD6" s="50" t="s">
+      <c r="Z6" s="50"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="50"/>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="51"/>
-      <c r="AF6" s="51"/>
-      <c r="AG6" s="51"/>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="47" t="s">
+      <c r="AE6" s="53"/>
+      <c r="AF6" s="53"/>
+      <c r="AG6" s="53"/>
+      <c r="AH6" s="54"/>
+      <c r="AI6" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="48"/>
-      <c r="AL6" s="48"/>
-      <c r="AM6" s="49"/>
-      <c r="AN6" s="50" t="s">
+      <c r="AJ6" s="50"/>
+      <c r="AK6" s="50"/>
+      <c r="AL6" s="50"/>
+      <c r="AM6" s="51"/>
+      <c r="AN6" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" s="51"/>
-      <c r="AP6" s="51"/>
-      <c r="AQ6" s="51"/>
-      <c r="AR6" s="52"/>
-      <c r="AS6" s="47" t="s">
+      <c r="AO6" s="53"/>
+      <c r="AP6" s="53"/>
+      <c r="AQ6" s="53"/>
+      <c r="AR6" s="54"/>
+      <c r="AS6" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="AT6" s="48"/>
-      <c r="AU6" s="48"/>
-      <c r="AV6" s="48"/>
-      <c r="AW6" s="49"/>
-      <c r="AX6" s="50" t="s">
+      <c r="AT6" s="50"/>
+      <c r="AU6" s="50"/>
+      <c r="AV6" s="50"/>
+      <c r="AW6" s="51"/>
+      <c r="AX6" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="AY6" s="51"/>
-      <c r="AZ6" s="51"/>
-      <c r="BA6" s="51"/>
-      <c r="BB6" s="52"/>
-      <c r="BC6" s="47" t="s">
+      <c r="AY6" s="53"/>
+      <c r="AZ6" s="53"/>
+      <c r="BA6" s="53"/>
+      <c r="BB6" s="54"/>
+      <c r="BC6" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="BD6" s="48"/>
-      <c r="BE6" s="48"/>
-      <c r="BF6" s="48"/>
-      <c r="BG6" s="49"/>
-      <c r="BH6" s="50" t="s">
+      <c r="BD6" s="50"/>
+      <c r="BE6" s="50"/>
+      <c r="BF6" s="50"/>
+      <c r="BG6" s="51"/>
+      <c r="BH6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="BI6" s="51"/>
-      <c r="BJ6" s="51"/>
-      <c r="BK6" s="51"/>
-      <c r="BL6" s="52"/>
-      <c r="BM6" s="47" t="s">
+      <c r="BI6" s="53"/>
+      <c r="BJ6" s="53"/>
+      <c r="BK6" s="53"/>
+      <c r="BL6" s="54"/>
+      <c r="BM6" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="BN6" s="48"/>
-      <c r="BO6" s="48"/>
-      <c r="BP6" s="48"/>
-      <c r="BQ6" s="49"/>
-      <c r="BR6" s="50" t="s">
+      <c r="BN6" s="50"/>
+      <c r="BO6" s="50"/>
+      <c r="BP6" s="50"/>
+      <c r="BQ6" s="51"/>
+      <c r="BR6" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="BS6" s="51"/>
-      <c r="BT6" s="51"/>
-      <c r="BU6" s="51"/>
-      <c r="BV6" s="52"/>
-      <c r="BW6" s="47" t="s">
+      <c r="BS6" s="53"/>
+      <c r="BT6" s="53"/>
+      <c r="BU6" s="53"/>
+      <c r="BV6" s="54"/>
+      <c r="BW6" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="BX6" s="48"/>
-      <c r="BY6" s="48"/>
-      <c r="BZ6" s="48"/>
-      <c r="CA6" s="49"/>
-      <c r="CB6" s="50" t="s">
+      <c r="BX6" s="50"/>
+      <c r="BY6" s="50"/>
+      <c r="BZ6" s="50"/>
+      <c r="CA6" s="51"/>
+      <c r="CB6" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="CC6" s="51"/>
-      <c r="CD6" s="51"/>
-      <c r="CE6" s="51"/>
-      <c r="CF6" s="52"/>
-      <c r="CG6" s="47" t="s">
+      <c r="CC6" s="53"/>
+      <c r="CD6" s="53"/>
+      <c r="CE6" s="53"/>
+      <c r="CF6" s="54"/>
+      <c r="CG6" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="CH6" s="48"/>
-      <c r="CI6" s="48"/>
-      <c r="CJ6" s="48"/>
-      <c r="CK6" s="49"/>
-      <c r="CL6" s="50" t="s">
+      <c r="CH6" s="50"/>
+      <c r="CI6" s="50"/>
+      <c r="CJ6" s="50"/>
+      <c r="CK6" s="51"/>
+      <c r="CL6" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="CM6" s="51"/>
-      <c r="CN6" s="51"/>
-      <c r="CO6" s="51"/>
-      <c r="CP6" s="52"/>
-      <c r="CQ6" s="47" t="s">
+      <c r="CM6" s="53"/>
+      <c r="CN6" s="53"/>
+      <c r="CO6" s="53"/>
+      <c r="CP6" s="54"/>
+      <c r="CQ6" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="CR6" s="48"/>
-      <c r="CS6" s="48"/>
-      <c r="CT6" s="48"/>
-      <c r="CU6" s="49"/>
+      <c r="CR6" s="50"/>
+      <c r="CS6" s="50"/>
+      <c r="CT6" s="50"/>
+      <c r="CU6" s="51"/>
     </row>
     <row r="7" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -3162,104 +3153,104 @@
       <c r="AC20" s="31"/>
     </row>
     <row r="21" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="55"/>
-      <c r="T21" s="55"/>
-      <c r="U21" s="55"/>
-      <c r="V21" s="55"/>
-      <c r="W21" s="55"/>
-      <c r="X21" s="55"/>
-      <c r="Y21" s="55"/>
-      <c r="Z21" s="55"/>
-      <c r="AA21" s="55"/>
-      <c r="AB21" s="55"/>
-      <c r="AC21" s="55"/>
-      <c r="AD21" s="55"/>
-      <c r="AE21" s="55"/>
-      <c r="AF21" s="55"/>
-      <c r="AG21" s="55"/>
-      <c r="AH21" s="55"/>
-      <c r="AI21" s="55"/>
-      <c r="AJ21" s="55"/>
-      <c r="AK21" s="55"/>
-      <c r="AL21" s="55"/>
-      <c r="AM21" s="55"/>
-      <c r="AN21" s="55"/>
-      <c r="AO21" s="55"/>
-      <c r="AP21" s="55"/>
-      <c r="AQ21" s="55"/>
-      <c r="AR21" s="55"/>
-      <c r="AS21" s="55"/>
-      <c r="AT21" s="55"/>
-      <c r="AU21" s="55"/>
-      <c r="AV21" s="55"/>
-      <c r="AW21" s="55"/>
-      <c r="AX21" s="55"/>
-      <c r="AY21" s="55"/>
-      <c r="AZ21" s="55"/>
-      <c r="BA21" s="55"/>
-      <c r="BB21" s="55"/>
-      <c r="BC21" s="55"/>
-      <c r="BD21" s="55"/>
-      <c r="BE21" s="55"/>
-      <c r="BF21" s="55"/>
-      <c r="BG21" s="55"/>
-      <c r="BH21" s="55"/>
-      <c r="BI21" s="55"/>
-      <c r="BJ21" s="55"/>
-      <c r="BK21" s="55"/>
-      <c r="BL21" s="55"/>
-      <c r="BM21" s="55"/>
-      <c r="BN21" s="55"/>
-      <c r="BO21" s="55"/>
-      <c r="BP21" s="55"/>
-      <c r="BQ21" s="55"/>
-      <c r="BR21" s="55"/>
-      <c r="BS21" s="55"/>
-      <c r="BT21" s="55"/>
-      <c r="BU21" s="55"/>
-      <c r="BV21" s="55"/>
-      <c r="BW21" s="55"/>
-      <c r="BX21" s="55"/>
-      <c r="BY21" s="55"/>
-      <c r="BZ21" s="55"/>
-      <c r="CA21" s="55"/>
-      <c r="CB21" s="55"/>
-      <c r="CC21" s="55"/>
-      <c r="CD21" s="55"/>
-      <c r="CE21" s="55"/>
-      <c r="CF21" s="55"/>
-      <c r="CG21" s="55"/>
-      <c r="CH21" s="55"/>
-      <c r="CI21" s="55"/>
-      <c r="CJ21" s="55"/>
-      <c r="CK21" s="55"/>
-      <c r="CL21" s="55"/>
-      <c r="CM21" s="55"/>
-      <c r="CN21" s="55"/>
-      <c r="CO21" s="55"/>
-      <c r="CP21" s="55"/>
-      <c r="CQ21" s="55"/>
-      <c r="CR21" s="55"/>
-      <c r="CS21" s="55"/>
-      <c r="CT21" s="55"/>
-      <c r="CU21" s="55"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="47"/>
+      <c r="Z21" s="47"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="47"/>
+      <c r="AF21" s="47"/>
+      <c r="AG21" s="47"/>
+      <c r="AH21" s="47"/>
+      <c r="AI21" s="47"/>
+      <c r="AJ21" s="47"/>
+      <c r="AK21" s="47"/>
+      <c r="AL21" s="47"/>
+      <c r="AM21" s="47"/>
+      <c r="AN21" s="47"/>
+      <c r="AO21" s="47"/>
+      <c r="AP21" s="47"/>
+      <c r="AQ21" s="47"/>
+      <c r="AR21" s="47"/>
+      <c r="AS21" s="47"/>
+      <c r="AT21" s="47"/>
+      <c r="AU21" s="47"/>
+      <c r="AV21" s="47"/>
+      <c r="AW21" s="47"/>
+      <c r="AX21" s="47"/>
+      <c r="AY21" s="47"/>
+      <c r="AZ21" s="47"/>
+      <c r="BA21" s="47"/>
+      <c r="BB21" s="47"/>
+      <c r="BC21" s="47"/>
+      <c r="BD21" s="47"/>
+      <c r="BE21" s="47"/>
+      <c r="BF21" s="47"/>
+      <c r="BG21" s="47"/>
+      <c r="BH21" s="47"/>
+      <c r="BI21" s="47"/>
+      <c r="BJ21" s="47"/>
+      <c r="BK21" s="47"/>
+      <c r="BL21" s="47"/>
+      <c r="BM21" s="47"/>
+      <c r="BN21" s="47"/>
+      <c r="BO21" s="47"/>
+      <c r="BP21" s="47"/>
+      <c r="BQ21" s="47"/>
+      <c r="BR21" s="47"/>
+      <c r="BS21" s="47"/>
+      <c r="BT21" s="47"/>
+      <c r="BU21" s="47"/>
+      <c r="BV21" s="47"/>
+      <c r="BW21" s="47"/>
+      <c r="BX21" s="47"/>
+      <c r="BY21" s="47"/>
+      <c r="BZ21" s="47"/>
+      <c r="CA21" s="47"/>
+      <c r="CB21" s="47"/>
+      <c r="CC21" s="47"/>
+      <c r="CD21" s="47"/>
+      <c r="CE21" s="47"/>
+      <c r="CF21" s="47"/>
+      <c r="CG21" s="47"/>
+      <c r="CH21" s="47"/>
+      <c r="CI21" s="47"/>
+      <c r="CJ21" s="47"/>
+      <c r="CK21" s="47"/>
+      <c r="CL21" s="47"/>
+      <c r="CM21" s="47"/>
+      <c r="CN21" s="47"/>
+      <c r="CO21" s="47"/>
+      <c r="CP21" s="47"/>
+      <c r="CQ21" s="47"/>
+      <c r="CR21" s="47"/>
+      <c r="CS21" s="47"/>
+      <c r="CT21" s="47"/>
+      <c r="CU21" s="47"/>
     </row>
     <row r="22" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
@@ -3554,104 +3545,104 @@
       <c r="CU25" s="35"/>
     </row>
     <row r="26" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="55"/>
-      <c r="S26" s="55"/>
-      <c r="T26" s="55"/>
-      <c r="U26" s="55"/>
-      <c r="V26" s="55"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="55"/>
-      <c r="Y26" s="55"/>
-      <c r="Z26" s="55"/>
-      <c r="AA26" s="55"/>
-      <c r="AB26" s="55"/>
-      <c r="AC26" s="55"/>
-      <c r="AD26" s="55"/>
-      <c r="AE26" s="55"/>
-      <c r="AF26" s="55"/>
-      <c r="AG26" s="55"/>
-      <c r="AH26" s="55"/>
-      <c r="AI26" s="55"/>
-      <c r="AJ26" s="55"/>
-      <c r="AK26" s="55"/>
-      <c r="AL26" s="55"/>
-      <c r="AM26" s="55"/>
-      <c r="AN26" s="55"/>
-      <c r="AO26" s="55"/>
-      <c r="AP26" s="55"/>
-      <c r="AQ26" s="55"/>
-      <c r="AR26" s="55"/>
-      <c r="AS26" s="55"/>
-      <c r="AT26" s="55"/>
-      <c r="AU26" s="55"/>
-      <c r="AV26" s="55"/>
-      <c r="AW26" s="55"/>
-      <c r="AX26" s="55"/>
-      <c r="AY26" s="55"/>
-      <c r="AZ26" s="55"/>
-      <c r="BA26" s="55"/>
-      <c r="BB26" s="55"/>
-      <c r="BC26" s="55"/>
-      <c r="BD26" s="55"/>
-      <c r="BE26" s="55"/>
-      <c r="BF26" s="55"/>
-      <c r="BG26" s="55"/>
-      <c r="BH26" s="55"/>
-      <c r="BI26" s="55"/>
-      <c r="BJ26" s="55"/>
-      <c r="BK26" s="55"/>
-      <c r="BL26" s="55"/>
-      <c r="BM26" s="55"/>
-      <c r="BN26" s="55"/>
-      <c r="BO26" s="55"/>
-      <c r="BP26" s="55"/>
-      <c r="BQ26" s="55"/>
-      <c r="BR26" s="55"/>
-      <c r="BS26" s="55"/>
-      <c r="BT26" s="55"/>
-      <c r="BU26" s="55"/>
-      <c r="BV26" s="55"/>
-      <c r="BW26" s="55"/>
-      <c r="BX26" s="55"/>
-      <c r="BY26" s="55"/>
-      <c r="BZ26" s="55"/>
-      <c r="CA26" s="55"/>
-      <c r="CB26" s="55"/>
-      <c r="CC26" s="55"/>
-      <c r="CD26" s="55"/>
-      <c r="CE26" s="55"/>
-      <c r="CF26" s="55"/>
-      <c r="CG26" s="55"/>
-      <c r="CH26" s="55"/>
-      <c r="CI26" s="55"/>
-      <c r="CJ26" s="55"/>
-      <c r="CK26" s="55"/>
-      <c r="CL26" s="55"/>
-      <c r="CM26" s="55"/>
-      <c r="CN26" s="55"/>
-      <c r="CO26" s="55"/>
-      <c r="CP26" s="55"/>
-      <c r="CQ26" s="55"/>
-      <c r="CR26" s="55"/>
-      <c r="CS26" s="55"/>
-      <c r="CT26" s="55"/>
-      <c r="CU26" s="55"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="47"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="47"/>
+      <c r="AE26" s="47"/>
+      <c r="AF26" s="47"/>
+      <c r="AG26" s="47"/>
+      <c r="AH26" s="47"/>
+      <c r="AI26" s="47"/>
+      <c r="AJ26" s="47"/>
+      <c r="AK26" s="47"/>
+      <c r="AL26" s="47"/>
+      <c r="AM26" s="47"/>
+      <c r="AN26" s="47"/>
+      <c r="AO26" s="47"/>
+      <c r="AP26" s="47"/>
+      <c r="AQ26" s="47"/>
+      <c r="AR26" s="47"/>
+      <c r="AS26" s="47"/>
+      <c r="AT26" s="47"/>
+      <c r="AU26" s="47"/>
+      <c r="AV26" s="47"/>
+      <c r="AW26" s="47"/>
+      <c r="AX26" s="47"/>
+      <c r="AY26" s="47"/>
+      <c r="AZ26" s="47"/>
+      <c r="BA26" s="47"/>
+      <c r="BB26" s="47"/>
+      <c r="BC26" s="47"/>
+      <c r="BD26" s="47"/>
+      <c r="BE26" s="47"/>
+      <c r="BF26" s="47"/>
+      <c r="BG26" s="47"/>
+      <c r="BH26" s="47"/>
+      <c r="BI26" s="47"/>
+      <c r="BJ26" s="47"/>
+      <c r="BK26" s="47"/>
+      <c r="BL26" s="47"/>
+      <c r="BM26" s="47"/>
+      <c r="BN26" s="47"/>
+      <c r="BO26" s="47"/>
+      <c r="BP26" s="47"/>
+      <c r="BQ26" s="47"/>
+      <c r="BR26" s="47"/>
+      <c r="BS26" s="47"/>
+      <c r="BT26" s="47"/>
+      <c r="BU26" s="47"/>
+      <c r="BV26" s="47"/>
+      <c r="BW26" s="47"/>
+      <c r="BX26" s="47"/>
+      <c r="BY26" s="47"/>
+      <c r="BZ26" s="47"/>
+      <c r="CA26" s="47"/>
+      <c r="CB26" s="47"/>
+      <c r="CC26" s="47"/>
+      <c r="CD26" s="47"/>
+      <c r="CE26" s="47"/>
+      <c r="CF26" s="47"/>
+      <c r="CG26" s="47"/>
+      <c r="CH26" s="47"/>
+      <c r="CI26" s="47"/>
+      <c r="CJ26" s="47"/>
+      <c r="CK26" s="47"/>
+      <c r="CL26" s="47"/>
+      <c r="CM26" s="47"/>
+      <c r="CN26" s="47"/>
+      <c r="CO26" s="47"/>
+      <c r="CP26" s="47"/>
+      <c r="CQ26" s="47"/>
+      <c r="CR26" s="47"/>
+      <c r="CS26" s="47"/>
+      <c r="CT26" s="47"/>
+      <c r="CU26" s="47"/>
     </row>
     <row r="27" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
@@ -3746,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -3818,10 +3809,10 @@
         <v>5</v>
       </c>
       <c r="G29" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
@@ -3952,105 +3943,105 @@
       <c r="CU30" s="35"/>
     </row>
     <row r="31" spans="1:99" s="45" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="56"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
-      <c r="X31" s="56"/>
-      <c r="Y31" s="56"/>
-      <c r="Z31" s="56"/>
-      <c r="AA31" s="56"/>
-      <c r="AB31" s="56"/>
-      <c r="AC31" s="56"/>
-      <c r="AD31" s="56"/>
-      <c r="AE31" s="56"/>
-      <c r="AF31" s="56"/>
-      <c r="AG31" s="56"/>
-      <c r="AH31" s="56"/>
-      <c r="AI31" s="56"/>
-      <c r="AJ31" s="56"/>
-      <c r="AK31" s="56"/>
-      <c r="AL31" s="56"/>
-      <c r="AM31" s="56"/>
-      <c r="AN31" s="56"/>
-      <c r="AO31" s="56"/>
-      <c r="AP31" s="56"/>
-      <c r="AQ31" s="56"/>
-      <c r="AR31" s="56"/>
-      <c r="AS31" s="56"/>
-      <c r="AT31" s="56"/>
-      <c r="AU31" s="56"/>
-      <c r="AV31" s="56"/>
-      <c r="AW31" s="56"/>
-      <c r="AX31" s="56"/>
-      <c r="AY31" s="56"/>
-      <c r="AZ31" s="56"/>
-      <c r="BA31" s="56"/>
-      <c r="BB31" s="56"/>
-      <c r="BC31" s="56"/>
-      <c r="BD31" s="56"/>
-      <c r="BE31" s="56"/>
-      <c r="BF31" s="56"/>
-      <c r="BG31" s="56"/>
-      <c r="BH31" s="56"/>
-      <c r="BI31" s="56"/>
-      <c r="BJ31" s="56"/>
-      <c r="BK31" s="56"/>
-      <c r="BL31" s="56"/>
-      <c r="BM31" s="56"/>
-      <c r="BN31" s="56"/>
-      <c r="BO31" s="56"/>
-      <c r="BP31" s="56"/>
-      <c r="BQ31" s="56"/>
-      <c r="BR31" s="56"/>
-      <c r="BS31" s="56"/>
-      <c r="BT31" s="56"/>
-      <c r="BU31" s="56"/>
-      <c r="BV31" s="56"/>
-      <c r="BW31" s="56"/>
-      <c r="BX31" s="56"/>
-      <c r="BY31" s="56"/>
-      <c r="BZ31" s="56"/>
-      <c r="CA31" s="56"/>
-      <c r="CB31" s="56"/>
-      <c r="CC31" s="56"/>
-      <c r="CD31" s="56"/>
-      <c r="CE31" s="56"/>
-      <c r="CF31" s="56"/>
-      <c r="CG31" s="56"/>
-      <c r="CH31" s="56"/>
-      <c r="CI31" s="56"/>
-      <c r="CJ31" s="56"/>
-      <c r="CK31" s="56"/>
-      <c r="CL31" s="56"/>
-      <c r="CM31" s="56"/>
-      <c r="CN31" s="56"/>
-      <c r="CO31" s="56"/>
-      <c r="CP31" s="56"/>
-      <c r="CQ31" s="56"/>
-      <c r="CR31" s="56"/>
-      <c r="CS31" s="56"/>
-      <c r="CT31" s="56"/>
-      <c r="CU31" s="56"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="48"/>
+      <c r="V31" s="48"/>
+      <c r="W31" s="48"/>
+      <c r="X31" s="48"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="48"/>
+      <c r="AA31" s="48"/>
+      <c r="AB31" s="48"/>
+      <c r="AC31" s="48"/>
+      <c r="AD31" s="48"/>
+      <c r="AE31" s="48"/>
+      <c r="AF31" s="48"/>
+      <c r="AG31" s="48"/>
+      <c r="AH31" s="48"/>
+      <c r="AI31" s="48"/>
+      <c r="AJ31" s="48"/>
+      <c r="AK31" s="48"/>
+      <c r="AL31" s="48"/>
+      <c r="AM31" s="48"/>
+      <c r="AN31" s="48"/>
+      <c r="AO31" s="48"/>
+      <c r="AP31" s="48"/>
+      <c r="AQ31" s="48"/>
+      <c r="AR31" s="48"/>
+      <c r="AS31" s="48"/>
+      <c r="AT31" s="48"/>
+      <c r="AU31" s="48"/>
+      <c r="AV31" s="48"/>
+      <c r="AW31" s="48"/>
+      <c r="AX31" s="48"/>
+      <c r="AY31" s="48"/>
+      <c r="AZ31" s="48"/>
+      <c r="BA31" s="48"/>
+      <c r="BB31" s="48"/>
+      <c r="BC31" s="48"/>
+      <c r="BD31" s="48"/>
+      <c r="BE31" s="48"/>
+      <c r="BF31" s="48"/>
+      <c r="BG31" s="48"/>
+      <c r="BH31" s="48"/>
+      <c r="BI31" s="48"/>
+      <c r="BJ31" s="48"/>
+      <c r="BK31" s="48"/>
+      <c r="BL31" s="48"/>
+      <c r="BM31" s="48"/>
+      <c r="BN31" s="48"/>
+      <c r="BO31" s="48"/>
+      <c r="BP31" s="48"/>
+      <c r="BQ31" s="48"/>
+      <c r="BR31" s="48"/>
+      <c r="BS31" s="48"/>
+      <c r="BT31" s="48"/>
+      <c r="BU31" s="48"/>
+      <c r="BV31" s="48"/>
+      <c r="BW31" s="48"/>
+      <c r="BX31" s="48"/>
+      <c r="BY31" s="48"/>
+      <c r="BZ31" s="48"/>
+      <c r="CA31" s="48"/>
+      <c r="CB31" s="48"/>
+      <c r="CC31" s="48"/>
+      <c r="CD31" s="48"/>
+      <c r="CE31" s="48"/>
+      <c r="CF31" s="48"/>
+      <c r="CG31" s="48"/>
+      <c r="CH31" s="48"/>
+      <c r="CI31" s="48"/>
+      <c r="CJ31" s="48"/>
+      <c r="CK31" s="48"/>
+      <c r="CL31" s="48"/>
+      <c r="CM31" s="48"/>
+      <c r="CN31" s="48"/>
+      <c r="CO31" s="48"/>
+      <c r="CP31" s="48"/>
+      <c r="CQ31" s="48"/>
+      <c r="CR31" s="48"/>
+      <c r="CS31" s="48"/>
+      <c r="CT31" s="48"/>
+      <c r="CU31" s="48"/>
     </row>
     <row r="32" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
@@ -4127,7 +4118,7 @@
     </row>
     <row r="33" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C33" s="29">
         <v>36</v>
@@ -4202,7 +4193,7 @@
     </row>
     <row r="34" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C34" s="29">
         <v>36</v>
@@ -4277,7 +4268,7 @@
     </row>
     <row r="35" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C35" s="29">
         <v>41</v>
@@ -4427,25 +4418,25 @@
     </row>
     <row r="37" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="38" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C37" s="29">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D37" s="29">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E37" s="29">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F37" s="29">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G37" s="30">
         <v>0</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I37" s="31"/>
       <c r="J37" s="31"/>
@@ -4501,20 +4492,20 @@
       <c r="CU37" s="35"/>
     </row>
     <row r="38" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="38" t="s">
-        <v>95</v>
+      <c r="B38" s="40" t="s">
+        <v>94</v>
       </c>
       <c r="C38" s="29">
         <v>36</v>
       </c>
       <c r="D38" s="29">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E38" s="29">
         <v>36</v>
       </c>
       <c r="F38" s="29">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G38" s="30">
         <v>0</v>
@@ -4577,19 +4568,19 @@
     </row>
     <row r="39" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" s="29">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D39" s="29">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E39" s="29">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F39" s="29">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G39" s="30">
         <v>0</v>
@@ -4651,20 +4642,20 @@
       <c r="CU39" s="35"/>
     </row>
     <row r="40" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="40" t="s">
-        <v>97</v>
+      <c r="B40" s="38" t="s">
+        <v>87</v>
       </c>
       <c r="C40" s="29">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D40" s="29">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E40" s="29">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F40" s="29">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G40" s="30">
         <v>0</v>
@@ -4725,202 +4716,202 @@
       <c r="CT40" s="35"/>
       <c r="CU40" s="35"/>
     </row>
-    <row r="41" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="29">
-        <v>51</v>
-      </c>
-      <c r="D41" s="29">
-        <v>5</v>
-      </c>
-      <c r="E41" s="29">
-        <v>51</v>
-      </c>
-      <c r="F41" s="29">
-        <v>5</v>
-      </c>
-      <c r="G41" s="30">
+    <row r="41" spans="1:99" s="44" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="46"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="46"/>
+      <c r="N41" s="46"/>
+      <c r="O41" s="46"/>
+      <c r="P41" s="46"/>
+      <c r="Q41" s="46"/>
+      <c r="R41" s="46"/>
+      <c r="S41" s="46"/>
+      <c r="T41" s="46"/>
+      <c r="U41" s="46"/>
+      <c r="V41" s="46"/>
+      <c r="W41" s="46"/>
+      <c r="X41" s="46"/>
+      <c r="Y41" s="46"/>
+      <c r="Z41" s="46"/>
+      <c r="AA41" s="46"/>
+      <c r="AB41" s="46"/>
+      <c r="AC41" s="46"/>
+      <c r="AD41" s="46"/>
+      <c r="AE41" s="46"/>
+      <c r="AF41" s="46"/>
+      <c r="AG41" s="46"/>
+      <c r="AH41" s="46"/>
+      <c r="AI41" s="46"/>
+      <c r="AJ41" s="46"/>
+      <c r="AK41" s="46"/>
+      <c r="AL41" s="46"/>
+      <c r="AM41" s="46"/>
+      <c r="AN41" s="46"/>
+      <c r="AO41" s="46"/>
+      <c r="AP41" s="46"/>
+      <c r="AQ41" s="46"/>
+      <c r="AR41" s="46"/>
+      <c r="AS41" s="46"/>
+      <c r="AT41" s="46"/>
+      <c r="AU41" s="46"/>
+      <c r="AV41" s="46"/>
+      <c r="AW41" s="46"/>
+      <c r="AX41" s="46"/>
+      <c r="AY41" s="46"/>
+      <c r="AZ41" s="46"/>
+      <c r="BA41" s="46"/>
+      <c r="BB41" s="46"/>
+      <c r="BC41" s="46"/>
+      <c r="BD41" s="46"/>
+      <c r="BE41" s="46"/>
+      <c r="BF41" s="46"/>
+      <c r="BG41" s="46"/>
+      <c r="BH41" s="46"/>
+      <c r="BI41" s="46"/>
+      <c r="BJ41" s="46"/>
+      <c r="BK41" s="46"/>
+      <c r="BL41" s="46"/>
+      <c r="BM41" s="46"/>
+      <c r="BN41" s="46"/>
+      <c r="BO41" s="46"/>
+      <c r="BP41" s="46"/>
+      <c r="BQ41" s="46"/>
+      <c r="BR41" s="46"/>
+      <c r="BS41" s="46"/>
+      <c r="BT41" s="46"/>
+      <c r="BU41" s="46"/>
+      <c r="BV41" s="46"/>
+      <c r="BW41" s="46"/>
+      <c r="BX41" s="46"/>
+      <c r="BY41" s="46"/>
+      <c r="BZ41" s="46"/>
+      <c r="CA41" s="46"/>
+      <c r="CB41" s="46"/>
+      <c r="CC41" s="46"/>
+      <c r="CD41" s="46"/>
+      <c r="CE41" s="46"/>
+      <c r="CF41" s="46"/>
+      <c r="CG41" s="46"/>
+      <c r="CH41" s="46"/>
+      <c r="CI41" s="46"/>
+      <c r="CJ41" s="46"/>
+      <c r="CK41" s="46"/>
+      <c r="CL41" s="46"/>
+      <c r="CM41" s="46"/>
+      <c r="CN41" s="46"/>
+      <c r="CO41" s="46"/>
+      <c r="CP41" s="46"/>
+      <c r="CQ41" s="46"/>
+      <c r="CR41" s="46"/>
+      <c r="CS41" s="46"/>
+      <c r="CT41" s="46"/>
+      <c r="CU41" s="46"/>
+    </row>
+    <row r="42" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="41">
+        <v>56</v>
+      </c>
+      <c r="D42" s="41">
+        <v>15</v>
+      </c>
+      <c r="E42" s="41">
+        <v>56</v>
+      </c>
+      <c r="F42" s="41">
+        <v>15</v>
+      </c>
+      <c r="G42" s="30">
         <v>0</v>
       </c>
-      <c r="H41" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="31"/>
-      <c r="Q41" s="31"/>
-      <c r="R41" s="31"/>
-      <c r="S41" s="31"/>
-      <c r="T41" s="31"/>
-      <c r="U41" s="31"/>
-      <c r="V41" s="31"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-      <c r="AA41" s="31"/>
-      <c r="AB41" s="31"/>
-      <c r="AC41" s="31"/>
-      <c r="BQ41" s="33"/>
-      <c r="BR41" s="34"/>
-      <c r="BS41" s="33"/>
-      <c r="BT41" s="33"/>
-      <c r="BU41" s="33"/>
-      <c r="BV41" s="33"/>
-      <c r="BW41" s="33"/>
-      <c r="BX41" s="33"/>
-      <c r="BY41" s="33"/>
-      <c r="BZ41" s="33"/>
-      <c r="CA41" s="33"/>
-      <c r="CB41" s="33"/>
-      <c r="CC41" s="33"/>
-      <c r="CD41" s="33"/>
-      <c r="CE41" s="33"/>
-      <c r="CF41" s="33"/>
-      <c r="CG41" s="33"/>
-      <c r="CH41" s="35"/>
-      <c r="CI41" s="35"/>
-      <c r="CJ41" s="35"/>
-      <c r="CK41" s="35"/>
-      <c r="CL41" s="35"/>
-      <c r="CM41" s="35"/>
-      <c r="CN41" s="35"/>
-      <c r="CO41" s="35"/>
-      <c r="CP41" s="35"/>
-      <c r="CQ41" s="35"/>
-      <c r="CR41" s="35"/>
-      <c r="CS41" s="35"/>
-      <c r="CT41" s="35"/>
-      <c r="CU41" s="35"/>
-    </row>
-    <row r="42" spans="1:99" s="44" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="46"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="46"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="46"/>
-      <c r="N42" s="46"/>
-      <c r="O42" s="46"/>
-      <c r="P42" s="46"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="46"/>
-      <c r="S42" s="46"/>
-      <c r="T42" s="46"/>
-      <c r="U42" s="46"/>
-      <c r="V42" s="46"/>
-      <c r="W42" s="46"/>
-      <c r="X42" s="46"/>
-      <c r="Y42" s="46"/>
-      <c r="Z42" s="46"/>
-      <c r="AA42" s="46"/>
-      <c r="AB42" s="46"/>
-      <c r="AC42" s="46"/>
-      <c r="AD42" s="46"/>
-      <c r="AE42" s="46"/>
-      <c r="AF42" s="46"/>
-      <c r="AG42" s="46"/>
-      <c r="AH42" s="46"/>
-      <c r="AI42" s="46"/>
-      <c r="AJ42" s="46"/>
-      <c r="AK42" s="46"/>
-      <c r="AL42" s="46"/>
-      <c r="AM42" s="46"/>
-      <c r="AN42" s="46"/>
-      <c r="AO42" s="46"/>
-      <c r="AP42" s="46"/>
-      <c r="AQ42" s="46"/>
-      <c r="AR42" s="46"/>
-      <c r="AS42" s="46"/>
-      <c r="AT42" s="46"/>
-      <c r="AU42" s="46"/>
-      <c r="AV42" s="46"/>
-      <c r="AW42" s="46"/>
-      <c r="AX42" s="46"/>
-      <c r="AY42" s="46"/>
-      <c r="AZ42" s="46"/>
-      <c r="BA42" s="46"/>
-      <c r="BB42" s="46"/>
-      <c r="BC42" s="46"/>
-      <c r="BD42" s="46"/>
-      <c r="BE42" s="46"/>
-      <c r="BF42" s="46"/>
-      <c r="BG42" s="46"/>
-      <c r="BH42" s="46"/>
-      <c r="BI42" s="46"/>
-      <c r="BJ42" s="46"/>
-      <c r="BK42" s="46"/>
-      <c r="BL42" s="46"/>
-      <c r="BM42" s="46"/>
-      <c r="BN42" s="46"/>
-      <c r="BO42" s="46"/>
-      <c r="BP42" s="46"/>
-      <c r="BQ42" s="46"/>
-      <c r="BR42" s="46"/>
-      <c r="BS42" s="46"/>
-      <c r="BT42" s="46"/>
-      <c r="BU42" s="46"/>
-      <c r="BV42" s="46"/>
-      <c r="BW42" s="46"/>
-      <c r="BX42" s="46"/>
-      <c r="BY42" s="46"/>
-      <c r="BZ42" s="46"/>
-      <c r="CA42" s="46"/>
-      <c r="CB42" s="46"/>
-      <c r="CC42" s="46"/>
-      <c r="CD42" s="46"/>
-      <c r="CE42" s="46"/>
-      <c r="CF42" s="46"/>
-      <c r="CG42" s="46"/>
-      <c r="CH42" s="46"/>
-      <c r="CI42" s="46"/>
-      <c r="CJ42" s="46"/>
-      <c r="CK42" s="46"/>
-      <c r="CL42" s="46"/>
-      <c r="CM42" s="46"/>
-      <c r="CN42" s="46"/>
-      <c r="CO42" s="46"/>
-      <c r="CP42" s="46"/>
-      <c r="CQ42" s="46"/>
-      <c r="CR42" s="46"/>
-      <c r="CS42" s="46"/>
-      <c r="CT42" s="46"/>
-      <c r="CU42" s="46"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="31"/>
+      <c r="T42" s="31"/>
+      <c r="U42" s="31"/>
+      <c r="V42" s="31"/>
+      <c r="W42" s="31"/>
+      <c r="X42" s="31"/>
+      <c r="Y42" s="31"/>
+      <c r="Z42" s="31"/>
+      <c r="AA42" s="31"/>
+      <c r="AB42" s="31"/>
+      <c r="AC42" s="31"/>
+      <c r="BQ42" s="33"/>
+      <c r="BR42" s="34"/>
+      <c r="BS42" s="33"/>
+      <c r="BT42" s="33"/>
+      <c r="BU42" s="33"/>
+      <c r="BV42" s="33"/>
+      <c r="BW42" s="33"/>
+      <c r="BX42" s="33"/>
+      <c r="BY42" s="33"/>
+      <c r="BZ42" s="33"/>
+      <c r="CA42" s="33"/>
+      <c r="CB42" s="33"/>
+      <c r="CC42" s="33"/>
+      <c r="CD42" s="33"/>
+      <c r="CE42" s="33"/>
+      <c r="CF42" s="33"/>
+      <c r="CG42" s="33"/>
+      <c r="CH42" s="35"/>
+      <c r="CI42" s="35"/>
+      <c r="CJ42" s="35"/>
+      <c r="CK42" s="35"/>
+      <c r="CL42" s="35"/>
+      <c r="CM42" s="35"/>
+      <c r="CN42" s="35"/>
+      <c r="CO42" s="35"/>
+      <c r="CP42" s="35"/>
+      <c r="CQ42" s="35"/>
+      <c r="CR42" s="35"/>
+      <c r="CS42" s="35"/>
+      <c r="CT42" s="35"/>
+      <c r="CU42" s="35"/>
     </row>
     <row r="43" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C43" s="41">
+      <c r="B43" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="29">
         <v>56</v>
       </c>
-      <c r="D43" s="41">
-        <v>15</v>
-      </c>
-      <c r="E43" s="41">
+      <c r="D43" s="29">
+        <v>3</v>
+      </c>
+      <c r="E43" s="29">
         <v>56</v>
       </c>
-      <c r="F43" s="41">
-        <v>15</v>
+      <c r="F43" s="29">
+        <v>3</v>
       </c>
       <c r="G43" s="30">
         <v>0</v>
       </c>
-      <c r="H43" s="24"/>
+      <c r="H43" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="I43" s="31"/>
       <c r="J43" s="31"/>
       <c r="K43" s="31"/>
@@ -4976,16 +4967,16 @@
     </row>
     <row r="44" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="38" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C44" s="29">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D44" s="29">
         <v>3</v>
       </c>
       <c r="E44" s="29">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F44" s="29">
         <v>3</v>
@@ -5051,25 +5042,25 @@
     </row>
     <row r="45" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="38" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C45" s="29">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D45" s="29">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E45" s="29">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F45" s="29">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G45" s="30">
         <v>0</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I45" s="31"/>
       <c r="J45" s="31"/>
@@ -5126,26 +5117,24 @@
     </row>
     <row r="46" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="38" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C46" s="29">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D46" s="29">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E46" s="29">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="F46" s="29">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G46" s="30">
         <v>0</v>
       </c>
-      <c r="H46" s="24" t="s">
-        <v>82</v>
-      </c>
+      <c r="H46" s="24"/>
       <c r="I46" s="31"/>
       <c r="J46" s="31"/>
       <c r="K46" s="31"/>
@@ -5199,96 +5188,121 @@
       <c r="CT46" s="35"/>
       <c r="CU46" s="35"/>
     </row>
-    <row r="47" spans="1:99" s="28" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="29">
-        <v>56</v>
-      </c>
-      <c r="D47" s="29">
-        <v>15</v>
-      </c>
-      <c r="E47" s="29">
-        <v>56</v>
-      </c>
-      <c r="F47" s="29">
-        <v>15</v>
-      </c>
-      <c r="G47" s="30">
-        <v>0</v>
-      </c>
-      <c r="H47" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="31"/>
-      <c r="P47" s="31"/>
-      <c r="Q47" s="31"/>
-      <c r="R47" s="31"/>
-      <c r="S47" s="31"/>
-      <c r="T47" s="31"/>
-      <c r="U47" s="31"/>
-      <c r="V47" s="31"/>
-      <c r="W47" s="31"/>
-      <c r="X47" s="31"/>
-      <c r="Y47" s="31"/>
-      <c r="Z47" s="31"/>
-      <c r="AA47" s="31"/>
-      <c r="AB47" s="31"/>
-      <c r="AC47" s="31"/>
-      <c r="BQ47" s="33"/>
-      <c r="BR47" s="34"/>
-      <c r="BS47" s="33"/>
-      <c r="BT47" s="33"/>
-      <c r="BU47" s="33"/>
-      <c r="BV47" s="33"/>
-      <c r="BW47" s="33"/>
-      <c r="BX47" s="33"/>
-      <c r="BY47" s="33"/>
-      <c r="BZ47" s="33"/>
-      <c r="CA47" s="33"/>
-      <c r="CB47" s="33"/>
-      <c r="CC47" s="33"/>
-      <c r="CD47" s="33"/>
-      <c r="CE47" s="33"/>
-      <c r="CF47" s="33"/>
-      <c r="CG47" s="33"/>
-      <c r="CH47" s="35"/>
-      <c r="CI47" s="35"/>
-      <c r="CJ47" s="35"/>
-      <c r="CK47" s="35"/>
-      <c r="CL47" s="35"/>
-      <c r="CM47" s="35"/>
-      <c r="CN47" s="35"/>
-      <c r="CO47" s="35"/>
-      <c r="CP47" s="35"/>
-      <c r="CQ47" s="35"/>
-      <c r="CR47" s="35"/>
-      <c r="CS47" s="35"/>
-      <c r="CT47" s="35"/>
-      <c r="CU47" s="35"/>
+    <row r="47" spans="1:99" s="44" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="46"/>
+      <c r="N47" s="46"/>
+      <c r="O47" s="46"/>
+      <c r="P47" s="46"/>
+      <c r="Q47" s="46"/>
+      <c r="R47" s="46"/>
+      <c r="S47" s="46"/>
+      <c r="T47" s="46"/>
+      <c r="U47" s="46"/>
+      <c r="V47" s="46"/>
+      <c r="W47" s="46"/>
+      <c r="X47" s="46"/>
+      <c r="Y47" s="46"/>
+      <c r="Z47" s="46"/>
+      <c r="AA47" s="46"/>
+      <c r="AB47" s="46"/>
+      <c r="AC47" s="46"/>
+      <c r="AD47" s="46"/>
+      <c r="AE47" s="46"/>
+      <c r="AF47" s="46"/>
+      <c r="AG47" s="46"/>
+      <c r="AH47" s="46"/>
+      <c r="AI47" s="46"/>
+      <c r="AJ47" s="46"/>
+      <c r="AK47" s="46"/>
+      <c r="AL47" s="46"/>
+      <c r="AM47" s="46"/>
+      <c r="AN47" s="46"/>
+      <c r="AO47" s="46"/>
+      <c r="AP47" s="46"/>
+      <c r="AQ47" s="46"/>
+      <c r="AR47" s="46"/>
+      <c r="AS47" s="46"/>
+      <c r="AT47" s="46"/>
+      <c r="AU47" s="46"/>
+      <c r="AV47" s="46"/>
+      <c r="AW47" s="46"/>
+      <c r="AX47" s="46"/>
+      <c r="AY47" s="46"/>
+      <c r="AZ47" s="46"/>
+      <c r="BA47" s="46"/>
+      <c r="BB47" s="46"/>
+      <c r="BC47" s="46"/>
+      <c r="BD47" s="46"/>
+      <c r="BE47" s="46"/>
+      <c r="BF47" s="46"/>
+      <c r="BG47" s="46"/>
+      <c r="BH47" s="46"/>
+      <c r="BI47" s="46"/>
+      <c r="BJ47" s="46"/>
+      <c r="BK47" s="46"/>
+      <c r="BL47" s="46"/>
+      <c r="BM47" s="46"/>
+      <c r="BN47" s="46"/>
+      <c r="BO47" s="46"/>
+      <c r="BP47" s="46"/>
+      <c r="BQ47" s="46"/>
+      <c r="BR47" s="46"/>
+      <c r="BS47" s="46"/>
+      <c r="BT47" s="46"/>
+      <c r="BU47" s="46"/>
+      <c r="BV47" s="46"/>
+      <c r="BW47" s="46"/>
+      <c r="BX47" s="46"/>
+      <c r="BY47" s="46"/>
+      <c r="BZ47" s="46"/>
+      <c r="CA47" s="46"/>
+      <c r="CB47" s="46"/>
+      <c r="CC47" s="46"/>
+      <c r="CD47" s="46"/>
+      <c r="CE47" s="46"/>
+      <c r="CF47" s="46"/>
+      <c r="CG47" s="46"/>
+      <c r="CH47" s="46"/>
+      <c r="CI47" s="46"/>
+      <c r="CJ47" s="46"/>
+      <c r="CK47" s="46"/>
+      <c r="CL47" s="46"/>
+      <c r="CM47" s="46"/>
+      <c r="CN47" s="46"/>
+      <c r="CO47" s="46"/>
+      <c r="CP47" s="46"/>
+      <c r="CQ47" s="46"/>
+      <c r="CR47" s="46"/>
+      <c r="CS47" s="46"/>
+      <c r="CT47" s="46"/>
+      <c r="CU47" s="46"/>
     </row>
     <row r="48" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="29">
-        <v>68</v>
-      </c>
-      <c r="D48" s="29">
-        <v>3</v>
-      </c>
-      <c r="E48" s="29">
-        <v>68</v>
-      </c>
-      <c r="F48" s="29">
-        <v>3</v>
+      <c r="B48" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="41">
+        <v>71</v>
+      </c>
+      <c r="D48" s="41">
+        <v>10</v>
+      </c>
+      <c r="E48" s="41">
+        <v>71</v>
+      </c>
+      <c r="F48" s="41">
+        <v>10</v>
       </c>
       <c r="G48" s="30">
         <v>0</v>
@@ -5347,194 +5361,195 @@
       <c r="CT48" s="35"/>
       <c r="CU48" s="35"/>
     </row>
-    <row r="49" spans="1:99" s="44" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="46"/>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="46"/>
-      <c r="H49" s="46"/>
-      <c r="I49" s="46"/>
-      <c r="J49" s="46"/>
-      <c r="K49" s="46"/>
-      <c r="L49" s="46"/>
-      <c r="M49" s="46"/>
-      <c r="N49" s="46"/>
-      <c r="O49" s="46"/>
-      <c r="P49" s="46"/>
-      <c r="Q49" s="46"/>
-      <c r="R49" s="46"/>
-      <c r="S49" s="46"/>
-      <c r="T49" s="46"/>
-      <c r="U49" s="46"/>
-      <c r="V49" s="46"/>
-      <c r="W49" s="46"/>
-      <c r="X49" s="46"/>
-      <c r="Y49" s="46"/>
-      <c r="Z49" s="46"/>
-      <c r="AA49" s="46"/>
-      <c r="AB49" s="46"/>
-      <c r="AC49" s="46"/>
-      <c r="AD49" s="46"/>
-      <c r="AE49" s="46"/>
-      <c r="AF49" s="46"/>
-      <c r="AG49" s="46"/>
-      <c r="AH49" s="46"/>
-      <c r="AI49" s="46"/>
-      <c r="AJ49" s="46"/>
-      <c r="AK49" s="46"/>
-      <c r="AL49" s="46"/>
-      <c r="AM49" s="46"/>
-      <c r="AN49" s="46"/>
-      <c r="AO49" s="46"/>
-      <c r="AP49" s="46"/>
-      <c r="AQ49" s="46"/>
-      <c r="AR49" s="46"/>
-      <c r="AS49" s="46"/>
-      <c r="AT49" s="46"/>
-      <c r="AU49" s="46"/>
-      <c r="AV49" s="46"/>
-      <c r="AW49" s="46"/>
-      <c r="AX49" s="46"/>
-      <c r="AY49" s="46"/>
-      <c r="AZ49" s="46"/>
-      <c r="BA49" s="46"/>
-      <c r="BB49" s="46"/>
-      <c r="BC49" s="46"/>
-      <c r="BD49" s="46"/>
-      <c r="BE49" s="46"/>
-      <c r="BF49" s="46"/>
-      <c r="BG49" s="46"/>
-      <c r="BH49" s="46"/>
-      <c r="BI49" s="46"/>
-      <c r="BJ49" s="46"/>
-      <c r="BK49" s="46"/>
-      <c r="BL49" s="46"/>
-      <c r="BM49" s="46"/>
-      <c r="BN49" s="46"/>
-      <c r="BO49" s="46"/>
-      <c r="BP49" s="46"/>
-      <c r="BQ49" s="46"/>
-      <c r="BR49" s="46"/>
-      <c r="BS49" s="46"/>
-      <c r="BT49" s="46"/>
-      <c r="BU49" s="46"/>
-      <c r="BV49" s="46"/>
-      <c r="BW49" s="46"/>
-      <c r="BX49" s="46"/>
-      <c r="BY49" s="46"/>
-      <c r="BZ49" s="46"/>
-      <c r="CA49" s="46"/>
-      <c r="CB49" s="46"/>
-      <c r="CC49" s="46"/>
-      <c r="CD49" s="46"/>
-      <c r="CE49" s="46"/>
-      <c r="CF49" s="46"/>
-      <c r="CG49" s="46"/>
-      <c r="CH49" s="46"/>
-      <c r="CI49" s="46"/>
-      <c r="CJ49" s="46"/>
-      <c r="CK49" s="46"/>
-      <c r="CL49" s="46"/>
-      <c r="CM49" s="46"/>
-      <c r="CN49" s="46"/>
-      <c r="CO49" s="46"/>
-      <c r="CP49" s="46"/>
-      <c r="CQ49" s="46"/>
-      <c r="CR49" s="46"/>
-      <c r="CS49" s="46"/>
-      <c r="CT49" s="46"/>
-      <c r="CU49" s="46"/>
-    </row>
-    <row r="50" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" s="41">
+    <row r="49" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="29">
         <v>71</v>
       </c>
-      <c r="D50" s="41">
+      <c r="D49" s="29">
         <v>10</v>
       </c>
-      <c r="E50" s="41">
+      <c r="E49" s="29">
         <v>71</v>
       </c>
-      <c r="F50" s="41">
+      <c r="F49" s="29">
         <v>10</v>
       </c>
-      <c r="G50" s="30">
+      <c r="G49" s="30">
         <v>0</v>
       </c>
-      <c r="H50" s="24"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="31"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
-      <c r="M50" s="31"/>
-      <c r="N50" s="31"/>
-      <c r="O50" s="31"/>
-      <c r="P50" s="31"/>
-      <c r="Q50" s="31"/>
-      <c r="R50" s="31"/>
-      <c r="S50" s="31"/>
-      <c r="T50" s="31"/>
-      <c r="U50" s="31"/>
-      <c r="V50" s="31"/>
-      <c r="W50" s="31"/>
-      <c r="X50" s="31"/>
-      <c r="Y50" s="31"/>
-      <c r="Z50" s="31"/>
-      <c r="AA50" s="31"/>
-      <c r="AB50" s="31"/>
-      <c r="AC50" s="31"/>
-      <c r="BQ50" s="33"/>
-      <c r="BR50" s="34"/>
-      <c r="BS50" s="33"/>
-      <c r="BT50" s="33"/>
-      <c r="BU50" s="33"/>
-      <c r="BV50" s="33"/>
-      <c r="BW50" s="33"/>
-      <c r="BX50" s="33"/>
-      <c r="BY50" s="33"/>
-      <c r="BZ50" s="33"/>
-      <c r="CA50" s="33"/>
-      <c r="CB50" s="33"/>
-      <c r="CC50" s="33"/>
-      <c r="CD50" s="33"/>
-      <c r="CE50" s="33"/>
-      <c r="CF50" s="33"/>
-      <c r="CG50" s="33"/>
-      <c r="CH50" s="35"/>
-      <c r="CI50" s="35"/>
-      <c r="CJ50" s="35"/>
-      <c r="CK50" s="35"/>
-      <c r="CL50" s="35"/>
-      <c r="CM50" s="35"/>
-      <c r="CN50" s="35"/>
-      <c r="CO50" s="35"/>
-      <c r="CP50" s="35"/>
-      <c r="CQ50" s="35"/>
-      <c r="CR50" s="35"/>
-      <c r="CS50" s="35"/>
-      <c r="CT50" s="35"/>
-      <c r="CU50" s="35"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31"/>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="31"/>
+      <c r="S49" s="31"/>
+      <c r="T49" s="31"/>
+      <c r="U49" s="31"/>
+      <c r="V49" s="31"/>
+      <c r="W49" s="31"/>
+      <c r="X49" s="31"/>
+      <c r="Y49" s="31"/>
+      <c r="Z49" s="31"/>
+      <c r="AA49" s="31"/>
+      <c r="AB49" s="31"/>
+      <c r="AC49" s="31"/>
+      <c r="BQ49" s="33"/>
+      <c r="BR49" s="34"/>
+      <c r="BS49" s="33"/>
+      <c r="BT49" s="33"/>
+      <c r="BU49" s="33"/>
+      <c r="BV49" s="33"/>
+      <c r="BW49" s="33"/>
+      <c r="BX49" s="33"/>
+      <c r="BY49" s="33"/>
+      <c r="BZ49" s="33"/>
+      <c r="CA49" s="33"/>
+      <c r="CB49" s="33"/>
+      <c r="CC49" s="33"/>
+      <c r="CD49" s="33"/>
+      <c r="CE49" s="33"/>
+      <c r="CF49" s="33"/>
+      <c r="CG49" s="33"/>
+      <c r="CH49" s="35"/>
+      <c r="CI49" s="35"/>
+      <c r="CJ49" s="35"/>
+      <c r="CK49" s="35"/>
+      <c r="CL49" s="35"/>
+      <c r="CM49" s="35"/>
+      <c r="CN49" s="35"/>
+      <c r="CO49" s="35"/>
+      <c r="CP49" s="35"/>
+      <c r="CQ49" s="35"/>
+      <c r="CR49" s="35"/>
+      <c r="CS49" s="35"/>
+      <c r="CT49" s="35"/>
+      <c r="CU49" s="35"/>
+    </row>
+    <row r="50" spans="1:99" s="44" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="46"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="46"/>
+      <c r="N50" s="46"/>
+      <c r="O50" s="46"/>
+      <c r="P50" s="46"/>
+      <c r="Q50" s="46"/>
+      <c r="R50" s="46"/>
+      <c r="S50" s="46"/>
+      <c r="T50" s="46"/>
+      <c r="U50" s="46"/>
+      <c r="V50" s="46"/>
+      <c r="W50" s="46"/>
+      <c r="X50" s="46"/>
+      <c r="Y50" s="46"/>
+      <c r="Z50" s="46"/>
+      <c r="AA50" s="46"/>
+      <c r="AB50" s="46"/>
+      <c r="AC50" s="46"/>
+      <c r="AD50" s="46"/>
+      <c r="AE50" s="46"/>
+      <c r="AF50" s="46"/>
+      <c r="AG50" s="46"/>
+      <c r="AH50" s="46"/>
+      <c r="AI50" s="46"/>
+      <c r="AJ50" s="46"/>
+      <c r="AK50" s="46"/>
+      <c r="AL50" s="46"/>
+      <c r="AM50" s="46"/>
+      <c r="AN50" s="46"/>
+      <c r="AO50" s="46"/>
+      <c r="AP50" s="46"/>
+      <c r="AQ50" s="46"/>
+      <c r="AR50" s="46"/>
+      <c r="AS50" s="46"/>
+      <c r="AT50" s="46"/>
+      <c r="AU50" s="46"/>
+      <c r="AV50" s="46"/>
+      <c r="AW50" s="46"/>
+      <c r="AX50" s="46"/>
+      <c r="AY50" s="46"/>
+      <c r="AZ50" s="46"/>
+      <c r="BA50" s="46"/>
+      <c r="BB50" s="46"/>
+      <c r="BC50" s="46"/>
+      <c r="BD50" s="46"/>
+      <c r="BE50" s="46"/>
+      <c r="BF50" s="46"/>
+      <c r="BG50" s="46"/>
+      <c r="BH50" s="46"/>
+      <c r="BI50" s="46"/>
+      <c r="BJ50" s="46"/>
+      <c r="BK50" s="46"/>
+      <c r="BL50" s="46"/>
+      <c r="BM50" s="46"/>
+      <c r="BN50" s="46"/>
+      <c r="BO50" s="46"/>
+      <c r="BP50" s="46"/>
+      <c r="BQ50" s="46"/>
+      <c r="BR50" s="46"/>
+      <c r="BS50" s="46"/>
+      <c r="BT50" s="46"/>
+      <c r="BU50" s="46"/>
+      <c r="BV50" s="46"/>
+      <c r="BW50" s="46"/>
+      <c r="BX50" s="46"/>
+      <c r="BY50" s="46"/>
+      <c r="BZ50" s="46"/>
+      <c r="CA50" s="46"/>
+      <c r="CB50" s="46"/>
+      <c r="CC50" s="46"/>
+      <c r="CD50" s="46"/>
+      <c r="CE50" s="46"/>
+      <c r="CF50" s="46"/>
+      <c r="CG50" s="46"/>
+      <c r="CH50" s="46"/>
+      <c r="CI50" s="46"/>
+      <c r="CJ50" s="46"/>
+      <c r="CK50" s="46"/>
+      <c r="CL50" s="46"/>
+      <c r="CM50" s="46"/>
+      <c r="CN50" s="46"/>
+      <c r="CO50" s="46"/>
+      <c r="CP50" s="46"/>
+      <c r="CQ50" s="46"/>
+      <c r="CR50" s="46"/>
+      <c r="CS50" s="46"/>
+      <c r="CT50" s="46"/>
+      <c r="CU50" s="46"/>
     </row>
     <row r="51" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="C51" s="29">
-        <v>71</v>
-      </c>
-      <c r="D51" s="29">
-        <v>10</v>
-      </c>
-      <c r="E51" s="29">
-        <v>71</v>
-      </c>
-      <c r="F51" s="29">
-        <v>10</v>
+      <c r="B51" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="41">
+        <v>81</v>
+      </c>
+      <c r="D51" s="41">
+        <v>5</v>
+      </c>
+      <c r="E51" s="41">
+        <v>81</v>
+      </c>
+      <c r="F51" s="41">
+        <v>5</v>
       </c>
       <c r="G51" s="30">
         <v>0</v>
@@ -5593,122 +5608,94 @@
       <c r="CT51" s="35"/>
       <c r="CU51" s="35"/>
     </row>
-    <row r="52" spans="1:99" s="44" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="46"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="46"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="46"/>
-      <c r="M52" s="46"/>
-      <c r="N52" s="46"/>
-      <c r="O52" s="46"/>
-      <c r="P52" s="46"/>
-      <c r="Q52" s="46"/>
-      <c r="R52" s="46"/>
-      <c r="S52" s="46"/>
-      <c r="T52" s="46"/>
-      <c r="U52" s="46"/>
-      <c r="V52" s="46"/>
-      <c r="W52" s="46"/>
-      <c r="X52" s="46"/>
-      <c r="Y52" s="46"/>
-      <c r="Z52" s="46"/>
-      <c r="AA52" s="46"/>
-      <c r="AB52" s="46"/>
-      <c r="AC52" s="46"/>
-      <c r="AD52" s="46"/>
-      <c r="AE52" s="46"/>
-      <c r="AF52" s="46"/>
-      <c r="AG52" s="46"/>
-      <c r="AH52" s="46"/>
-      <c r="AI52" s="46"/>
-      <c r="AJ52" s="46"/>
-      <c r="AK52" s="46"/>
-      <c r="AL52" s="46"/>
-      <c r="AM52" s="46"/>
-      <c r="AN52" s="46"/>
-      <c r="AO52" s="46"/>
-      <c r="AP52" s="46"/>
-      <c r="AQ52" s="46"/>
-      <c r="AR52" s="46"/>
-      <c r="AS52" s="46"/>
-      <c r="AT52" s="46"/>
-      <c r="AU52" s="46"/>
-      <c r="AV52" s="46"/>
-      <c r="AW52" s="46"/>
-      <c r="AX52" s="46"/>
-      <c r="AY52" s="46"/>
-      <c r="AZ52" s="46"/>
-      <c r="BA52" s="46"/>
-      <c r="BB52" s="46"/>
-      <c r="BC52" s="46"/>
-      <c r="BD52" s="46"/>
-      <c r="BE52" s="46"/>
-      <c r="BF52" s="46"/>
-      <c r="BG52" s="46"/>
-      <c r="BH52" s="46"/>
-      <c r="BI52" s="46"/>
-      <c r="BJ52" s="46"/>
-      <c r="BK52" s="46"/>
-      <c r="BL52" s="46"/>
-      <c r="BM52" s="46"/>
-      <c r="BN52" s="46"/>
-      <c r="BO52" s="46"/>
-      <c r="BP52" s="46"/>
-      <c r="BQ52" s="46"/>
-      <c r="BR52" s="46"/>
-      <c r="BS52" s="46"/>
-      <c r="BT52" s="46"/>
-      <c r="BU52" s="46"/>
-      <c r="BV52" s="46"/>
-      <c r="BW52" s="46"/>
-      <c r="BX52" s="46"/>
-      <c r="BY52" s="46"/>
-      <c r="BZ52" s="46"/>
-      <c r="CA52" s="46"/>
-      <c r="CB52" s="46"/>
-      <c r="CC52" s="46"/>
-      <c r="CD52" s="46"/>
-      <c r="CE52" s="46"/>
-      <c r="CF52" s="46"/>
-      <c r="CG52" s="46"/>
-      <c r="CH52" s="46"/>
-      <c r="CI52" s="46"/>
-      <c r="CJ52" s="46"/>
-      <c r="CK52" s="46"/>
-      <c r="CL52" s="46"/>
-      <c r="CM52" s="46"/>
-      <c r="CN52" s="46"/>
-      <c r="CO52" s="46"/>
-      <c r="CP52" s="46"/>
-      <c r="CQ52" s="46"/>
-      <c r="CR52" s="46"/>
-      <c r="CS52" s="46"/>
-      <c r="CT52" s="46"/>
-      <c r="CU52" s="46"/>
+    <row r="52" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="29">
+        <v>81</v>
+      </c>
+      <c r="D52" s="29">
+        <v>3</v>
+      </c>
+      <c r="E52" s="29">
+        <v>81</v>
+      </c>
+      <c r="F52" s="29">
+        <v>3</v>
+      </c>
+      <c r="G52" s="30">
+        <v>0</v>
+      </c>
+      <c r="H52" s="24"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="31"/>
+      <c r="K52" s="31"/>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
+      <c r="N52" s="31"/>
+      <c r="O52" s="31"/>
+      <c r="P52" s="31"/>
+      <c r="Q52" s="31"/>
+      <c r="R52" s="31"/>
+      <c r="S52" s="31"/>
+      <c r="T52" s="31"/>
+      <c r="U52" s="31"/>
+      <c r="V52" s="31"/>
+      <c r="W52" s="31"/>
+      <c r="X52" s="31"/>
+      <c r="Y52" s="31"/>
+      <c r="Z52" s="31"/>
+      <c r="AA52" s="31"/>
+      <c r="AB52" s="31"/>
+      <c r="AC52" s="31"/>
+      <c r="BQ52" s="33"/>
+      <c r="BR52" s="34"/>
+      <c r="BS52" s="33"/>
+      <c r="BT52" s="33"/>
+      <c r="BU52" s="33"/>
+      <c r="BV52" s="33"/>
+      <c r="BW52" s="33"/>
+      <c r="BX52" s="33"/>
+      <c r="BY52" s="33"/>
+      <c r="BZ52" s="33"/>
+      <c r="CA52" s="33"/>
+      <c r="CB52" s="33"/>
+      <c r="CC52" s="33"/>
+      <c r="CD52" s="33"/>
+      <c r="CE52" s="33"/>
+      <c r="CF52" s="33"/>
+      <c r="CG52" s="33"/>
+      <c r="CH52" s="35"/>
+      <c r="CI52" s="35"/>
+      <c r="CJ52" s="35"/>
+      <c r="CK52" s="35"/>
+      <c r="CL52" s="35"/>
+      <c r="CM52" s="35"/>
+      <c r="CN52" s="35"/>
+      <c r="CO52" s="35"/>
+      <c r="CP52" s="35"/>
+      <c r="CQ52" s="35"/>
+      <c r="CR52" s="35"/>
+      <c r="CS52" s="35"/>
+      <c r="CT52" s="35"/>
+      <c r="CU52" s="35"/>
     </row>
     <row r="53" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C53" s="41">
-        <v>81</v>
-      </c>
-      <c r="D53" s="41">
-        <v>5</v>
-      </c>
-      <c r="E53" s="41">
-        <v>81</v>
-      </c>
-      <c r="F53" s="41">
-        <v>5</v>
+      <c r="B53" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="29">
+        <v>84</v>
+      </c>
+      <c r="D53" s="29">
+        <v>2</v>
+      </c>
+      <c r="E53" s="29">
+        <v>84</v>
+      </c>
+      <c r="F53" s="29">
+        <v>2</v>
       </c>
       <c r="G53" s="30">
         <v>0</v>
@@ -5768,20 +5755,20 @@
       <c r="CU53" s="35"/>
     </row>
     <row r="54" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="39" t="s">
-        <v>92</v>
+      <c r="B54" s="38" t="s">
+        <v>101</v>
       </c>
       <c r="C54" s="29">
         <v>81</v>
       </c>
       <c r="D54" s="29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E54" s="29">
         <v>81</v>
       </c>
       <c r="F54" s="29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G54" s="30">
         <v>0</v>
@@ -5840,97 +5827,125 @@
       <c r="CT54" s="35"/>
       <c r="CU54" s="35"/>
     </row>
-    <row r="55" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="C55" s="29">
-        <v>84</v>
-      </c>
-      <c r="D55" s="29">
-        <v>2</v>
-      </c>
-      <c r="E55" s="29">
-        <v>84</v>
-      </c>
-      <c r="F55" s="29">
-        <v>2</v>
-      </c>
-      <c r="G55" s="30">
-        <v>0</v>
-      </c>
-      <c r="H55" s="24"/>
-      <c r="I55" s="31"/>
-      <c r="J55" s="31"/>
-      <c r="K55" s="31"/>
-      <c r="L55" s="31"/>
-      <c r="M55" s="31"/>
-      <c r="N55" s="31"/>
-      <c r="O55" s="31"/>
-      <c r="P55" s="31"/>
-      <c r="Q55" s="31"/>
-      <c r="R55" s="31"/>
-      <c r="S55" s="31"/>
-      <c r="T55" s="31"/>
-      <c r="U55" s="31"/>
-      <c r="V55" s="31"/>
-      <c r="W55" s="31"/>
-      <c r="X55" s="31"/>
-      <c r="Y55" s="31"/>
-      <c r="Z55" s="31"/>
-      <c r="AA55" s="31"/>
-      <c r="AB55" s="31"/>
-      <c r="AC55" s="31"/>
-      <c r="BQ55" s="33"/>
-      <c r="BR55" s="34"/>
-      <c r="BS55" s="33"/>
-      <c r="BT55" s="33"/>
-      <c r="BU55" s="33"/>
-      <c r="BV55" s="33"/>
-      <c r="BW55" s="33"/>
-      <c r="BX55" s="33"/>
-      <c r="BY55" s="33"/>
-      <c r="BZ55" s="33"/>
-      <c r="CA55" s="33"/>
-      <c r="CB55" s="33"/>
-      <c r="CC55" s="33"/>
-      <c r="CD55" s="33"/>
-      <c r="CE55" s="33"/>
-      <c r="CF55" s="33"/>
-      <c r="CG55" s="33"/>
-      <c r="CH55" s="35"/>
-      <c r="CI55" s="35"/>
-      <c r="CJ55" s="35"/>
-      <c r="CK55" s="35"/>
-      <c r="CL55" s="35"/>
-      <c r="CM55" s="35"/>
-      <c r="CN55" s="35"/>
-      <c r="CO55" s="35"/>
-      <c r="CP55" s="35"/>
-      <c r="CQ55" s="35"/>
-      <c r="CR55" s="35"/>
-      <c r="CS55" s="35"/>
-      <c r="CT55" s="35"/>
-      <c r="CU55" s="35"/>
+    <row r="55" spans="1:99" s="44" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="46"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="46"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="46"/>
+      <c r="M55" s="46"/>
+      <c r="N55" s="46"/>
+      <c r="O55" s="46"/>
+      <c r="P55" s="46"/>
+      <c r="Q55" s="46"/>
+      <c r="R55" s="46"/>
+      <c r="S55" s="46"/>
+      <c r="T55" s="46"/>
+      <c r="U55" s="46"/>
+      <c r="V55" s="46"/>
+      <c r="W55" s="46"/>
+      <c r="X55" s="46"/>
+      <c r="Y55" s="46"/>
+      <c r="Z55" s="46"/>
+      <c r="AA55" s="46"/>
+      <c r="AB55" s="46"/>
+      <c r="AC55" s="46"/>
+      <c r="AD55" s="46"/>
+      <c r="AE55" s="46"/>
+      <c r="AF55" s="46"/>
+      <c r="AG55" s="46"/>
+      <c r="AH55" s="46"/>
+      <c r="AI55" s="46"/>
+      <c r="AJ55" s="46"/>
+      <c r="AK55" s="46"/>
+      <c r="AL55" s="46"/>
+      <c r="AM55" s="46"/>
+      <c r="AN55" s="46"/>
+      <c r="AO55" s="46"/>
+      <c r="AP55" s="46"/>
+      <c r="AQ55" s="46"/>
+      <c r="AR55" s="46"/>
+      <c r="AS55" s="46"/>
+      <c r="AT55" s="46"/>
+      <c r="AU55" s="46"/>
+      <c r="AV55" s="46"/>
+      <c r="AW55" s="46"/>
+      <c r="AX55" s="46"/>
+      <c r="AY55" s="46"/>
+      <c r="AZ55" s="46"/>
+      <c r="BA55" s="46"/>
+      <c r="BB55" s="46"/>
+      <c r="BC55" s="46"/>
+      <c r="BD55" s="46"/>
+      <c r="BE55" s="46"/>
+      <c r="BF55" s="46"/>
+      <c r="BG55" s="46"/>
+      <c r="BH55" s="46"/>
+      <c r="BI55" s="46"/>
+      <c r="BJ55" s="46"/>
+      <c r="BK55" s="46"/>
+      <c r="BL55" s="46"/>
+      <c r="BM55" s="46"/>
+      <c r="BN55" s="46"/>
+      <c r="BO55" s="46"/>
+      <c r="BP55" s="46"/>
+      <c r="BQ55" s="46"/>
+      <c r="BR55" s="46"/>
+      <c r="BS55" s="46"/>
+      <c r="BT55" s="46"/>
+      <c r="BU55" s="46"/>
+      <c r="BV55" s="46"/>
+      <c r="BW55" s="46"/>
+      <c r="BX55" s="46"/>
+      <c r="BY55" s="46"/>
+      <c r="BZ55" s="46"/>
+      <c r="CA55" s="46"/>
+      <c r="CB55" s="46"/>
+      <c r="CC55" s="46"/>
+      <c r="CD55" s="46"/>
+      <c r="CE55" s="46"/>
+      <c r="CF55" s="46"/>
+      <c r="CG55" s="46"/>
+      <c r="CH55" s="46"/>
+      <c r="CI55" s="46"/>
+      <c r="CJ55" s="46"/>
+      <c r="CK55" s="46"/>
+      <c r="CL55" s="46"/>
+      <c r="CM55" s="46"/>
+      <c r="CN55" s="46"/>
+      <c r="CO55" s="46"/>
+      <c r="CP55" s="46"/>
+      <c r="CQ55" s="46"/>
+      <c r="CR55" s="46"/>
+      <c r="CS55" s="46"/>
+      <c r="CT55" s="46"/>
+      <c r="CU55" s="46"/>
     </row>
     <row r="56" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" s="29">
-        <v>81</v>
-      </c>
-      <c r="D56" s="29">
-        <v>5</v>
-      </c>
-      <c r="E56" s="29">
-        <v>81</v>
-      </c>
-      <c r="F56" s="29">
-        <v>5</v>
+      <c r="B56" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="41">
+        <v>11</v>
+      </c>
+      <c r="D56" s="41">
+        <v>80</v>
+      </c>
+      <c r="E56" s="41">
+        <v>11</v>
+      </c>
+      <c r="F56" s="41">
+        <v>80</v>
       </c>
       <c r="G56" s="30">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H56" s="24"/>
       <c r="I56" s="31"/>
@@ -5986,125 +6001,99 @@
       <c r="CT56" s="35"/>
       <c r="CU56" s="35"/>
     </row>
-    <row r="57" spans="1:99" s="44" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="46"/>
-      <c r="B57" s="46"/>
-      <c r="C57" s="46"/>
-      <c r="D57" s="46"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="46"/>
-      <c r="H57" s="46"/>
-      <c r="I57" s="46"/>
-      <c r="J57" s="46"/>
-      <c r="K57" s="46"/>
-      <c r="L57" s="46"/>
-      <c r="M57" s="46"/>
-      <c r="N57" s="46"/>
-      <c r="O57" s="46"/>
-      <c r="P57" s="46"/>
-      <c r="Q57" s="46"/>
-      <c r="R57" s="46"/>
-      <c r="S57" s="46"/>
-      <c r="T57" s="46"/>
-      <c r="U57" s="46"/>
-      <c r="V57" s="46"/>
-      <c r="W57" s="46"/>
-      <c r="X57" s="46"/>
-      <c r="Y57" s="46"/>
-      <c r="Z57" s="46"/>
-      <c r="AA57" s="46"/>
-      <c r="AB57" s="46"/>
-      <c r="AC57" s="46"/>
-      <c r="AD57" s="46"/>
-      <c r="AE57" s="46"/>
-      <c r="AF57" s="46"/>
-      <c r="AG57" s="46"/>
-      <c r="AH57" s="46"/>
-      <c r="AI57" s="46"/>
-      <c r="AJ57" s="46"/>
-      <c r="AK57" s="46"/>
-      <c r="AL57" s="46"/>
-      <c r="AM57" s="46"/>
-      <c r="AN57" s="46"/>
-      <c r="AO57" s="46"/>
-      <c r="AP57" s="46"/>
-      <c r="AQ57" s="46"/>
-      <c r="AR57" s="46"/>
-      <c r="AS57" s="46"/>
-      <c r="AT57" s="46"/>
-      <c r="AU57" s="46"/>
-      <c r="AV57" s="46"/>
-      <c r="AW57" s="46"/>
-      <c r="AX57" s="46"/>
-      <c r="AY57" s="46"/>
-      <c r="AZ57" s="46"/>
-      <c r="BA57" s="46"/>
-      <c r="BB57" s="46"/>
-      <c r="BC57" s="46"/>
-      <c r="BD57" s="46"/>
-      <c r="BE57" s="46"/>
-      <c r="BF57" s="46"/>
-      <c r="BG57" s="46"/>
-      <c r="BH57" s="46"/>
-      <c r="BI57" s="46"/>
-      <c r="BJ57" s="46"/>
-      <c r="BK57" s="46"/>
-      <c r="BL57" s="46"/>
-      <c r="BM57" s="46"/>
-      <c r="BN57" s="46"/>
-      <c r="BO57" s="46"/>
-      <c r="BP57" s="46"/>
-      <c r="BQ57" s="46"/>
-      <c r="BR57" s="46"/>
-      <c r="BS57" s="46"/>
-      <c r="BT57" s="46"/>
-      <c r="BU57" s="46"/>
-      <c r="BV57" s="46"/>
-      <c r="BW57" s="46"/>
-      <c r="BX57" s="46"/>
-      <c r="BY57" s="46"/>
-      <c r="BZ57" s="46"/>
-      <c r="CA57" s="46"/>
-      <c r="CB57" s="46"/>
-      <c r="CC57" s="46"/>
-      <c r="CD57" s="46"/>
-      <c r="CE57" s="46"/>
-      <c r="CF57" s="46"/>
-      <c r="CG57" s="46"/>
-      <c r="CH57" s="46"/>
-      <c r="CI57" s="46"/>
-      <c r="CJ57" s="46"/>
-      <c r="CK57" s="46"/>
-      <c r="CL57" s="46"/>
-      <c r="CM57" s="46"/>
-      <c r="CN57" s="46"/>
-      <c r="CO57" s="46"/>
-      <c r="CP57" s="46"/>
-      <c r="CQ57" s="46"/>
-      <c r="CR57" s="46"/>
-      <c r="CS57" s="46"/>
-      <c r="CT57" s="46"/>
-      <c r="CU57" s="46"/>
+    <row r="57" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" s="41">
+        <v>11</v>
+      </c>
+      <c r="D57" s="41">
+        <v>2</v>
+      </c>
+      <c r="E57" s="41">
+        <v>11</v>
+      </c>
+      <c r="F57" s="41">
+        <v>2</v>
+      </c>
+      <c r="G57" s="30">
+        <v>1</v>
+      </c>
+      <c r="H57" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I57" s="31"/>
+      <c r="J57" s="31"/>
+      <c r="K57" s="31"/>
+      <c r="L57" s="31"/>
+      <c r="M57" s="31"/>
+      <c r="N57" s="31"/>
+      <c r="O57" s="31"/>
+      <c r="P57" s="31"/>
+      <c r="Q57" s="31"/>
+      <c r="R57" s="31"/>
+      <c r="S57" s="31"/>
+      <c r="T57" s="31"/>
+      <c r="U57" s="31"/>
+      <c r="V57" s="31"/>
+      <c r="W57" s="31"/>
+      <c r="X57" s="31"/>
+      <c r="Y57" s="31"/>
+      <c r="Z57" s="31"/>
+      <c r="AA57" s="31"/>
+      <c r="AB57" s="31"/>
+      <c r="AC57" s="31"/>
+      <c r="BQ57" s="33"/>
+      <c r="BR57" s="34"/>
+      <c r="BS57" s="33"/>
+      <c r="BT57" s="33"/>
+      <c r="BU57" s="33"/>
+      <c r="BV57" s="33"/>
+      <c r="BW57" s="33"/>
+      <c r="BX57" s="33"/>
+      <c r="BY57" s="33"/>
+      <c r="BZ57" s="33"/>
+      <c r="CA57" s="33"/>
+      <c r="CB57" s="33"/>
+      <c r="CC57" s="33"/>
+      <c r="CD57" s="33"/>
+      <c r="CE57" s="33"/>
+      <c r="CF57" s="33"/>
+      <c r="CG57" s="33"/>
+      <c r="CH57" s="35"/>
+      <c r="CI57" s="35"/>
+      <c r="CJ57" s="35"/>
+      <c r="CK57" s="35"/>
+      <c r="CL57" s="35"/>
+      <c r="CM57" s="35"/>
+      <c r="CN57" s="35"/>
+      <c r="CO57" s="35"/>
+      <c r="CP57" s="35"/>
+      <c r="CQ57" s="35"/>
+      <c r="CR57" s="35"/>
+      <c r="CS57" s="35"/>
+      <c r="CT57" s="35"/>
+      <c r="CU57" s="35"/>
     </row>
     <row r="58" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="18" t="s">
-        <v>66</v>
+      <c r="B58" s="38" t="s">
+        <v>105</v>
       </c>
       <c r="C58" s="41">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D58" s="41">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E58" s="41">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F58" s="41">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="G58" s="30">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="H58" s="24"/>
       <c r="I58" s="31"/>
@@ -6161,20 +6150,20 @@
       <c r="CU58" s="35"/>
     </row>
     <row r="59" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="38" t="s">
-        <v>105</v>
+      <c r="B59" s="40" t="s">
+        <v>110</v>
       </c>
       <c r="C59" s="41">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D59" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E59" s="41">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F59" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G59" s="30">
         <v>1</v>
@@ -6236,25 +6225,27 @@
       <c r="CU59" s="35"/>
     </row>
     <row r="60" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="38" t="s">
-        <v>108</v>
+      <c r="B60" s="40" t="s">
+        <v>111</v>
       </c>
       <c r="C60" s="41">
         <v>13</v>
       </c>
       <c r="D60" s="41">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E60" s="41">
         <v>13</v>
       </c>
       <c r="F60" s="41">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G60" s="30">
         <v>1</v>
       </c>
-      <c r="H60" s="24"/>
+      <c r="H60" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="I60" s="31"/>
       <c r="J60" s="31"/>
       <c r="K60" s="31"/>
@@ -6308,9 +6299,9 @@
       <c r="CT60" s="35"/>
       <c r="CU60" s="35"/>
     </row>
-    <row r="61" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:99" s="28" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C61" s="41">
         <v>13</v>
@@ -6328,7 +6319,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="24" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="I61" s="31"/>
       <c r="J61" s="31"/>
@@ -6385,26 +6376,24 @@
     </row>
     <row r="62" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C62" s="41">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D62" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E62" s="41">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F62" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G62" s="30">
         <v>1</v>
       </c>
-      <c r="H62" s="24" t="s">
-        <v>81</v>
-      </c>
+      <c r="H62" s="24"/>
       <c r="I62" s="31"/>
       <c r="J62" s="31"/>
       <c r="K62" s="31"/>
@@ -6458,18 +6447,18 @@
       <c r="CT62" s="35"/>
       <c r="CU62" s="35"/>
     </row>
-    <row r="63" spans="1:99" s="28" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C63" s="41">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D63" s="41">
         <v>3</v>
       </c>
       <c r="E63" s="41">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F63" s="41">
         <v>3</v>
@@ -6478,7 +6467,7 @@
         <v>1</v>
       </c>
       <c r="H63" s="24" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="I63" s="31"/>
       <c r="J63" s="31"/>
@@ -6535,24 +6524,26 @@
     </row>
     <row r="64" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C64" s="41">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D64" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E64" s="41">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F64" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G64" s="30">
         <v>1</v>
       </c>
-      <c r="H64" s="24"/>
+      <c r="H64" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="I64" s="31"/>
       <c r="J64" s="31"/>
       <c r="K64" s="31"/>
@@ -6608,7 +6599,7 @@
     </row>
     <row r="65" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C65" s="41">
         <v>17</v>
@@ -6626,7 +6617,7 @@
         <v>1</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I65" s="31"/>
       <c r="J65" s="31"/>
@@ -6683,26 +6674,24 @@
     </row>
     <row r="66" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C66" s="41">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D66" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E66" s="41">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F66" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G66" s="30">
         <v>1</v>
       </c>
-      <c r="H66" s="24" t="s">
-        <v>122</v>
-      </c>
+      <c r="H66" s="24"/>
       <c r="I66" s="31"/>
       <c r="J66" s="31"/>
       <c r="K66" s="31"/>
@@ -6758,26 +6747,24 @@
     </row>
     <row r="67" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C67" s="41">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D67" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E67" s="41">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F67" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G67" s="30">
         <v>1</v>
       </c>
-      <c r="H67" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="H67" s="24"/>
       <c r="I67" s="31"/>
       <c r="J67" s="31"/>
       <c r="K67" s="31"/>
@@ -6832,23 +6819,23 @@
       <c r="CU67" s="35"/>
     </row>
     <row r="68" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="40" t="s">
-        <v>120</v>
+      <c r="B68" s="38" t="s">
+        <v>106</v>
       </c>
       <c r="C68" s="41">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D68" s="41">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E68" s="41">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F68" s="41">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G68" s="30">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H68" s="24"/>
       <c r="I68" s="31"/>
@@ -6906,22 +6893,22 @@
     </row>
     <row r="69" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C69" s="41">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D69" s="41">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E69" s="41">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F69" s="41">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G69" s="30">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H69" s="24"/>
       <c r="I69" s="31"/>
@@ -6979,22 +6966,22 @@
     </row>
     <row r="70" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C70" s="41">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D70" s="41">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E70" s="41">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F70" s="41">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G70" s="30">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="H70" s="24"/>
       <c r="I70" s="31"/>
@@ -7051,23 +7038,23 @@
       <c r="CU70" s="35"/>
     </row>
     <row r="71" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="40" t="s">
-        <v>123</v>
+      <c r="B71" s="38" t="s">
+        <v>108</v>
       </c>
       <c r="C71" s="41">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D71" s="41">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E71" s="41">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="F71" s="41">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G71" s="30">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="H71" s="24"/>
       <c r="I71" s="31"/>
@@ -7125,22 +7112,22 @@
     </row>
     <row r="72" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C72" s="41">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="D72" s="41">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="E72" s="41">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="F72" s="41">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="G72" s="30">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H72" s="24"/>
       <c r="I72" s="31"/>
@@ -7198,19 +7185,19 @@
     </row>
     <row r="73" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="38" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C73" s="41">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D73" s="41">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E73" s="41">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="F73" s="41">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G73" s="30">
         <v>0</v>
@@ -7270,20 +7257,20 @@
       <c r="CU73" s="35"/>
     </row>
     <row r="74" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="38" t="s">
-        <v>112</v>
+      <c r="B74" s="39" t="s">
+        <v>104</v>
       </c>
       <c r="C74" s="41">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D74" s="41">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E74" s="41">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="F74" s="41">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G74" s="30">
         <v>0</v>
@@ -7342,154 +7329,82 @@
       <c r="CT74" s="35"/>
       <c r="CU74" s="35"/>
     </row>
-    <row r="75" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="C75" s="41">
-        <v>82</v>
-      </c>
-      <c r="D75" s="41">
-        <v>2</v>
-      </c>
-      <c r="E75" s="41">
-        <v>82</v>
-      </c>
-      <c r="F75" s="41">
-        <v>2</v>
-      </c>
-      <c r="G75" s="30">
-        <v>0</v>
-      </c>
-      <c r="H75" s="24"/>
-      <c r="I75" s="31"/>
-      <c r="J75" s="31"/>
-      <c r="K75" s="31"/>
-      <c r="L75" s="31"/>
-      <c r="M75" s="31"/>
-      <c r="N75" s="31"/>
-      <c r="O75" s="31"/>
-      <c r="P75" s="31"/>
-      <c r="Q75" s="31"/>
-      <c r="R75" s="31"/>
-      <c r="S75" s="31"/>
-      <c r="T75" s="31"/>
-      <c r="U75" s="31"/>
-      <c r="V75" s="31"/>
-      <c r="W75" s="31"/>
-      <c r="X75" s="31"/>
-      <c r="Y75" s="31"/>
-      <c r="Z75" s="31"/>
-      <c r="AA75" s="31"/>
-      <c r="AB75" s="31"/>
-      <c r="AC75" s="31"/>
-      <c r="BQ75" s="33"/>
-      <c r="BR75" s="34"/>
-      <c r="BS75" s="33"/>
-      <c r="BT75" s="33"/>
-      <c r="BU75" s="33"/>
-      <c r="BV75" s="33"/>
-      <c r="BW75" s="33"/>
-      <c r="BX75" s="33"/>
-      <c r="BY75" s="33"/>
-      <c r="BZ75" s="33"/>
-      <c r="CA75" s="33"/>
-      <c r="CB75" s="33"/>
-      <c r="CC75" s="33"/>
-      <c r="CD75" s="33"/>
-      <c r="CE75" s="33"/>
-      <c r="CF75" s="33"/>
-      <c r="CG75" s="33"/>
-      <c r="CH75" s="35"/>
-      <c r="CI75" s="35"/>
-      <c r="CJ75" s="35"/>
-      <c r="CK75" s="35"/>
-      <c r="CL75" s="35"/>
-      <c r="CM75" s="35"/>
-      <c r="CN75" s="35"/>
-      <c r="CO75" s="35"/>
-      <c r="CP75" s="35"/>
-      <c r="CQ75" s="35"/>
-      <c r="CR75" s="35"/>
-      <c r="CS75" s="35"/>
-      <c r="CT75" s="35"/>
-      <c r="CU75" s="35"/>
-    </row>
-    <row r="76" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C76" s="41">
-        <v>86</v>
-      </c>
-      <c r="D76" s="41">
-        <v>7</v>
-      </c>
-      <c r="E76" s="41">
-        <v>86</v>
-      </c>
-      <c r="F76" s="41">
-        <v>7</v>
-      </c>
-      <c r="G76" s="30">
-        <v>0</v>
-      </c>
-      <c r="H76" s="24"/>
-      <c r="I76" s="31"/>
-      <c r="J76" s="31"/>
-      <c r="K76" s="31"/>
-      <c r="L76" s="31"/>
-      <c r="M76" s="31"/>
-      <c r="N76" s="31"/>
-      <c r="O76" s="31"/>
-      <c r="P76" s="31"/>
-      <c r="Q76" s="31"/>
-      <c r="R76" s="31"/>
-      <c r="S76" s="31"/>
-      <c r="T76" s="31"/>
-      <c r="U76" s="31"/>
-      <c r="V76" s="31"/>
-      <c r="W76" s="31"/>
-      <c r="X76" s="31"/>
-      <c r="Y76" s="31"/>
-      <c r="Z76" s="31"/>
-      <c r="AA76" s="31"/>
-      <c r="AB76" s="31"/>
-      <c r="AC76" s="31"/>
-      <c r="BQ76" s="33"/>
-      <c r="BR76" s="34"/>
-      <c r="BS76" s="33"/>
-      <c r="BT76" s="33"/>
-      <c r="BU76" s="33"/>
-      <c r="BV76" s="33"/>
-      <c r="BW76" s="33"/>
-      <c r="BX76" s="33"/>
-      <c r="BY76" s="33"/>
-      <c r="BZ76" s="33"/>
-      <c r="CA76" s="33"/>
-      <c r="CB76" s="33"/>
-      <c r="CC76" s="33"/>
-      <c r="CD76" s="33"/>
-      <c r="CE76" s="33"/>
-      <c r="CF76" s="33"/>
-      <c r="CG76" s="33"/>
-      <c r="CH76" s="35"/>
-      <c r="CI76" s="35"/>
-      <c r="CJ76" s="35"/>
-      <c r="CK76" s="35"/>
-      <c r="CL76" s="35"/>
-      <c r="CM76" s="35"/>
-      <c r="CN76" s="35"/>
-      <c r="CO76" s="35"/>
-      <c r="CP76" s="35"/>
-      <c r="CQ76" s="35"/>
-      <c r="CR76" s="35"/>
-      <c r="CS76" s="35"/>
-      <c r="CT76" s="35"/>
-      <c r="CU76" s="35"/>
+    <row r="75" spans="2:99" x14ac:dyDescent="0.3">
+      <c r="H75" s="27"/>
+      <c r="J75" s="19"/>
+      <c r="K75" s="19"/>
+      <c r="L75" s="19"/>
+      <c r="M75" s="19"/>
+      <c r="N75" s="19"/>
+      <c r="O75" s="19"/>
+      <c r="P75" s="19"/>
+      <c r="Q75" s="19"/>
+      <c r="R75" s="19"/>
+      <c r="S75" s="19"/>
+      <c r="T75" s="19"/>
+      <c r="U75" s="19"/>
+      <c r="V75" s="19"/>
+      <c r="W75" s="19"/>
+      <c r="X75" s="19"/>
+      <c r="Y75" s="19"/>
+      <c r="Z75" s="19"/>
+      <c r="AA75" s="19"/>
+      <c r="AB75" s="19"/>
+      <c r="AC75" s="19"/>
+      <c r="BR75" s="21"/>
+      <c r="BS75" s="21"/>
+      <c r="BT75" s="21"/>
+      <c r="BU75" s="21"/>
+      <c r="BV75" s="21"/>
+      <c r="BW75" s="21"/>
+      <c r="BX75" s="21"/>
+      <c r="BY75" s="21"/>
+      <c r="BZ75" s="21"/>
+      <c r="CA75" s="21"/>
+      <c r="CB75" s="21"/>
+      <c r="CC75" s="21"/>
+      <c r="CD75" s="21"/>
+      <c r="CE75" s="21"/>
+      <c r="CF75" s="21"/>
+      <c r="CG75" s="21"/>
+      <c r="CH75" s="21"/>
+      <c r="CI75" s="21"/>
+      <c r="CJ75" s="21"/>
+      <c r="CK75" s="21"/>
+      <c r="CL75" s="21"/>
+      <c r="CM75" s="21"/>
+      <c r="CN75" s="21"/>
+      <c r="CO75" s="21"/>
+      <c r="CP75" s="21"/>
+      <c r="CQ75" s="21"/>
+      <c r="CR75" s="21"/>
+      <c r="CS75" s="21"/>
+      <c r="CT75" s="21"/>
+      <c r="CU75" s="21"/>
+    </row>
+    <row r="76" spans="2:99" x14ac:dyDescent="0.3">
+      <c r="J76" s="19"/>
+      <c r="K76" s="19"/>
+      <c r="L76" s="19"/>
+      <c r="M76" s="19"/>
+      <c r="N76" s="19"/>
+      <c r="O76" s="19"/>
+      <c r="P76" s="19"/>
+      <c r="Q76" s="19"/>
+      <c r="R76" s="19"/>
+      <c r="S76" s="19"/>
+      <c r="T76" s="19"/>
+      <c r="U76" s="19"/>
+      <c r="V76" s="19"/>
+      <c r="W76" s="19"/>
+      <c r="X76" s="19"/>
+      <c r="Y76" s="19"/>
+      <c r="Z76" s="19"/>
+      <c r="AA76" s="19"/>
+      <c r="AB76" s="19"/>
+      <c r="AC76" s="19"/>
     </row>
     <row r="77" spans="2:99" x14ac:dyDescent="0.3">
-      <c r="H77" s="27"/>
       <c r="J77" s="19"/>
       <c r="K77" s="19"/>
       <c r="L77" s="19"/>
@@ -7510,36 +7425,6 @@
       <c r="AA77" s="19"/>
       <c r="AB77" s="19"/>
       <c r="AC77" s="19"/>
-      <c r="BR77" s="21"/>
-      <c r="BS77" s="21"/>
-      <c r="BT77" s="21"/>
-      <c r="BU77" s="21"/>
-      <c r="BV77" s="21"/>
-      <c r="BW77" s="21"/>
-      <c r="BX77" s="21"/>
-      <c r="BY77" s="21"/>
-      <c r="BZ77" s="21"/>
-      <c r="CA77" s="21"/>
-      <c r="CB77" s="21"/>
-      <c r="CC77" s="21"/>
-      <c r="CD77" s="21"/>
-      <c r="CE77" s="21"/>
-      <c r="CF77" s="21"/>
-      <c r="CG77" s="21"/>
-      <c r="CH77" s="21"/>
-      <c r="CI77" s="21"/>
-      <c r="CJ77" s="21"/>
-      <c r="CK77" s="21"/>
-      <c r="CL77" s="21"/>
-      <c r="CM77" s="21"/>
-      <c r="CN77" s="21"/>
-      <c r="CO77" s="21"/>
-      <c r="CP77" s="21"/>
-      <c r="CQ77" s="21"/>
-      <c r="CR77" s="21"/>
-      <c r="CS77" s="21"/>
-      <c r="CT77" s="21"/>
-      <c r="CU77" s="21"/>
     </row>
     <row r="78" spans="2:99" x14ac:dyDescent="0.3">
       <c r="J78" s="19"/>
@@ -7651,67 +7536,24 @@
       <c r="AB82" s="19"/>
       <c r="AC82" s="19"/>
     </row>
-    <row r="83" spans="10:29" x14ac:dyDescent="0.3">
-      <c r="J83" s="19"/>
-      <c r="K83" s="19"/>
-      <c r="L83" s="19"/>
-      <c r="M83" s="19"/>
-      <c r="N83" s="19"/>
-      <c r="O83" s="19"/>
-      <c r="P83" s="19"/>
-      <c r="Q83" s="19"/>
-      <c r="R83" s="19"/>
-      <c r="S83" s="19"/>
-      <c r="T83" s="19"/>
-      <c r="U83" s="19"/>
-      <c r="V83" s="19"/>
-      <c r="W83" s="19"/>
-      <c r="X83" s="19"/>
-      <c r="Y83" s="19"/>
-      <c r="Z83" s="19"/>
-      <c r="AA83" s="19"/>
-      <c r="AB83" s="19"/>
-      <c r="AC83" s="19"/>
-    </row>
-    <row r="84" spans="10:29" x14ac:dyDescent="0.3">
-      <c r="J84" s="19"/>
-      <c r="K84" s="19"/>
-      <c r="L84" s="19"/>
-      <c r="M84" s="19"/>
-      <c r="N84" s="19"/>
-      <c r="O84" s="19"/>
-      <c r="P84" s="19"/>
-      <c r="Q84" s="19"/>
-      <c r="R84" s="19"/>
-      <c r="S84" s="19"/>
-      <c r="T84" s="19"/>
-      <c r="U84" s="19"/>
-      <c r="V84" s="19"/>
-      <c r="W84" s="19"/>
-      <c r="X84" s="19"/>
-      <c r="Y84" s="19"/>
-      <c r="Z84" s="19"/>
-      <c r="AA84" s="19"/>
-      <c r="AB84" s="19"/>
-      <c r="AC84" s="19"/>
-    </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A13:CU13"/>
-    <mergeCell ref="B21:CU21"/>
-    <mergeCell ref="B26:CU26"/>
-    <mergeCell ref="A31:CU31"/>
-    <mergeCell ref="A42:CU42"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="AD5:AH5"/>
-    <mergeCell ref="AD6:AH6"/>
-    <mergeCell ref="B2:G4"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="O6:S6"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A55:CU55"/>
+    <mergeCell ref="B47:CU47"/>
+    <mergeCell ref="A50:CU50"/>
+    <mergeCell ref="CQ5:CU5"/>
+    <mergeCell ref="CQ6:CU6"/>
+    <mergeCell ref="CL5:CP5"/>
+    <mergeCell ref="CL6:CP6"/>
+    <mergeCell ref="AX5:BB5"/>
+    <mergeCell ref="AX6:BB6"/>
+    <mergeCell ref="AI5:AM5"/>
+    <mergeCell ref="AI6:AM6"/>
+    <mergeCell ref="AN5:AR5"/>
+    <mergeCell ref="AN6:AR6"/>
+    <mergeCell ref="AS5:AW5"/>
+    <mergeCell ref="AS6:AW6"/>
+    <mergeCell ref="Y5:AC5"/>
     <mergeCell ref="BE2:BW2"/>
     <mergeCell ref="BE3:BW3"/>
     <mergeCell ref="CB5:CF5"/>
@@ -7728,24 +7570,23 @@
     <mergeCell ref="BC6:BG6"/>
     <mergeCell ref="BH5:BL5"/>
     <mergeCell ref="BH6:BL6"/>
-    <mergeCell ref="A57:CU57"/>
-    <mergeCell ref="B49:CU49"/>
-    <mergeCell ref="A52:CU52"/>
-    <mergeCell ref="CQ5:CU5"/>
-    <mergeCell ref="CQ6:CU6"/>
-    <mergeCell ref="CL5:CP5"/>
-    <mergeCell ref="CL6:CP6"/>
-    <mergeCell ref="AX5:BB5"/>
-    <mergeCell ref="AX6:BB6"/>
-    <mergeCell ref="AI5:AM5"/>
-    <mergeCell ref="AI6:AM6"/>
-    <mergeCell ref="AN5:AR5"/>
-    <mergeCell ref="AN6:AR6"/>
-    <mergeCell ref="AS5:AW5"/>
-    <mergeCell ref="AS6:AW6"/>
-    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="AD6:AH6"/>
+    <mergeCell ref="B2:G4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="O6:S6"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A13:CU13"/>
+    <mergeCell ref="B21:CU21"/>
+    <mergeCell ref="B26:CU26"/>
+    <mergeCell ref="A31:CU31"/>
+    <mergeCell ref="A41:CU41"/>
   </mergeCells>
-  <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J53:CU56 J50:CU51 J32:CU41 J43:CU48 J58:CU59 J75:CU75">
+  <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J51:CU54 J48:CU49 J56:CU57 J73:CU73 J32:CU40 J42:CU46">
     <cfRule type="expression" dxfId="25" priority="84">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -7771,7 +7612,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77:G77 I77:BQ77">
+  <conditionalFormatting sqref="B75:G75 I75:BQ75">
     <cfRule type="expression" dxfId="17" priority="85">
       <formula>TRUE</formula>
     </cfRule>
@@ -7781,7 +7622,7 @@
       <formula>J$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J76:CU76">
+  <conditionalFormatting sqref="J74:CU74">
     <cfRule type="expression" dxfId="15" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -7807,7 +7648,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J60:CU74">
+  <conditionalFormatting sqref="J58:CU72">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>

<commit_message>
projeto mecanico finalizado. AV01 completa
</commit_message>
<xml_diff>
--- a/LaTeX Project/Documentos/Gantt.xlsx
+++ b/LaTeX Project/Documentos/Gantt.xlsx
@@ -358,9 +358,6 @@
     <t>Desenvolver diagramas esquemáticos (hardware)</t>
   </si>
   <si>
-    <t>Desenvolver diagramas esquemáticos (software)</t>
-  </si>
-  <si>
     <t>Iniciar desenvolvimento do aplicativo para Android</t>
   </si>
   <si>
@@ -394,9 +391,6 @@
     <t>Invólucro</t>
   </si>
   <si>
-    <t>Imprimí-lo usando uma impressora 3D</t>
-  </si>
-  <si>
     <t>Projetá-lo (via software), com base nos datasheets</t>
   </si>
   <si>
@@ -467,6 +461,12 @@
   </si>
   <si>
     <t>Detalhes finais</t>
+  </si>
+  <si>
+    <t>Desenvolver diagramas de classes (software)</t>
+  </si>
+  <si>
+    <t>Confecção do Invólucro</t>
   </si>
 </sst>
 </file>
@@ -1007,6 +1007,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1025,16 +1031,10 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1801,8 +1801,8 @@
   </sheetPr>
   <dimension ref="A2:CU82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BN20" sqref="BN20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1827,47 +1827,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="24" t="s">
         <v>78</v>
       </c>
       <c r="I2" s="16"/>
-      <c r="BE2" s="53" t="s">
+      <c r="BE2" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" s="53"/>
-      <c r="BG2" s="53"/>
-      <c r="BH2" s="53"/>
-      <c r="BI2" s="53"/>
-      <c r="BJ2" s="53"/>
-      <c r="BK2" s="53"/>
-      <c r="BL2" s="53"/>
-      <c r="BM2" s="53"/>
-      <c r="BN2" s="53"/>
-      <c r="BO2" s="53"/>
-      <c r="BP2" s="53"/>
-      <c r="BQ2" s="53"/>
-      <c r="BR2" s="53"/>
-      <c r="BS2" s="53"/>
-      <c r="BT2" s="53"/>
-      <c r="BU2" s="53"/>
-      <c r="BV2" s="53"/>
-      <c r="BW2" s="53"/>
+      <c r="BF2" s="56"/>
+      <c r="BG2" s="56"/>
+      <c r="BH2" s="56"/>
+      <c r="BI2" s="56"/>
+      <c r="BJ2" s="56"/>
+      <c r="BK2" s="56"/>
+      <c r="BL2" s="56"/>
+      <c r="BM2" s="56"/>
+      <c r="BN2" s="56"/>
+      <c r="BO2" s="56"/>
+      <c r="BP2" s="56"/>
+      <c r="BQ2" s="56"/>
+      <c r="BR2" s="56"/>
+      <c r="BS2" s="56"/>
+      <c r="BT2" s="56"/>
+      <c r="BU2" s="56"/>
+      <c r="BV2" s="56"/>
+      <c r="BW2" s="56"/>
     </row>
     <row r="3" spans="1:99" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="24" t="s">
         <v>79</v>
       </c>
@@ -1916,35 +1916,35 @@
       <c r="AQ3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="BE3" s="53" t="s">
+      <c r="BE3" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="BF3" s="53"/>
-      <c r="BG3" s="53"/>
-      <c r="BH3" s="53"/>
-      <c r="BI3" s="53"/>
-      <c r="BJ3" s="53"/>
-      <c r="BK3" s="53"/>
-      <c r="BL3" s="53"/>
-      <c r="BM3" s="53"/>
-      <c r="BN3" s="53"/>
-      <c r="BO3" s="53"/>
-      <c r="BP3" s="53"/>
-      <c r="BQ3" s="53"/>
-      <c r="BR3" s="53"/>
-      <c r="BS3" s="53"/>
-      <c r="BT3" s="53"/>
-      <c r="BU3" s="53"/>
-      <c r="BV3" s="53"/>
-      <c r="BW3" s="53"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
+      <c r="BI3" s="56"/>
+      <c r="BJ3" s="56"/>
+      <c r="BK3" s="56"/>
+      <c r="BL3" s="56"/>
+      <c r="BM3" s="56"/>
+      <c r="BN3" s="56"/>
+      <c r="BO3" s="56"/>
+      <c r="BP3" s="56"/>
+      <c r="BQ3" s="56"/>
+      <c r="BR3" s="56"/>
+      <c r="BS3" s="56"/>
+      <c r="BT3" s="56"/>
+      <c r="BU3" s="56"/>
+      <c r="BV3" s="56"/>
+      <c r="BW3" s="56"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="24" t="s">
         <v>80</v>
       </c>
@@ -1975,132 +1975,132 @@
       <c r="AY4" s="19"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="47" t="s">
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="50" t="s">
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="47" t="s">
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="48"/>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="50" t="s">
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="50"/>
+      <c r="AB5" s="50"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="51"/>
-      <c r="AF5" s="51"/>
-      <c r="AG5" s="51"/>
-      <c r="AH5" s="52"/>
-      <c r="AI5" s="47" t="s">
+      <c r="AE5" s="53"/>
+      <c r="AF5" s="53"/>
+      <c r="AG5" s="53"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="48"/>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="49"/>
-      <c r="AN5" s="50" t="s">
+      <c r="AJ5" s="50"/>
+      <c r="AK5" s="50"/>
+      <c r="AL5" s="50"/>
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="51"/>
-      <c r="AP5" s="51"/>
-      <c r="AQ5" s="51"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="47" t="s">
+      <c r="AO5" s="53"/>
+      <c r="AP5" s="53"/>
+      <c r="AQ5" s="53"/>
+      <c r="AR5" s="54"/>
+      <c r="AS5" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="AT5" s="48"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="48"/>
-      <c r="AW5" s="49"/>
-      <c r="AX5" s="50" t="s">
+      <c r="AT5" s="50"/>
+      <c r="AU5" s="50"/>
+      <c r="AV5" s="50"/>
+      <c r="AW5" s="51"/>
+      <c r="AX5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="AY5" s="51"/>
-      <c r="AZ5" s="51"/>
-      <c r="BA5" s="51"/>
-      <c r="BB5" s="52"/>
-      <c r="BC5" s="47" t="s">
+      <c r="AY5" s="53"/>
+      <c r="AZ5" s="53"/>
+      <c r="BA5" s="53"/>
+      <c r="BB5" s="54"/>
+      <c r="BC5" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="BD5" s="48"/>
-      <c r="BE5" s="48"/>
-      <c r="BF5" s="48"/>
-      <c r="BG5" s="49"/>
-      <c r="BH5" s="50" t="s">
+      <c r="BD5" s="50"/>
+      <c r="BE5" s="50"/>
+      <c r="BF5" s="50"/>
+      <c r="BG5" s="51"/>
+      <c r="BH5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="BI5" s="51"/>
-      <c r="BJ5" s="51"/>
-      <c r="BK5" s="51"/>
-      <c r="BL5" s="52"/>
-      <c r="BM5" s="47" t="s">
+      <c r="BI5" s="53"/>
+      <c r="BJ5" s="53"/>
+      <c r="BK5" s="53"/>
+      <c r="BL5" s="54"/>
+      <c r="BM5" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="BN5" s="48"/>
-      <c r="BO5" s="48"/>
-      <c r="BP5" s="48"/>
-      <c r="BQ5" s="49"/>
-      <c r="BR5" s="50" t="s">
+      <c r="BN5" s="50"/>
+      <c r="BO5" s="50"/>
+      <c r="BP5" s="50"/>
+      <c r="BQ5" s="51"/>
+      <c r="BR5" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="BS5" s="51"/>
-      <c r="BT5" s="51"/>
-      <c r="BU5" s="51"/>
-      <c r="BV5" s="52"/>
-      <c r="BW5" s="47" t="s">
+      <c r="BS5" s="53"/>
+      <c r="BT5" s="53"/>
+      <c r="BU5" s="53"/>
+      <c r="BV5" s="54"/>
+      <c r="BW5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="BX5" s="48"/>
-      <c r="BY5" s="48"/>
-      <c r="BZ5" s="48"/>
-      <c r="CA5" s="49"/>
-      <c r="CB5" s="50" t="s">
+      <c r="BX5" s="50"/>
+      <c r="BY5" s="50"/>
+      <c r="BZ5" s="50"/>
+      <c r="CA5" s="51"/>
+      <c r="CB5" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="CC5" s="51"/>
-      <c r="CD5" s="51"/>
-      <c r="CE5" s="51"/>
-      <c r="CF5" s="52"/>
-      <c r="CG5" s="47" t="s">
+      <c r="CC5" s="53"/>
+      <c r="CD5" s="53"/>
+      <c r="CE5" s="53"/>
+      <c r="CF5" s="54"/>
+      <c r="CG5" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="CH5" s="48"/>
-      <c r="CI5" s="48"/>
-      <c r="CJ5" s="48"/>
-      <c r="CK5" s="49"/>
-      <c r="CL5" s="50" t="s">
+      <c r="CH5" s="50"/>
+      <c r="CI5" s="50"/>
+      <c r="CJ5" s="50"/>
+      <c r="CK5" s="51"/>
+      <c r="CL5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="CM5" s="51"/>
-      <c r="CN5" s="51"/>
-      <c r="CO5" s="51"/>
-      <c r="CP5" s="52"/>
-      <c r="CQ5" s="47" t="s">
+      <c r="CM5" s="53"/>
+      <c r="CN5" s="53"/>
+      <c r="CO5" s="53"/>
+      <c r="CP5" s="54"/>
+      <c r="CQ5" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="CR5" s="48"/>
-      <c r="CS5" s="48"/>
-      <c r="CT5" s="48"/>
-      <c r="CU5" s="49"/>
+      <c r="CR5" s="50"/>
+      <c r="CS5" s="50"/>
+      <c r="CT5" s="50"/>
+      <c r="CU5" s="51"/>
     </row>
     <row r="6" spans="1:99" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -2123,132 +2123,132 @@
         <v>75</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="47" t="s">
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="50" t="s">
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="51"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="47" t="s">
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="Z6" s="48"/>
-      <c r="AA6" s="48"/>
-      <c r="AB6" s="48"/>
-      <c r="AC6" s="49"/>
-      <c r="AD6" s="50" t="s">
+      <c r="Z6" s="50"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="50"/>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="51"/>
-      <c r="AF6" s="51"/>
-      <c r="AG6" s="51"/>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="47" t="s">
+      <c r="AE6" s="53"/>
+      <c r="AF6" s="53"/>
+      <c r="AG6" s="53"/>
+      <c r="AH6" s="54"/>
+      <c r="AI6" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="48"/>
-      <c r="AL6" s="48"/>
-      <c r="AM6" s="49"/>
-      <c r="AN6" s="50" t="s">
+      <c r="AJ6" s="50"/>
+      <c r="AK6" s="50"/>
+      <c r="AL6" s="50"/>
+      <c r="AM6" s="51"/>
+      <c r="AN6" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" s="51"/>
-      <c r="AP6" s="51"/>
-      <c r="AQ6" s="51"/>
-      <c r="AR6" s="52"/>
-      <c r="AS6" s="47" t="s">
+      <c r="AO6" s="53"/>
+      <c r="AP6" s="53"/>
+      <c r="AQ6" s="53"/>
+      <c r="AR6" s="54"/>
+      <c r="AS6" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="AT6" s="48"/>
-      <c r="AU6" s="48"/>
-      <c r="AV6" s="48"/>
-      <c r="AW6" s="49"/>
-      <c r="AX6" s="50" t="s">
+      <c r="AT6" s="50"/>
+      <c r="AU6" s="50"/>
+      <c r="AV6" s="50"/>
+      <c r="AW6" s="51"/>
+      <c r="AX6" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="AY6" s="51"/>
-      <c r="AZ6" s="51"/>
-      <c r="BA6" s="51"/>
-      <c r="BB6" s="52"/>
-      <c r="BC6" s="47" t="s">
+      <c r="AY6" s="53"/>
+      <c r="AZ6" s="53"/>
+      <c r="BA6" s="53"/>
+      <c r="BB6" s="54"/>
+      <c r="BC6" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="BD6" s="48"/>
-      <c r="BE6" s="48"/>
-      <c r="BF6" s="48"/>
-      <c r="BG6" s="49"/>
-      <c r="BH6" s="50" t="s">
+      <c r="BD6" s="50"/>
+      <c r="BE6" s="50"/>
+      <c r="BF6" s="50"/>
+      <c r="BG6" s="51"/>
+      <c r="BH6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="BI6" s="51"/>
-      <c r="BJ6" s="51"/>
-      <c r="BK6" s="51"/>
-      <c r="BL6" s="52"/>
-      <c r="BM6" s="47" t="s">
+      <c r="BI6" s="53"/>
+      <c r="BJ6" s="53"/>
+      <c r="BK6" s="53"/>
+      <c r="BL6" s="54"/>
+      <c r="BM6" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="BN6" s="48"/>
-      <c r="BO6" s="48"/>
-      <c r="BP6" s="48"/>
-      <c r="BQ6" s="49"/>
-      <c r="BR6" s="50" t="s">
+      <c r="BN6" s="50"/>
+      <c r="BO6" s="50"/>
+      <c r="BP6" s="50"/>
+      <c r="BQ6" s="51"/>
+      <c r="BR6" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="BS6" s="51"/>
-      <c r="BT6" s="51"/>
-      <c r="BU6" s="51"/>
-      <c r="BV6" s="52"/>
-      <c r="BW6" s="47" t="s">
+      <c r="BS6" s="53"/>
+      <c r="BT6" s="53"/>
+      <c r="BU6" s="53"/>
+      <c r="BV6" s="54"/>
+      <c r="BW6" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="BX6" s="48"/>
-      <c r="BY6" s="48"/>
-      <c r="BZ6" s="48"/>
-      <c r="CA6" s="49"/>
-      <c r="CB6" s="50" t="s">
+      <c r="BX6" s="50"/>
+      <c r="BY6" s="50"/>
+      <c r="BZ6" s="50"/>
+      <c r="CA6" s="51"/>
+      <c r="CB6" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="CC6" s="51"/>
-      <c r="CD6" s="51"/>
-      <c r="CE6" s="51"/>
-      <c r="CF6" s="52"/>
-      <c r="CG6" s="47" t="s">
+      <c r="CC6" s="53"/>
+      <c r="CD6" s="53"/>
+      <c r="CE6" s="53"/>
+      <c r="CF6" s="54"/>
+      <c r="CG6" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="CH6" s="48"/>
-      <c r="CI6" s="48"/>
-      <c r="CJ6" s="48"/>
-      <c r="CK6" s="49"/>
-      <c r="CL6" s="50" t="s">
+      <c r="CH6" s="50"/>
+      <c r="CI6" s="50"/>
+      <c r="CJ6" s="50"/>
+      <c r="CK6" s="51"/>
+      <c r="CL6" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="CM6" s="51"/>
-      <c r="CN6" s="51"/>
-      <c r="CO6" s="51"/>
-      <c r="CP6" s="52"/>
-      <c r="CQ6" s="47" t="s">
+      <c r="CM6" s="53"/>
+      <c r="CN6" s="53"/>
+      <c r="CO6" s="53"/>
+      <c r="CP6" s="54"/>
+      <c r="CQ6" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="CR6" s="48"/>
-      <c r="CS6" s="48"/>
-      <c r="CT6" s="48"/>
-      <c r="CU6" s="49"/>
+      <c r="CR6" s="50"/>
+      <c r="CS6" s="50"/>
+      <c r="CT6" s="50"/>
+      <c r="CU6" s="51"/>
     </row>
     <row r="7" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -3153,104 +3153,104 @@
       <c r="AC20" s="31"/>
     </row>
     <row r="21" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="55"/>
-      <c r="T21" s="55"/>
-      <c r="U21" s="55"/>
-      <c r="V21" s="55"/>
-      <c r="W21" s="55"/>
-      <c r="X21" s="55"/>
-      <c r="Y21" s="55"/>
-      <c r="Z21" s="55"/>
-      <c r="AA21" s="55"/>
-      <c r="AB21" s="55"/>
-      <c r="AC21" s="55"/>
-      <c r="AD21" s="55"/>
-      <c r="AE21" s="55"/>
-      <c r="AF21" s="55"/>
-      <c r="AG21" s="55"/>
-      <c r="AH21" s="55"/>
-      <c r="AI21" s="55"/>
-      <c r="AJ21" s="55"/>
-      <c r="AK21" s="55"/>
-      <c r="AL21" s="55"/>
-      <c r="AM21" s="55"/>
-      <c r="AN21" s="55"/>
-      <c r="AO21" s="55"/>
-      <c r="AP21" s="55"/>
-      <c r="AQ21" s="55"/>
-      <c r="AR21" s="55"/>
-      <c r="AS21" s="55"/>
-      <c r="AT21" s="55"/>
-      <c r="AU21" s="55"/>
-      <c r="AV21" s="55"/>
-      <c r="AW21" s="55"/>
-      <c r="AX21" s="55"/>
-      <c r="AY21" s="55"/>
-      <c r="AZ21" s="55"/>
-      <c r="BA21" s="55"/>
-      <c r="BB21" s="55"/>
-      <c r="BC21" s="55"/>
-      <c r="BD21" s="55"/>
-      <c r="BE21" s="55"/>
-      <c r="BF21" s="55"/>
-      <c r="BG21" s="55"/>
-      <c r="BH21" s="55"/>
-      <c r="BI21" s="55"/>
-      <c r="BJ21" s="55"/>
-      <c r="BK21" s="55"/>
-      <c r="BL21" s="55"/>
-      <c r="BM21" s="55"/>
-      <c r="BN21" s="55"/>
-      <c r="BO21" s="55"/>
-      <c r="BP21" s="55"/>
-      <c r="BQ21" s="55"/>
-      <c r="BR21" s="55"/>
-      <c r="BS21" s="55"/>
-      <c r="BT21" s="55"/>
-      <c r="BU21" s="55"/>
-      <c r="BV21" s="55"/>
-      <c r="BW21" s="55"/>
-      <c r="BX21" s="55"/>
-      <c r="BY21" s="55"/>
-      <c r="BZ21" s="55"/>
-      <c r="CA21" s="55"/>
-      <c r="CB21" s="55"/>
-      <c r="CC21" s="55"/>
-      <c r="CD21" s="55"/>
-      <c r="CE21" s="55"/>
-      <c r="CF21" s="55"/>
-      <c r="CG21" s="55"/>
-      <c r="CH21" s="55"/>
-      <c r="CI21" s="55"/>
-      <c r="CJ21" s="55"/>
-      <c r="CK21" s="55"/>
-      <c r="CL21" s="55"/>
-      <c r="CM21" s="55"/>
-      <c r="CN21" s="55"/>
-      <c r="CO21" s="55"/>
-      <c r="CP21" s="55"/>
-      <c r="CQ21" s="55"/>
-      <c r="CR21" s="55"/>
-      <c r="CS21" s="55"/>
-      <c r="CT21" s="55"/>
-      <c r="CU21" s="55"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="47"/>
+      <c r="Z21" s="47"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="47"/>
+      <c r="AF21" s="47"/>
+      <c r="AG21" s="47"/>
+      <c r="AH21" s="47"/>
+      <c r="AI21" s="47"/>
+      <c r="AJ21" s="47"/>
+      <c r="AK21" s="47"/>
+      <c r="AL21" s="47"/>
+      <c r="AM21" s="47"/>
+      <c r="AN21" s="47"/>
+      <c r="AO21" s="47"/>
+      <c r="AP21" s="47"/>
+      <c r="AQ21" s="47"/>
+      <c r="AR21" s="47"/>
+      <c r="AS21" s="47"/>
+      <c r="AT21" s="47"/>
+      <c r="AU21" s="47"/>
+      <c r="AV21" s="47"/>
+      <c r="AW21" s="47"/>
+      <c r="AX21" s="47"/>
+      <c r="AY21" s="47"/>
+      <c r="AZ21" s="47"/>
+      <c r="BA21" s="47"/>
+      <c r="BB21" s="47"/>
+      <c r="BC21" s="47"/>
+      <c r="BD21" s="47"/>
+      <c r="BE21" s="47"/>
+      <c r="BF21" s="47"/>
+      <c r="BG21" s="47"/>
+      <c r="BH21" s="47"/>
+      <c r="BI21" s="47"/>
+      <c r="BJ21" s="47"/>
+      <c r="BK21" s="47"/>
+      <c r="BL21" s="47"/>
+      <c r="BM21" s="47"/>
+      <c r="BN21" s="47"/>
+      <c r="BO21" s="47"/>
+      <c r="BP21" s="47"/>
+      <c r="BQ21" s="47"/>
+      <c r="BR21" s="47"/>
+      <c r="BS21" s="47"/>
+      <c r="BT21" s="47"/>
+      <c r="BU21" s="47"/>
+      <c r="BV21" s="47"/>
+      <c r="BW21" s="47"/>
+      <c r="BX21" s="47"/>
+      <c r="BY21" s="47"/>
+      <c r="BZ21" s="47"/>
+      <c r="CA21" s="47"/>
+      <c r="CB21" s="47"/>
+      <c r="CC21" s="47"/>
+      <c r="CD21" s="47"/>
+      <c r="CE21" s="47"/>
+      <c r="CF21" s="47"/>
+      <c r="CG21" s="47"/>
+      <c r="CH21" s="47"/>
+      <c r="CI21" s="47"/>
+      <c r="CJ21" s="47"/>
+      <c r="CK21" s="47"/>
+      <c r="CL21" s="47"/>
+      <c r="CM21" s="47"/>
+      <c r="CN21" s="47"/>
+      <c r="CO21" s="47"/>
+      <c r="CP21" s="47"/>
+      <c r="CQ21" s="47"/>
+      <c r="CR21" s="47"/>
+      <c r="CS21" s="47"/>
+      <c r="CT21" s="47"/>
+      <c r="CU21" s="47"/>
     </row>
     <row r="22" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
@@ -3545,104 +3545,104 @@
       <c r="CU25" s="35"/>
     </row>
     <row r="26" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="55"/>
-      <c r="S26" s="55"/>
-      <c r="T26" s="55"/>
-      <c r="U26" s="55"/>
-      <c r="V26" s="55"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="55"/>
-      <c r="Y26" s="55"/>
-      <c r="Z26" s="55"/>
-      <c r="AA26" s="55"/>
-      <c r="AB26" s="55"/>
-      <c r="AC26" s="55"/>
-      <c r="AD26" s="55"/>
-      <c r="AE26" s="55"/>
-      <c r="AF26" s="55"/>
-      <c r="AG26" s="55"/>
-      <c r="AH26" s="55"/>
-      <c r="AI26" s="55"/>
-      <c r="AJ26" s="55"/>
-      <c r="AK26" s="55"/>
-      <c r="AL26" s="55"/>
-      <c r="AM26" s="55"/>
-      <c r="AN26" s="55"/>
-      <c r="AO26" s="55"/>
-      <c r="AP26" s="55"/>
-      <c r="AQ26" s="55"/>
-      <c r="AR26" s="55"/>
-      <c r="AS26" s="55"/>
-      <c r="AT26" s="55"/>
-      <c r="AU26" s="55"/>
-      <c r="AV26" s="55"/>
-      <c r="AW26" s="55"/>
-      <c r="AX26" s="55"/>
-      <c r="AY26" s="55"/>
-      <c r="AZ26" s="55"/>
-      <c r="BA26" s="55"/>
-      <c r="BB26" s="55"/>
-      <c r="BC26" s="55"/>
-      <c r="BD26" s="55"/>
-      <c r="BE26" s="55"/>
-      <c r="BF26" s="55"/>
-      <c r="BG26" s="55"/>
-      <c r="BH26" s="55"/>
-      <c r="BI26" s="55"/>
-      <c r="BJ26" s="55"/>
-      <c r="BK26" s="55"/>
-      <c r="BL26" s="55"/>
-      <c r="BM26" s="55"/>
-      <c r="BN26" s="55"/>
-      <c r="BO26" s="55"/>
-      <c r="BP26" s="55"/>
-      <c r="BQ26" s="55"/>
-      <c r="BR26" s="55"/>
-      <c r="BS26" s="55"/>
-      <c r="BT26" s="55"/>
-      <c r="BU26" s="55"/>
-      <c r="BV26" s="55"/>
-      <c r="BW26" s="55"/>
-      <c r="BX26" s="55"/>
-      <c r="BY26" s="55"/>
-      <c r="BZ26" s="55"/>
-      <c r="CA26" s="55"/>
-      <c r="CB26" s="55"/>
-      <c r="CC26" s="55"/>
-      <c r="CD26" s="55"/>
-      <c r="CE26" s="55"/>
-      <c r="CF26" s="55"/>
-      <c r="CG26" s="55"/>
-      <c r="CH26" s="55"/>
-      <c r="CI26" s="55"/>
-      <c r="CJ26" s="55"/>
-      <c r="CK26" s="55"/>
-      <c r="CL26" s="55"/>
-      <c r="CM26" s="55"/>
-      <c r="CN26" s="55"/>
-      <c r="CO26" s="55"/>
-      <c r="CP26" s="55"/>
-      <c r="CQ26" s="55"/>
-      <c r="CR26" s="55"/>
-      <c r="CS26" s="55"/>
-      <c r="CT26" s="55"/>
-      <c r="CU26" s="55"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="47"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="47"/>
+      <c r="AE26" s="47"/>
+      <c r="AF26" s="47"/>
+      <c r="AG26" s="47"/>
+      <c r="AH26" s="47"/>
+      <c r="AI26" s="47"/>
+      <c r="AJ26" s="47"/>
+      <c r="AK26" s="47"/>
+      <c r="AL26" s="47"/>
+      <c r="AM26" s="47"/>
+      <c r="AN26" s="47"/>
+      <c r="AO26" s="47"/>
+      <c r="AP26" s="47"/>
+      <c r="AQ26" s="47"/>
+      <c r="AR26" s="47"/>
+      <c r="AS26" s="47"/>
+      <c r="AT26" s="47"/>
+      <c r="AU26" s="47"/>
+      <c r="AV26" s="47"/>
+      <c r="AW26" s="47"/>
+      <c r="AX26" s="47"/>
+      <c r="AY26" s="47"/>
+      <c r="AZ26" s="47"/>
+      <c r="BA26" s="47"/>
+      <c r="BB26" s="47"/>
+      <c r="BC26" s="47"/>
+      <c r="BD26" s="47"/>
+      <c r="BE26" s="47"/>
+      <c r="BF26" s="47"/>
+      <c r="BG26" s="47"/>
+      <c r="BH26" s="47"/>
+      <c r="BI26" s="47"/>
+      <c r="BJ26" s="47"/>
+      <c r="BK26" s="47"/>
+      <c r="BL26" s="47"/>
+      <c r="BM26" s="47"/>
+      <c r="BN26" s="47"/>
+      <c r="BO26" s="47"/>
+      <c r="BP26" s="47"/>
+      <c r="BQ26" s="47"/>
+      <c r="BR26" s="47"/>
+      <c r="BS26" s="47"/>
+      <c r="BT26" s="47"/>
+      <c r="BU26" s="47"/>
+      <c r="BV26" s="47"/>
+      <c r="BW26" s="47"/>
+      <c r="BX26" s="47"/>
+      <c r="BY26" s="47"/>
+      <c r="BZ26" s="47"/>
+      <c r="CA26" s="47"/>
+      <c r="CB26" s="47"/>
+      <c r="CC26" s="47"/>
+      <c r="CD26" s="47"/>
+      <c r="CE26" s="47"/>
+      <c r="CF26" s="47"/>
+      <c r="CG26" s="47"/>
+      <c r="CH26" s="47"/>
+      <c r="CI26" s="47"/>
+      <c r="CJ26" s="47"/>
+      <c r="CK26" s="47"/>
+      <c r="CL26" s="47"/>
+      <c r="CM26" s="47"/>
+      <c r="CN26" s="47"/>
+      <c r="CO26" s="47"/>
+      <c r="CP26" s="47"/>
+      <c r="CQ26" s="47"/>
+      <c r="CR26" s="47"/>
+      <c r="CS26" s="47"/>
+      <c r="CT26" s="47"/>
+      <c r="CU26" s="47"/>
     </row>
     <row r="27" spans="1:99" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
@@ -3661,7 +3661,7 @@
         <v>10</v>
       </c>
       <c r="G27" s="30">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="H27" s="24"/>
       <c r="I27" s="31"/>
@@ -3734,10 +3734,10 @@
         <v>5</v>
       </c>
       <c r="G28" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -3812,7 +3812,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="30" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="38" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="C30" s="29">
         <v>26</v>
@@ -3884,7 +3884,7 @@
         <v>10</v>
       </c>
       <c r="G30" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="24" t="s">
         <v>77</v>
@@ -3943,105 +3943,105 @@
       <c r="CU30" s="35"/>
     </row>
     <row r="31" spans="1:99" s="45" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="56"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
-      <c r="X31" s="56"/>
-      <c r="Y31" s="56"/>
-      <c r="Z31" s="56"/>
-      <c r="AA31" s="56"/>
-      <c r="AB31" s="56"/>
-      <c r="AC31" s="56"/>
-      <c r="AD31" s="56"/>
-      <c r="AE31" s="56"/>
-      <c r="AF31" s="56"/>
-      <c r="AG31" s="56"/>
-      <c r="AH31" s="56"/>
-      <c r="AI31" s="56"/>
-      <c r="AJ31" s="56"/>
-      <c r="AK31" s="56"/>
-      <c r="AL31" s="56"/>
-      <c r="AM31" s="56"/>
-      <c r="AN31" s="56"/>
-      <c r="AO31" s="56"/>
-      <c r="AP31" s="56"/>
-      <c r="AQ31" s="56"/>
-      <c r="AR31" s="56"/>
-      <c r="AS31" s="56"/>
-      <c r="AT31" s="56"/>
-      <c r="AU31" s="56"/>
-      <c r="AV31" s="56"/>
-      <c r="AW31" s="56"/>
-      <c r="AX31" s="56"/>
-      <c r="AY31" s="56"/>
-      <c r="AZ31" s="56"/>
-      <c r="BA31" s="56"/>
-      <c r="BB31" s="56"/>
-      <c r="BC31" s="56"/>
-      <c r="BD31" s="56"/>
-      <c r="BE31" s="56"/>
-      <c r="BF31" s="56"/>
-      <c r="BG31" s="56"/>
-      <c r="BH31" s="56"/>
-      <c r="BI31" s="56"/>
-      <c r="BJ31" s="56"/>
-      <c r="BK31" s="56"/>
-      <c r="BL31" s="56"/>
-      <c r="BM31" s="56"/>
-      <c r="BN31" s="56"/>
-      <c r="BO31" s="56"/>
-      <c r="BP31" s="56"/>
-      <c r="BQ31" s="56"/>
-      <c r="BR31" s="56"/>
-      <c r="BS31" s="56"/>
-      <c r="BT31" s="56"/>
-      <c r="BU31" s="56"/>
-      <c r="BV31" s="56"/>
-      <c r="BW31" s="56"/>
-      <c r="BX31" s="56"/>
-      <c r="BY31" s="56"/>
-      <c r="BZ31" s="56"/>
-      <c r="CA31" s="56"/>
-      <c r="CB31" s="56"/>
-      <c r="CC31" s="56"/>
-      <c r="CD31" s="56"/>
-      <c r="CE31" s="56"/>
-      <c r="CF31" s="56"/>
-      <c r="CG31" s="56"/>
-      <c r="CH31" s="56"/>
-      <c r="CI31" s="56"/>
-      <c r="CJ31" s="56"/>
-      <c r="CK31" s="56"/>
-      <c r="CL31" s="56"/>
-      <c r="CM31" s="56"/>
-      <c r="CN31" s="56"/>
-      <c r="CO31" s="56"/>
-      <c r="CP31" s="56"/>
-      <c r="CQ31" s="56"/>
-      <c r="CR31" s="56"/>
-      <c r="CS31" s="56"/>
-      <c r="CT31" s="56"/>
-      <c r="CU31" s="56"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="48"/>
+      <c r="V31" s="48"/>
+      <c r="W31" s="48"/>
+      <c r="X31" s="48"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="48"/>
+      <c r="AA31" s="48"/>
+      <c r="AB31" s="48"/>
+      <c r="AC31" s="48"/>
+      <c r="AD31" s="48"/>
+      <c r="AE31" s="48"/>
+      <c r="AF31" s="48"/>
+      <c r="AG31" s="48"/>
+      <c r="AH31" s="48"/>
+      <c r="AI31" s="48"/>
+      <c r="AJ31" s="48"/>
+      <c r="AK31" s="48"/>
+      <c r="AL31" s="48"/>
+      <c r="AM31" s="48"/>
+      <c r="AN31" s="48"/>
+      <c r="AO31" s="48"/>
+      <c r="AP31" s="48"/>
+      <c r="AQ31" s="48"/>
+      <c r="AR31" s="48"/>
+      <c r="AS31" s="48"/>
+      <c r="AT31" s="48"/>
+      <c r="AU31" s="48"/>
+      <c r="AV31" s="48"/>
+      <c r="AW31" s="48"/>
+      <c r="AX31" s="48"/>
+      <c r="AY31" s="48"/>
+      <c r="AZ31" s="48"/>
+      <c r="BA31" s="48"/>
+      <c r="BB31" s="48"/>
+      <c r="BC31" s="48"/>
+      <c r="BD31" s="48"/>
+      <c r="BE31" s="48"/>
+      <c r="BF31" s="48"/>
+      <c r="BG31" s="48"/>
+      <c r="BH31" s="48"/>
+      <c r="BI31" s="48"/>
+      <c r="BJ31" s="48"/>
+      <c r="BK31" s="48"/>
+      <c r="BL31" s="48"/>
+      <c r="BM31" s="48"/>
+      <c r="BN31" s="48"/>
+      <c r="BO31" s="48"/>
+      <c r="BP31" s="48"/>
+      <c r="BQ31" s="48"/>
+      <c r="BR31" s="48"/>
+      <c r="BS31" s="48"/>
+      <c r="BT31" s="48"/>
+      <c r="BU31" s="48"/>
+      <c r="BV31" s="48"/>
+      <c r="BW31" s="48"/>
+      <c r="BX31" s="48"/>
+      <c r="BY31" s="48"/>
+      <c r="BZ31" s="48"/>
+      <c r="CA31" s="48"/>
+      <c r="CB31" s="48"/>
+      <c r="CC31" s="48"/>
+      <c r="CD31" s="48"/>
+      <c r="CE31" s="48"/>
+      <c r="CF31" s="48"/>
+      <c r="CG31" s="48"/>
+      <c r="CH31" s="48"/>
+      <c r="CI31" s="48"/>
+      <c r="CJ31" s="48"/>
+      <c r="CK31" s="48"/>
+      <c r="CL31" s="48"/>
+      <c r="CM31" s="48"/>
+      <c r="CN31" s="48"/>
+      <c r="CO31" s="48"/>
+      <c r="CP31" s="48"/>
+      <c r="CQ31" s="48"/>
+      <c r="CR31" s="48"/>
+      <c r="CS31" s="48"/>
+      <c r="CT31" s="48"/>
+      <c r="CU31" s="48"/>
     </row>
     <row r="32" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
@@ -4060,7 +4060,7 @@
         <v>20</v>
       </c>
       <c r="G32" s="30">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="H32" s="24"/>
       <c r="I32" s="31"/>
@@ -4118,7 +4118,7 @@
     </row>
     <row r="33" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33" s="29">
         <v>36</v>
@@ -4133,7 +4133,7 @@
         <v>8</v>
       </c>
       <c r="G33" s="30">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="H33" s="24" t="s">
         <v>77</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="34" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C34" s="29">
         <v>36</v>
@@ -4268,7 +4268,7 @@
     </row>
     <row r="35" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="42" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="C35" s="29">
         <v>41</v>
@@ -4283,7 +4283,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="30">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="H35" s="24" t="s">
         <v>77</v>
@@ -4343,7 +4343,7 @@
     </row>
     <row r="36" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" s="29">
         <v>36</v>
@@ -4358,7 +4358,7 @@
         <v>20</v>
       </c>
       <c r="G36" s="30">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H36" s="24" t="s">
         <v>82</v>
@@ -4418,7 +4418,7 @@
     </row>
     <row r="37" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="29">
         <v>36</v>
@@ -4433,7 +4433,7 @@
         <v>15</v>
       </c>
       <c r="G37" s="30">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="H37" s="24" t="s">
         <v>81</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="38" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" s="29">
         <v>36</v>
@@ -4508,7 +4508,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="24" t="s">
         <v>81</v>
@@ -4568,7 +4568,7 @@
     </row>
     <row r="39" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="29">
         <v>40</v>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="40" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" s="29">
         <v>51</v>
@@ -4892,7 +4892,7 @@
     </row>
     <row r="43" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C43" s="29">
         <v>56</v>
@@ -4967,7 +4967,7 @@
     </row>
     <row r="44" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C44" s="29">
         <v>59</v>
@@ -5042,7 +5042,7 @@
     </row>
     <row r="45" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="29">
         <v>56</v>
@@ -5117,7 +5117,7 @@
     </row>
     <row r="46" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C46" s="29">
         <v>68</v>
@@ -5363,7 +5363,7 @@
     </row>
     <row r="49" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C49" s="29">
         <v>71</v>
@@ -5610,7 +5610,7 @@
     </row>
     <row r="52" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C52" s="29">
         <v>81</v>
@@ -5683,7 +5683,7 @@
     </row>
     <row r="53" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C53" s="29">
         <v>84</v>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="54" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C54" s="29">
         <v>81</v>
@@ -6003,7 +6003,7 @@
     </row>
     <row r="57" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C57" s="41">
         <v>11</v>
@@ -6078,7 +6078,7 @@
     </row>
     <row r="58" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C58" s="41">
         <v>13</v>
@@ -6151,7 +6151,7 @@
     </row>
     <row r="59" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C59" s="41">
         <v>13</v>
@@ -6226,7 +6226,7 @@
     </row>
     <row r="60" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C60" s="41">
         <v>13</v>
@@ -6301,7 +6301,7 @@
     </row>
     <row r="61" spans="1:99" s="28" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="40" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C61" s="41">
         <v>13</v>
@@ -6319,7 +6319,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I61" s="31"/>
       <c r="J61" s="31"/>
@@ -6376,7 +6376,7 @@
     </row>
     <row r="62" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C62" s="41">
         <v>16</v>
@@ -6449,7 +6449,7 @@
     </row>
     <row r="63" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C63" s="41">
         <v>17</v>
@@ -6524,7 +6524,7 @@
     </row>
     <row r="64" spans="1:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C64" s="41">
         <v>17</v>
@@ -6542,7 +6542,7 @@
         <v>1</v>
       </c>
       <c r="H64" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I64" s="31"/>
       <c r="J64" s="31"/>
@@ -6599,7 +6599,7 @@
     </row>
     <row r="65" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C65" s="41">
         <v>17</v>
@@ -6674,7 +6674,7 @@
     </row>
     <row r="66" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C66" s="41">
         <v>19</v>
@@ -6747,7 +6747,7 @@
     </row>
     <row r="67" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C67" s="41">
         <v>20</v>
@@ -6820,7 +6820,7 @@
     </row>
     <row r="68" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C68" s="41">
         <v>22</v>
@@ -6893,7 +6893,7 @@
     </row>
     <row r="69" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C69" s="41">
         <v>22</v>
@@ -6966,7 +6966,7 @@
     </row>
     <row r="70" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C70" s="41">
         <v>36</v>
@@ -7039,7 +7039,7 @@
     </row>
     <row r="71" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C71" s="41">
         <v>71</v>
@@ -7112,7 +7112,7 @@
     </row>
     <row r="72" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C72" s="41">
         <v>78</v>
@@ -7185,7 +7185,7 @@
     </row>
     <row r="73" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C73" s="41">
         <v>82</v>
@@ -7258,7 +7258,7 @@
     </row>
     <row r="74" spans="2:99" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C74" s="41">
         <v>86</v>
@@ -7538,21 +7538,22 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A13:CU13"/>
-    <mergeCell ref="B21:CU21"/>
-    <mergeCell ref="B26:CU26"/>
-    <mergeCell ref="A31:CU31"/>
-    <mergeCell ref="A41:CU41"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="AD5:AH5"/>
-    <mergeCell ref="AD6:AH6"/>
-    <mergeCell ref="B2:G4"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="O6:S6"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A55:CU55"/>
+    <mergeCell ref="B47:CU47"/>
+    <mergeCell ref="A50:CU50"/>
+    <mergeCell ref="CQ5:CU5"/>
+    <mergeCell ref="CQ6:CU6"/>
+    <mergeCell ref="CL5:CP5"/>
+    <mergeCell ref="CL6:CP6"/>
+    <mergeCell ref="AX5:BB5"/>
+    <mergeCell ref="AX6:BB6"/>
+    <mergeCell ref="AI5:AM5"/>
+    <mergeCell ref="AI6:AM6"/>
+    <mergeCell ref="AN5:AR5"/>
+    <mergeCell ref="AN6:AR6"/>
+    <mergeCell ref="AS5:AW5"/>
+    <mergeCell ref="AS6:AW6"/>
+    <mergeCell ref="Y5:AC5"/>
     <mergeCell ref="BE2:BW2"/>
     <mergeCell ref="BE3:BW3"/>
     <mergeCell ref="CB5:CF5"/>
@@ -7569,22 +7570,21 @@
     <mergeCell ref="BC6:BG6"/>
     <mergeCell ref="BH5:BL5"/>
     <mergeCell ref="BH6:BL6"/>
-    <mergeCell ref="A55:CU55"/>
-    <mergeCell ref="B47:CU47"/>
-    <mergeCell ref="A50:CU50"/>
-    <mergeCell ref="CQ5:CU5"/>
-    <mergeCell ref="CQ6:CU6"/>
-    <mergeCell ref="CL5:CP5"/>
-    <mergeCell ref="CL6:CP6"/>
-    <mergeCell ref="AX5:BB5"/>
-    <mergeCell ref="AX6:BB6"/>
-    <mergeCell ref="AI5:AM5"/>
-    <mergeCell ref="AI6:AM6"/>
-    <mergeCell ref="AN5:AR5"/>
-    <mergeCell ref="AN6:AR6"/>
-    <mergeCell ref="AS5:AW5"/>
-    <mergeCell ref="AS6:AW6"/>
-    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="AD6:AH6"/>
+    <mergeCell ref="B2:G4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="O6:S6"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="A13:CU13"/>
+    <mergeCell ref="B21:CU21"/>
+    <mergeCell ref="B26:CU26"/>
+    <mergeCell ref="A31:CU31"/>
+    <mergeCell ref="A41:CU41"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:CU20 J27:CU30 J9:CU12 J22:CU25 J51:CU54 J48:CU49 J56:CU57 J73:CU73 J32:CU40 J42:CU46">
     <cfRule type="expression" dxfId="25" priority="84">

</xml_diff>